<commit_message>
edit 06_28 goal, comment. add 06.29 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -19,7 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
   <x:si>
     <x:t>1. DateBook_Comment 부분 수정
 2. GIT보고서 수정
@@ -46,10 +52,24 @@
  - 개발 설계</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
+    <x:t>1-1. Datebook Comment 부분 요약
+1-2. GIT 보고서 다시 작성
+1-3. PPT 머릿글 요약 작성
+1-4. 파일명 수정
+1-5 최종 아이디어 선정 이유 작성
+2. 요구사항 수집 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -63,46 +83,37 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 아이디어 도출
 2. 최종 아이디어 선정
 3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
   </x:si>
   <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
+  </x:si>
+  <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
   </x:si>
   <x:si>
-    <x:t>1-1. Datebook Comment 부분 요약 (완)
-1-2. GIT 보고서 다시 작성 (완)
-1-3. PPT 머릿글 요약 작성
-1-4. 파일명 수정 (완)
-1-5 최종 아이디어 선정 이유 작성
-2. 요구사항 수집 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1-1. PPT 머릿글 보완
-1-2. 교통사고 그래프 검색
-1-3. 최종 아이디어 선정 이유 보완</x:t>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -145,12 +156,28 @@
       <x:sz val="10"/>
       <x:color rgb="ff000000"/>
     </x:font>
-    <x:font>
-      <x:name val="맑은 고딕"/>
-      <x:sz val="11"/>
-      <x:color rgb="ffffffff"/>
-      <x:b val="1"/>
-    </x:font>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ffffffff"/>
+          <x:b val="1"/>
+          <hs:size val="100"/>
+          <hs:ratio val="100"/>
+          <hs:spacing val="0"/>
+          <hs:offset val="0"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="11"/>
+          <x:color rgb="ffffffff"/>
+          <x:b val="1"/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:fonts>
   <x:fills count="3">
     <x:fill>
@@ -257,7 +284,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="17">
+  <x:cellXfs count="18">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -415,6 +442,19 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="20" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
@@ -1111,8 +1151,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B2:E31"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="E5" activeCellId="0" sqref="E5:E5"/>
+    <x:sheetView tabSelected="1" topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="D7" activeCellId="0" sqref="D7:D7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -1134,10 +1174,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D2" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E2" s="5" t="s">
         <x:v>8</x:v>
-      </x:c>
-      <x:c r="E2" s="5" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -1145,13 +1185,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="13" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E3" s="7" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -1159,13 +1199,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -1173,13 +1213,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D5" s="10" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E5" s="10" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -1187,29 +1227,35 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="16" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D6" s="10" t="s">
-        <x:v>13</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="2:5" ht="39.549999999999997">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="2:5" ht="79.049999999999997">
       <x:c r="B7" s="11">
         <x:v>44375</x:v>
       </x:c>
-      <x:c r="C7" s="8"/>
+      <x:c r="C7" s="17" t="s">
+        <x:v>11</x:v>
+      </x:c>
       <x:c r="D7" s="10" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E7" s="9"/>
-    </x:row>
-    <x:row r="8" spans="2:5">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E7" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="2:5" ht="26.350000000000001">
       <x:c r="B8" s="8"/>
       <x:c r="C8" s="8"/>
-      <x:c r="D8" s="9"/>
+      <x:c r="D8" s="10" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="E8" s="9"/>
     </x:row>
     <x:row r="9" spans="2:5">

</xml_diff>

<commit_message>
add 06_29 comment, 06_30 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -19,12 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
   </x:si>
   <x:si>
     <x:t>1. DateBook_Comment 부분 수정
@@ -42,16 +44,6 @@
 3. 개발 계획서 및 요구사항 작성</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 현장실습 OT
- - 기업 소개 및 업무 설명
- - 앞으로 수행하게 될 프로젝트 설명
-2. 기존에 진행했던 캡스톤프로젝트 첨언
-3. 제품 개발 과정 설명
- - 제품 기획 
- - 개발 기획  
- - 개발 설계</x:t>
-  </x:si>
-  <x:si>
     <x:t>1-1. Datebook Comment 부분 요약
 1-2. GIT 보고서 다시 작성
 1-3. PPT 머릿글 요약 작성
@@ -60,16 +52,10 @@
 2. 요구사항 수집 및 분석</x:t>
   </x:si>
   <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -83,37 +69,60 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
+    <x:t>1. 현장실습 OT
+ - 기업 소개 및 업무 설명
+ - 앞으로 수행하게 될 프로젝트 설명
+2. 기존에 진행했던 캡스톤프로젝트 첨언
+3. 제품 개발 과정 설명
+ - 제품 기획 
+ - 개발 기획  
+ - 개발 설계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
     <x:t>1. 아이디어 도출
 2. 최종 아이디어 선정
 3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
   </x:si>
   <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 진행사항 체크 및 2주차 목표 설정
-2. 06.28 회의록 작성
-3. 상용화 된 타 앱 기능 분석
-4. 요구사항 정의
- - 회원가입, DB, 무결성 (미완)
-5. vi사용법 설명</x:t>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화</x:t>
   </x:si>
   <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
   </x:si>
   <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
+    <x:t>1. vi 명령어 설명서 작성 완료
+2. 요구사항 정의 및 분류
+ - 기능적 요구사항
+ - 비기능적 요구사항</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -156,28 +165,12 @@
       <x:sz val="10"/>
       <x:color rgb="ff000000"/>
     </x:font>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:font hs:extension="1">
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ffffffff"/>
-          <x:b val="1"/>
-          <hs:size val="100"/>
-          <hs:ratio val="100"/>
-          <hs:spacing val="0"/>
-          <hs:offset val="0"/>
-        </x:font>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:font>
-          <x:name val="맑은 고딕"/>
-          <x:sz val="11"/>
-          <x:color rgb="ffffffff"/>
-          <x:b val="1"/>
-        </x:font>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ffffffff"/>
+      <x:b val="1"/>
+    </x:font>
   </x:fonts>
   <x:fills count="3">
     <x:fill>
@@ -284,7 +277,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="18">
+  <x:cellXfs count="20">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -456,6 +449,32 @@
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -1149,10 +1168,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="B2:E31"/>
+  <x:dimension ref="B2:E36"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D7" activeCellId="0" sqref="D7:D7"/>
+      <x:selection activeCell="D6" activeCellId="0" sqref="D6:D6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -1168,16 +1187,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D2" s="4" t="s">
-        <x:v>5</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="5" t="s">
-        <x:v>8</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -1185,13 +1204,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="13" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E3" s="7" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -1199,13 +1218,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -1213,10 +1232,10 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="10" t="s">
-        <x:v>10</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E5" s="10" t="s">
         <x:v>2</x:v>
@@ -1227,10 +1246,10 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="16" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="10" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s">
         <x:v>1</x:v>
@@ -1241,160 +1260,229 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="17" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="10" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E7" s="10" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="2:5" ht="52.700000000000003">
+      <x:c r="B8" s="11">
+        <x:v>44376</x:v>
+      </x:c>
+      <x:c r="C8" s="18" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D8" s="10" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="2:5">
+      <x:c r="B9" s="11">
+        <x:v>44377</x:v>
+      </x:c>
+      <x:c r="C9" s="8"/>
+      <x:c r="D9" s="10" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E7" s="10" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="2:5" ht="26.350000000000001">
-      <x:c r="B8" s="8"/>
-      <x:c r="C8" s="8"/>
-      <x:c r="D8" s="10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E8" s="9"/>
-    </x:row>
-    <x:row r="9" spans="2:5">
-      <x:c r="B9" s="8"/>
-      <x:c r="C9" s="8"/>
-      <x:c r="D9" s="9"/>
       <x:c r="E9" s="9"/>
     </x:row>
     <x:row r="10" spans="2:5">
-      <x:c r="B10" s="8"/>
+      <x:c r="B10" s="11">
+        <x:v>44378</x:v>
+      </x:c>
       <x:c r="C10" s="8"/>
       <x:c r="D10" s="9"/>
       <x:c r="E10" s="9"/>
     </x:row>
     <x:row r="11" spans="2:5">
-      <x:c r="B11" s="8"/>
+      <x:c r="B11" s="11">
+        <x:v>44379</x:v>
+      </x:c>
       <x:c r="C11" s="8"/>
       <x:c r="D11" s="9"/>
       <x:c r="E11" s="9"/>
     </x:row>
     <x:row r="12" spans="2:5">
-      <x:c r="B12" s="8"/>
+      <x:c r="B12" s="11">
+        <x:v>44382</x:v>
+      </x:c>
       <x:c r="C12" s="8"/>
       <x:c r="D12" s="9"/>
       <x:c r="E12" s="9"/>
     </x:row>
     <x:row r="13" spans="2:5">
-      <x:c r="B13" s="8"/>
+      <x:c r="B13" s="11">
+        <x:v>44383</x:v>
+      </x:c>
       <x:c r="C13" s="8"/>
       <x:c r="D13" s="9"/>
       <x:c r="E13" s="9"/>
     </x:row>
     <x:row r="14" spans="2:5">
-      <x:c r="B14" s="8"/>
+      <x:c r="B14" s="11">
+        <x:v>44384</x:v>
+      </x:c>
       <x:c r="C14" s="8"/>
       <x:c r="D14" s="9"/>
       <x:c r="E14" s="9"/>
     </x:row>
     <x:row r="15" spans="2:5">
-      <x:c r="B15" s="8"/>
+      <x:c r="B15" s="11">
+        <x:v>44385</x:v>
+      </x:c>
       <x:c r="C15" s="8"/>
       <x:c r="D15" s="9"/>
       <x:c r="E15" s="9"/>
     </x:row>
     <x:row r="16" spans="2:5">
-      <x:c r="B16" s="8"/>
+      <x:c r="B16" s="11">
+        <x:v>44386</x:v>
+      </x:c>
       <x:c r="C16" s="8"/>
       <x:c r="D16" s="9"/>
       <x:c r="E16" s="9"/>
     </x:row>
     <x:row r="17" spans="2:5">
-      <x:c r="B17" s="8"/>
+      <x:c r="B17" s="11">
+        <x:v>44389</x:v>
+      </x:c>
       <x:c r="C17" s="8"/>
       <x:c r="D17" s="9"/>
       <x:c r="E17" s="9"/>
     </x:row>
     <x:row r="18" spans="2:5">
-      <x:c r="B18" s="8"/>
+      <x:c r="B18" s="11">
+        <x:v>44390</x:v>
+      </x:c>
       <x:c r="C18" s="8"/>
       <x:c r="D18" s="9"/>
       <x:c r="E18" s="9"/>
     </x:row>
     <x:row r="19" spans="2:5">
-      <x:c r="B19" s="8"/>
+      <x:c r="B19" s="11">
+        <x:v>44391</x:v>
+      </x:c>
       <x:c r="C19" s="8"/>
       <x:c r="D19" s="9"/>
       <x:c r="E19" s="9"/>
     </x:row>
     <x:row r="20" spans="2:5">
-      <x:c r="B20" s="8"/>
+      <x:c r="B20" s="11">
+        <x:v>44392</x:v>
+      </x:c>
       <x:c r="C20" s="8"/>
       <x:c r="D20" s="9"/>
       <x:c r="E20" s="9"/>
     </x:row>
     <x:row r="21" spans="2:5">
-      <x:c r="B21" s="8"/>
+      <x:c r="B21" s="11">
+        <x:v>44393</x:v>
+      </x:c>
       <x:c r="C21" s="8"/>
       <x:c r="D21" s="9"/>
       <x:c r="E21" s="9"/>
     </x:row>
     <x:row r="22" spans="2:5">
-      <x:c r="B22" s="8"/>
+      <x:c r="B22" s="11">
+        <x:v>44396</x:v>
+      </x:c>
       <x:c r="C22" s="8"/>
       <x:c r="D22" s="9"/>
       <x:c r="E22" s="9"/>
     </x:row>
     <x:row r="23" spans="2:5">
-      <x:c r="B23" s="8"/>
+      <x:c r="B23" s="11">
+        <x:v>44397</x:v>
+      </x:c>
       <x:c r="C23" s="8"/>
       <x:c r="D23" s="9"/>
       <x:c r="E23" s="9"/>
     </x:row>
     <x:row r="24" spans="2:5">
-      <x:c r="B24" s="8"/>
+      <x:c r="B24" s="11">
+        <x:v>44398</x:v>
+      </x:c>
       <x:c r="C24" s="8"/>
       <x:c r="D24" s="9"/>
       <x:c r="E24" s="9"/>
     </x:row>
     <x:row r="25" spans="2:5">
-      <x:c r="B25" s="8"/>
+      <x:c r="B25" s="11">
+        <x:v>44399</x:v>
+      </x:c>
       <x:c r="C25" s="8"/>
       <x:c r="D25" s="9"/>
       <x:c r="E25" s="9"/>
     </x:row>
     <x:row r="26" spans="2:5">
-      <x:c r="B26" s="8"/>
+      <x:c r="B26" s="11">
+        <x:v>44400</x:v>
+      </x:c>
       <x:c r="C26" s="8"/>
       <x:c r="D26" s="9"/>
       <x:c r="E26" s="9"/>
     </x:row>
     <x:row r="27" spans="2:5">
-      <x:c r="B27" s="8"/>
+      <x:c r="B27" s="11">
+        <x:v>44403</x:v>
+      </x:c>
       <x:c r="C27" s="8"/>
       <x:c r="D27" s="9"/>
       <x:c r="E27" s="9"/>
     </x:row>
     <x:row r="28" spans="2:5">
-      <x:c r="B28" s="8"/>
+      <x:c r="B28" s="11">
+        <x:v>44404</x:v>
+      </x:c>
       <x:c r="C28" s="8"/>
       <x:c r="D28" s="9"/>
       <x:c r="E28" s="9"/>
     </x:row>
     <x:row r="29" spans="2:5">
-      <x:c r="B29" s="8"/>
+      <x:c r="B29" s="11">
+        <x:v>44405</x:v>
+      </x:c>
       <x:c r="C29" s="8"/>
       <x:c r="D29" s="9"/>
       <x:c r="E29" s="9"/>
     </x:row>
     <x:row r="30" spans="2:5">
-      <x:c r="B30" s="8"/>
+      <x:c r="B30" s="11">
+        <x:v>44406</x:v>
+      </x:c>
       <x:c r="C30" s="8"/>
       <x:c r="D30" s="9"/>
       <x:c r="E30" s="9"/>
     </x:row>
     <x:row r="31" spans="2:5">
-      <x:c r="B31" s="8"/>
+      <x:c r="B31" s="11">
+        <x:v>44407</x:v>
+      </x:c>
       <x:c r="C31" s="8"/>
       <x:c r="D31" s="9"/>
       <x:c r="E31" s="9"/>
+    </x:row>
+    <x:row r="32" spans="2:2">
+      <x:c r="B32" s="19"/>
+    </x:row>
+    <x:row r="33" spans="2:2">
+      <x:c r="B33" s="19"/>
+    </x:row>
+    <x:row r="34" spans="2:2">
+      <x:c r="B34" s="19"/>
+    </x:row>
+    <x:row r="35" spans="2:2">
+      <x:c r="B35" s="19"/>
+    </x:row>
+    <x:row r="36" spans="2:2">
+      <x:c r="B36" s="19"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>

<commit_message>
add 07.02 Comment add 07.05 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -19,28 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
-  <x:si>
-    <x:t>1. 아이디어 도출
- - 컴퓨터 견적 추천 앱
- - 주차시 사고발생 알림 앱
-2. 주제 아이디어 최종 선정
- - 차량 관리 어플
-3. 개발 계획서 및 요구사항 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <x:si>
     <x:t>1. 현장실습 OT
  - 기업 소개 및 업무 설명
@@ -52,35 +31,6 @@
  - 개발 설계</x:t>
   </x:si>
   <x:si>
-    <x:t>1-1. Datebook Comment 부분 요약
-1-2. GIT 보고서 다시 작성
-1-3. PPT 머릿글 요약 작성
-1-4. 파일명 수정
-1-5 최종 아이디어 선정 이유 작성
-2. 요구사항 수집 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Git 목록 삭제
-2. 요구사항 분석
-3. 요구사항 검증</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 요구사항 수집 및 정의
 2. 요구사항 분석
 3. 구현 가능 여부 확인</x:t>
@@ -90,24 +40,6 @@
 2. 요구사항 정의 및 분류
  - 기능적 요구사항
  - 비기능적 요구사항</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 진행사항 체크 및 2주차 목표 설정
-2. 06.28 회의록 작성
-3. 상용화 된 타 앱 기능 분석
-4. 요구사항 정의
- - 회원가입, DB, 무결성 (미완)
-5. vi사용법 설명</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -121,48 +53,126 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+ - 컴퓨터 견적 추천 앱
+ - 주차시 사고발생 알림 앱
+2. 주제 아이디어 최종 선정
+ - 차량 관리 어플
+3. 개발 계획서 및 요구사항 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1-1. Datebook Comment 부분 요약
+1-2. GIT 보고서 다시 작성
+1-3. PPT 머릿글 요약 작성
+1-4. 파일명 수정
+1-5 최종 아이디어 선정 이유 작성
+2. 요구사항 수집 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 07.02 회의록 작성
+2. Git 업로드 한 것 중 중복된 것들 삭제
+3. 어플 흐름 구상도 작성
+4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
+  </x:si>
+  <x:si>
     <x:t>1. 06.28 회의록 작성
 2. 요구사항 정의 및 분석</x:t>
   </x:si>
   <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 인터페이스 구상도 작성
+2. 요구사항 분류하여 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1211,7 +1221,7 @@
   <x:dimension ref="B2:E36"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D13" activeCellId="0" sqref="D13:D13"/>
+      <x:selection activeCell="D4" activeCellId="0" sqref="D4:D4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -1227,16 +1237,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D2" s="4" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E2" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -1244,13 +1254,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="13" t="s">
-        <x:v>21</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
         <x:v>26</x:v>
       </x:c>
       <x:c r="E3" s="7" t="s">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -1258,13 +1268,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s">
-        <x:v>21</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
-        <x:v>14</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -1272,13 +1282,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D5" s="10" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="E5" s="10" t="s">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -1286,13 +1296,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="16" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D6" s="10" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E6" s="15" t="s">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="E6" s="15" t="s">
-        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -1300,13 +1310,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="12" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D7" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E7" s="10" t="s">
         <x:v>23</x:v>
-      </x:c>
-      <x:c r="D7" s="10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E7" s="10" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -1314,13 +1324,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="12" t="s">
-        <x:v>24</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D8" s="10" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E8" s="10" t="s">
-        <x:v>10</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -1328,10 +1338,10 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="18" t="s">
-        <x:v>25</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D9" s="10" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E9" s="10" t="s">
         <x:v>12</x:v>
@@ -1342,16 +1352,16 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="19" t="s">
-        <x:v>20</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D10" s="10" t="s">
-        <x:v>9</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E10" s="10" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="2:5" ht="39.549999999999997">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="2:5" ht="65.849999999999994">
       <x:c r="B11" s="11">
         <x:v>44379</x:v>
       </x:c>
@@ -1359,16 +1369,20 @@
         <x:v>0.35208333333333336</x:v>
       </x:c>
       <x:c r="D11" s="10" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="E11" s="9"/>
-    </x:row>
-    <x:row r="12" spans="2:5">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E11" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="2:5" ht="26.350000000000001">
       <x:c r="B12" s="11">
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="8"/>
-      <x:c r="D12" s="9"/>
+      <x:c r="D12" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
       <x:c r="E12" s="9"/>
     </x:row>
     <x:row r="13" spans="2:5">

</xml_diff>

<commit_message>
add 0705 comment, 0706 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -19,7 +19,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+  <x:si>
+    <x:t>1. 요구사항 분석 (실현성 확인)
+2. 데이터 흐름도 수정
+ - 차량 관련 새소식 창 삭제 및 다른 사항 수정
+3. Menu_Tree 작성
+4. Flow_Chart 작성
+5. 필요 자료 추가 조사
+ -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+ - 컴퓨터 견적 추천 앱
+ - 주차시 사고발생 알림 앱
+2. 주제 아이디어 최종 선정
+ - 차량 관리 어플
+3. 개발 계획서 및 요구사항 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
+  </x:si>
   <x:si>
     <x:t>1. 현장실습 OT
  - 기업 소개 및 업무 설명
@@ -29,17 +59,6 @@
  - 제품 기획 
  - 개발 기획  
  - 개발 설계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성 완료
-2. 요구사항 정의 및 분류
- - 기능적 요구사항
- - 비기능적 요구사항</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -53,21 +72,6 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
- - 컴퓨터 견적 추천 앱
- - 주차시 사고발생 알림 앱
-2. 주제 아이디어 최종 선정
- - 차량 관리 어플
-3. 개발 계획서 및 요구사항 작성</x:t>
-  </x:si>
-  <x:si>
     <x:t>1-1. Datebook Comment 부분 요약
 1-2. GIT 보고서 다시 작성
 1-3. PPT 머릿글 요약 작성
@@ -76,8 +80,10 @@
 2. 요구사항 수집 및 분석</x:t>
   </x:si>
   <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
   </x:si>
   <x:si>
     <x:t>1. 요구사항 정의 및 분석 - 체계화
@@ -86,16 +92,15 @@
 3. 구현 가능 여부 확인</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
+    <x:t>1. vi 명령어 설명서 작성 완료
+2. 요구사항 정의 및 분류
+ - 기능적 요구사항
+ - 비기능적 요구사항</x:t>
   </x:si>
   <x:si>
     <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
   </x:si>
   <x:si>
     <x:t>1. 아이디어 도출
@@ -108,40 +113,19 @@
 3. 15:00 ~ 지도교수 면담</x:t>
   </x:si>
   <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 07.02 회의록 작성
+2. Git 업로드 한 것 중 중복된 것들 삭제
+3. 어플 흐름 구상도 작성
+4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
   </x:si>
   <x:si>
     <x:t>1. 진행사항 체크 및 2주차 목표 설정
@@ -152,27 +136,64 @@
 5. vi사용법 설명</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 07.02 회의록 작성
-2. Git 업로드 한 것 중 중복된 것들 삭제
-3. 어플 흐름 구상도 작성
-4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
   </x:si>
   <x:si>
     <x:t>1. 06.28 회의록 작성
 2. 요구사항 정의 및 분석</x:t>
   </x:si>
   <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
   </x:si>
   <x:si>
     <x:t>1. 인터페이스 구상도 작성
-2. 요구사항 분류하여 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Git 목록 삭제
-2. 요구사항 분석
-3. 인터페이스 구상도 작성</x:t>
+2. 요구사항 분류하여 수정
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가 자료조사</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -327,7 +348,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="20">
+  <x:cellXfs count="22">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -499,6 +520,32 @@
       <mc:Fallback>
         <x:xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="20" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="20" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -1220,8 +1267,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B2:E36"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D4" activeCellId="0" sqref="D4:D4"/>
+    <x:sheetView tabSelected="1" topLeftCell="C10" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="D12" activeCellId="0" sqref="D12:D12"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -1237,16 +1284,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D2" s="4" t="s">
+      <x:c r="E2" s="5" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="E2" s="5" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -1254,13 +1301,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="13" t="s">
-        <x:v>17</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E3" s="7" t="s">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -1268,13 +1315,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s">
-        <x:v>17</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -1282,13 +1329,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>18</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D5" s="10" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="E5" s="10" t="s">
-        <x:v>5</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -1296,13 +1343,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="16" t="s">
-        <x:v>18</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D6" s="10" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -1310,13 +1357,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="12" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D7" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E7" s="10" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D7" s="10" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E7" s="10" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -1324,13 +1371,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="12" t="s">
-        <x:v>14</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D8" s="10" t="s">
-        <x:v>7</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E8" s="10" t="s">
-        <x:v>2</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -1338,7 +1385,7 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="18" t="s">
-        <x:v>15</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D9" s="10" t="s">
         <x:v>8</x:v>
@@ -1352,45 +1399,51 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="19" t="s">
-        <x:v>13</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D10" s="10" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E10" s="10" t="s">
         <x:v>1</x:v>
-      </x:c>
-      <x:c r="E10" s="10" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
       <x:c r="B11" s="11">
         <x:v>44379</x:v>
       </x:c>
-      <x:c r="C11" s="14">
-        <x:v>0.35208333333333336</x:v>
+      <x:c r="C11" s="21" t="s">
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D11" s="10" t="s">
-        <x:v>28</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="10" t="s">
-        <x:v>24</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="2:5" ht="26.350000000000001">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="2:5" ht="105.40000000000001">
       <x:c r="B12" s="11">
         <x:v>44382</x:v>
       </x:c>
-      <x:c r="C12" s="8"/>
+      <x:c r="C12" s="20" t="s">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="D12" s="10" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="E12" s="9"/>
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E12" s="10" t="s">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="13" spans="2:5">
       <x:c r="B13" s="11">
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="8"/>
-      <x:c r="D13" s="9"/>
+      <x:c r="D13" s="9" t="s">
+        <x:v>32</x:v>
+      </x:c>
       <x:c r="E13" s="9"/>
     </x:row>
     <x:row r="14" spans="2:5">

</xml_diff>

<commit_message>
add 0706 comment, 0707 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <x:si>
     <x:t>1. 요구사항 분석 (실현성 확인)
 2. 데이터 흐름도 수정
@@ -30,25 +30,12 @@
  -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
- - 컴퓨터 견적 추천 앱
- - 주차시 사고발생 알림 앱
-2. 주제 아이디어 최종 선정
- - 차량 관리 어플
-3. 개발 계획서 및 요구사항 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
+    <x:t>1-1. Datebook Comment 부분 요약
+1-2. GIT 보고서 다시 작성
+1-3. PPT 머릿글 요약 작성
+1-4. 파일명 수정
+1-5 최종 아이디어 선정 이유 작성
+2. 요구사항 수집 및 분석</x:t>
   </x:si>
   <x:si>
     <x:t>1. 현장실습 OT
@@ -59,6 +46,146 @@
  - 제품 기획 
  - 개발 기획  
  - 개발 설계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 인터페이스 구상도 작성
+2. 요구사항 분류하여 수정
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+ - 컴퓨터 견적 추천 앱
+ - 주차시 사고발생 알림 앱
+2. 주제 아이디어 최종 선정
+ - 차량 관리 어플
+3. 개발 계획서 및 요구사항 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 07.02 회의록 작성
+2. Git 업로드 한 것 중 중복된 것들 삭제
+3. 어플 흐름 구상도 작성
+4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 필요 자료 추가 조사
+2. 한계점 및 필요기술 추가
+ - 차량 블루투스와 어플 연결 어떻게?
+ - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성 완료
+2. 요구사항 정의 및 분류
+ - 기능적 요구사항
+ - 비기능적 요구사항</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사(관련 코드)
+2. FlowChart 수정 및 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -72,128 +199,12 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>1-1. Datebook Comment 부분 요약
-1-2. GIT 보고서 다시 작성
-1-3. PPT 머릿글 요약 작성
-1-4. 파일명 수정
-1-5 최종 아이디어 선정 이유 작성
-2. 요구사항 수집 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성 완료
-2. 요구사항 정의 및 분류
- - 기능적 요구사항
- - 비기능적 요구사항</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Git 목록 삭제
-2. 요구사항 분석
-3. 인터페이스 구상도 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:25
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 07.02 회의록 작성
-2. Git 업로드 한 것 중 중복된 것들 삭제
-3. 어플 흐름 구상도 작성
-4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 진행사항 체크 및 2주차 목표 설정
-2. 06.28 회의록 작성
-3. 상용화 된 타 앱 기능 분석
-4. 요구사항 정의
- - 회원가입, DB, 무결성 (미완)
-5. vi사용법 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 인터페이스 구상도 작성
-2. 요구사항 분류하여 수정
-3. 추가 자료조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가 자료조사</x:t>
+    <x:t>1. 앱 화면별 Sequence 작성
+2. 앱 화면별 어떻게 구성할 것인지 구상</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -348,7 +359,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="22">
+  <x:cellXfs count="23">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -571,6 +582,19 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="20" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
@@ -1267,8 +1291,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B2:E36"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="C10" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D12" activeCellId="0" sqref="D12:D12"/>
+    <x:sheetView tabSelected="1" topLeftCell="C8" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="E14" activeCellId="0" sqref="E14:E14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -1284,16 +1308,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D2" s="4" t="s">
-        <x:v>21</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -1301,13 +1325,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="13" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
-        <x:v>30</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E3" s="7" t="s">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -1315,13 +1339,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>7</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
-        <x:v>5</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -1329,13 +1353,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D5" s="10" t="s">
-        <x:v>11</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E5" s="10" t="s">
-        <x:v>2</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -1343,13 +1367,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="16" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D6" s="10" t="s">
-        <x:v>6</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -1360,10 +1384,10 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="D7" s="10" t="s">
-        <x:v>19</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E7" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -1371,13 +1395,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="12" t="s">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D8" s="10" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E8" s="10" t="s">
-        <x:v>9</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -1388,10 +1412,10 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="D9" s="10" t="s">
-        <x:v>8</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E9" s="10" t="s">
-        <x:v>12</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -1399,13 +1423,13 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="19" t="s">
-        <x:v>26</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D10" s="10" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E10" s="10" t="s">
-        <x:v>1</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
@@ -1413,13 +1437,13 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="21" t="s">
-        <x:v>17</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D11" s="10" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E11" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:5" ht="105.40000000000001">
@@ -1427,31 +1451,37 @@
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="20" t="s">
-        <x:v>14</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D12" s="10" t="s">
-        <x:v>31</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E12" s="10" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="2:5">
+    <x:row r="13" spans="2:5" ht="52.700000000000003">
       <x:c r="B13" s="11">
         <x:v>44383</x:v>
       </x:c>
-      <x:c r="C13" s="8"/>
-      <x:c r="D13" s="9" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E13" s="9"/>
-    </x:row>
-    <x:row r="14" spans="2:5">
+      <x:c r="C13" s="22" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D13" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E13" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="2:5" ht="26.350000000000001">
       <x:c r="B14" s="11">
         <x:v>44384</x:v>
       </x:c>
       <x:c r="C14" s="8"/>
-      <x:c r="D14" s="9"/>
+      <x:c r="D14" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
       <x:c r="E14" s="9"/>
     </x:row>
     <x:row r="15" spans="2:5">

</xml_diff>

<commit_message>
add 0707 comment, 0708 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -19,7 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
+  </x:si>
   <x:si>
     <x:t>1. 요구사항 분석 (실현성 확인)
 2. 데이터 흐름도 수정
@@ -30,12 +38,21 @@
  -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
   </x:si>
   <x:si>
-    <x:t>1-1. Datebook Comment 부분 요약
-1-2. GIT 보고서 다시 작성
-1-3. PPT 머릿글 요약 작성
-1-4. 파일명 수정
-1-5 최종 아이디어 선정 이유 작성
-2. 요구사항 수집 및 분석</x:t>
+    <x:t>1. (2-2) 수익적 요소 추가
+2. (4-1) 기능정의 추가
+3. 추가 자료 조사
+ - 비슷한 어플(마이클) 화면 구성 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 07.02 회의록 작성
+2. Git 업로드 한 것 중 중복된 것들 삭제
+3. 어플 흐름 구상도 작성
+4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사
+2. 요구사항 추가 조사
+3. 경쟁 어플 기능 비교 보완</x:t>
   </x:si>
   <x:si>
     <x:t>1. 현장실습 OT
@@ -48,31 +65,18 @@
  - 개발 설계</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 인터페이스 구상도 작성
-2. 요구사항 분류하여 수정
-3. 추가 자료조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
+    <x:t>1. 필요 자료 추가 조사
+2. 한계점 및 필요기술 추가
+ - 차량 블루투스와 어플 연결 어떻게?
+ - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1-1. Datebook Comment 부분 요약
+1-2. GIT 보고서 다시 작성
+1-3. PPT 머릿글 요약 작성
+1-4. 파일명 수정
+1-5 최종 아이디어 선정 이유 작성
+2. 요구사항 수집 및 분석</x:t>
   </x:si>
   <x:si>
     <x:t>1. 아이디어 도출
@@ -83,109 +87,11 @@
 3. 개발 계획서 및 요구사항 작성</x:t>
   </x:si>
   <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 진행사항 체크 및 2주차 목표 설정
-2. 06.28 회의록 작성
-3. 상용화 된 타 앱 기능 분석
-4. 요구사항 정의
- - 회원가입, DB, 무결성 (미완)
-5. vi사용법 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 07.02 회의록 작성
-2. Git 업로드 한 것 중 중복된 것들 삭제
-3. 어플 흐름 구상도 작성
-4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Git 목록 삭제
-2. 요구사항 분석
-3. 인터페이스 구상도 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 필요 자료 추가 조사
-2. 한계점 및 필요기술 추가
- - 차량 블루투스와 어플 연결 어떻게?
- - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성 완료
-2. 요구사항 정의 및 분류
- - 기능적 요구사항
- - 비기능적 요구사항</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:25
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 추가 자료조사(관련 코드)
-2. FlowChart 수정 및 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -199,12 +105,122 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
+    <x:t>08:22
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 인터페이스 구상도 작성
+2. 요구사항 분류하여 수정
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사(관련 코드)
+2. FlowChart 수정 및 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성 완료
+2. 요구사항 정의 및 분류
+ - 기능적 요구사항
+ - 비기능적 요구사항</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
   </x:si>
   <x:si>
     <x:t>1. 앱 화면별 Sequence 작성
-2. 앱 화면별 어떻게 구성할 것인지 구상</x:t>
+2. 앱 화면별 어떻게 구성할 것인지 구상
+3. 추가 자료조사</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -359,7 +375,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="23">
+  <x:cellXfs count="24">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -582,6 +598,19 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="20" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
@@ -1291,8 +1320,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B2:E36"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="C8" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="E14" activeCellId="0" sqref="E14:E14"/>
+    <x:sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="D15" activeCellId="0" sqref="D15:D15"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -1308,16 +1337,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>10</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D2" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E2" s="5" t="s">
-        <x:v>12</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -1325,13 +1354,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="13" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D3" s="7" t="s">
-        <x:v>33</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E3" s="7" t="s">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -1339,13 +1368,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>19</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
-        <x:v>32</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -1353,10 +1382,10 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D5" s="10" t="s">
-        <x:v>4</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E5" s="10" t="s">
         <x:v>8</x:v>
@@ -1367,13 +1396,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="16" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D6" s="10" t="s">
-        <x:v>1</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -1381,13 +1410,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="12" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D7" s="10" t="s">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E7" s="10" t="s">
-        <x:v>13</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -1395,13 +1424,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="12" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D8" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E8" s="10" t="s">
-        <x:v>21</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -1409,13 +1438,13 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="18" t="s">
-        <x:v>29</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D9" s="10" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E9" s="10" t="s">
-        <x:v>3</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -1423,13 +1452,13 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="19" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D10" s="10" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E10" s="10" t="s">
-        <x:v>17</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
@@ -1437,13 +1466,13 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="21" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D11" s="10" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="E11" s="10" t="s">
-        <x:v>14</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:5" ht="105.40000000000001">
@@ -1454,10 +1483,10 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="D12" s="10" t="s">
-        <x:v>6</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E12" s="10" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="2:5" ht="52.700000000000003">
@@ -1465,31 +1494,37 @@
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="22" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D13" s="10" t="s">
-        <x:v>30</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E13" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="2:5" ht="26.350000000000001">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="2:5" ht="52.700000000000003">
       <x:c r="B14" s="11">
         <x:v>44384</x:v>
       </x:c>
-      <x:c r="C14" s="8"/>
+      <x:c r="C14" s="23" t="s">
+        <x:v>11</x:v>
+      </x:c>
       <x:c r="D14" s="10" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="E14" s="9"/>
-    </x:row>
-    <x:row r="15" spans="2:5">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="E14" s="10" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="2:5" ht="39.549999999999997">
       <x:c r="B15" s="11">
         <x:v>44385</x:v>
       </x:c>
       <x:c r="C15" s="8"/>
-      <x:c r="D15" s="9"/>
+      <x:c r="D15" s="10" t="s">
+        <x:v>4</x:v>
+      </x:c>
       <x:c r="E15" s="9"/>
     </x:row>
     <x:row r="16" spans="2:5">

</xml_diff>

<commit_message>
add 2sheet Menu_Tree, Def_Func add 0709 comment, 0712 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8568" activeTab="2"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8568"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Datebook" sheetId="1" r:id="rId4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="240">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="242">
   <x:si>
     <x:t>1. 요구사항 수집 및 정의
  - 관련 필요 자료 조사
@@ -279,6 +279,10 @@
     <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
   </x:si>
   <x:si>
+    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
+2. 요구사항 추가 및 수정</x:t>
+  </x:si>
+  <x:si>
     <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
 로그인 버튼이 나와야 한다.</x:t>
   </x:si>
@@ -712,6 +716,10 @@
   </x:si>
   <x:si>
     <x:t>봄</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 플로우 차트 작성
+2. 설계 계획서 작성</x:t>
   </x:si>
   <x:si>
     <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
@@ -2867,9 +2875,9 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B2:E42"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="2" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24:E24"/>
+      <x:selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18:D18"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -2885,16 +2893,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="4" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C2" s="5" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D2" s="5" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="E2" s="6" t="s">
         <x:v>86</x:v>
-      </x:c>
-      <x:c r="C2" s="5" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="D2" s="5" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="E2" s="6" t="s">
-        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -2902,10 +2910,10 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="14" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="D3" s="8" t="s">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="E3" s="8" t="s">
         <x:v>13</x:v>
@@ -2916,7 +2924,7 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="13" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="D4" s="11" t="s">
         <x:v>51</x:v>
@@ -2930,10 +2938,10 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="15" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D5" s="11" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E5" s="11" t="s">
         <x:v>5</x:v>
@@ -2944,7 +2952,7 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="17" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D6" s="11" t="s">
         <x:v>9</x:v>
@@ -2958,10 +2966,10 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="13" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="D7" s="11" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="E7" s="11" t="s">
         <x:v>46</x:v>
@@ -2972,7 +2980,7 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="13" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="D8" s="11" t="s">
         <x:v>30</x:v>
@@ -2986,13 +2994,13 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="18" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="D9" s="11" t="s">
         <x:v>52</x:v>
       </x:c>
       <x:c r="E9" s="11" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -3000,7 +3008,7 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="19" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="D10" s="11" t="s">
         <x:v>36</x:v>
@@ -3014,7 +3022,7 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="21" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="D11" s="11" t="s">
         <x:v>55</x:v>
@@ -3028,7 +3036,7 @@
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="20" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D12" s="11" t="s">
         <x:v>38</x:v>
@@ -3042,13 +3050,13 @@
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="22" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="D13" s="11" t="s">
         <x:v>54</x:v>
       </x:c>
       <x:c r="E13" s="11" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5" ht="52.700000000000003">
@@ -3056,7 +3064,7 @@
         <x:v>44384</x:v>
       </x:c>
       <x:c r="C14" s="23" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D14" s="11" t="s">
         <x:v>50</x:v>
@@ -3070,7 +3078,7 @@
         <x:v>44385</x:v>
       </x:c>
       <x:c r="C15" s="29" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D15" s="11" t="s">
         <x:v>37</x:v>
@@ -3087,16 +3095,20 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="D16" s="11" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="E16" s="10"/>
-    </x:row>
-    <x:row r="17" spans="2:5">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="E16" s="11" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="2:5" ht="26.350000000000001">
       <x:c r="B17" s="12">
         <x:v>44389</x:v>
       </x:c>
       <x:c r="C17" s="9"/>
-      <x:c r="D17" s="10"/>
+      <x:c r="D17" s="11" t="s">
+        <x:v>199</x:v>
+      </x:c>
       <x:c r="E17" s="10"/>
     </x:row>
     <x:row r="18" spans="2:5">
@@ -3327,54 +3339,54 @@
   <x:sheetData>
     <x:row r="1" spans="1:9" ht="17.149999999999999">
       <x:c r="A1" s="25" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B1" s="43" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C1" s="44" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D1" s="44" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E1" s="44" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F1" s="44" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G1" s="44" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="H1" s="44" t="s">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="I1" s="45" t="s">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:9">
       <x:c r="A2" s="38" t="s">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B2" s="30" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="C2" s="33" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D2" s="33" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E2" s="48" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F2" s="48"/>
       <x:c r="G2" s="48"/>
       <x:c r="H2" s="48"/>
       <x:c r="I2" s="48" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9">
@@ -3383,13 +3395,13 @@
       <x:c r="C3" s="34"/>
       <x:c r="D3" s="34"/>
       <x:c r="E3" s="47" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F3" s="47"/>
       <x:c r="G3" s="47"/>
       <x:c r="H3" s="47"/>
       <x:c r="I3" s="47" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
@@ -3398,7 +3410,7 @@
       <x:c r="C4" s="34"/>
       <x:c r="D4" s="34"/>
       <x:c r="E4" s="47" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F4" s="47"/>
       <x:c r="G4" s="47"/>
@@ -3411,10 +3423,10 @@
       <x:c r="C5" s="34"/>
       <x:c r="D5" s="34"/>
       <x:c r="E5" s="36" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F5" s="47" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G5" s="47"/>
       <x:c r="H5" s="47"/>
@@ -3427,7 +3439,7 @@
       <x:c r="D6" s="35"/>
       <x:c r="E6" s="35"/>
       <x:c r="F6" s="47" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G6" s="47"/>
       <x:c r="H6" s="47"/>
@@ -3438,10 +3450,10 @@
       <x:c r="B7" s="31"/>
       <x:c r="C7" s="34"/>
       <x:c r="D7" s="36" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="E7" s="47" t="s">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F7" s="47"/>
       <x:c r="G7" s="47"/>
@@ -3454,7 +3466,7 @@
       <x:c r="C8" s="34"/>
       <x:c r="D8" s="34"/>
       <x:c r="E8" s="47" t="s">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F8" s="47"/>
       <x:c r="G8" s="47"/>
@@ -3469,13 +3481,13 @@
       <x:c r="C9" s="34"/>
       <x:c r="D9" s="34"/>
       <x:c r="E9" s="47" t="s">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F9" s="47"/>
       <x:c r="G9" s="47"/>
       <x:c r="H9" s="47"/>
       <x:c r="I9" s="47" t="s">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
@@ -3484,10 +3496,10 @@
       <x:c r="C10" s="34"/>
       <x:c r="D10" s="34"/>
       <x:c r="E10" s="36" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F10" s="47" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="G10" s="47"/>
       <x:c r="H10" s="47"/>
@@ -3500,12 +3512,12 @@
       <x:c r="D11" s="34"/>
       <x:c r="E11" s="34"/>
       <x:c r="F11" s="47" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="G11" s="47"/>
       <x:c r="H11" s="47"/>
       <x:c r="I11" s="47" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
@@ -3515,7 +3527,7 @@
       <x:c r="D12" s="34"/>
       <x:c r="E12" s="34"/>
       <x:c r="F12" s="47" t="s">
-        <x:v>203</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="G12" s="47"/>
       <x:c r="H12" s="47"/>
@@ -3559,19 +3571,19 @@
       <x:c r="A14" s="39"/>
       <x:c r="B14" s="31"/>
       <x:c r="C14" s="36" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="D14" s="36" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="E14" s="47" t="s">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F14" s="47"/>
       <x:c r="G14" s="47"/>
       <x:c r="H14" s="47"/>
       <x:c r="I14" s="47" t="s">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="J14" s="28"/>
       <x:c r="K14" s="28"/>
@@ -3599,7 +3611,7 @@
       <x:c r="C15" s="34"/>
       <x:c r="D15" s="34"/>
       <x:c r="E15" s="47" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F15" s="47"/>
       <x:c r="G15" s="47"/>
@@ -3633,7 +3645,7 @@
       <x:c r="C16" s="34"/>
       <x:c r="D16" s="34"/>
       <x:c r="E16" s="47" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F16" s="47"/>
       <x:c r="G16" s="47"/>
@@ -3664,13 +3676,13 @@
       <x:c r="C17" s="34"/>
       <x:c r="D17" s="35"/>
       <x:c r="E17" s="47" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F17" s="47"/>
       <x:c r="G17" s="47"/>
       <x:c r="H17" s="47"/>
       <x:c r="I17" s="47" t="s">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="J17" s="28"/>
       <x:c r="K17" s="28"/>
@@ -3697,13 +3709,13 @@
       <x:c r="B18" s="31"/>
       <x:c r="C18" s="34"/>
       <x:c r="D18" s="47" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="E18" s="47" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F18" s="47" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G18" s="47"/>
       <x:c r="H18" s="47"/>
@@ -3733,14 +3745,14 @@
       <x:c r="B19" s="31"/>
       <x:c r="C19" s="34"/>
       <x:c r="D19" s="47" t="s">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="E19" s="47"/>
       <x:c r="F19" s="47"/>
       <x:c r="G19" s="47"/>
       <x:c r="H19" s="47"/>
       <x:c r="I19" s="36" t="s">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="J19" s="28"/>
       <x:c r="K19" s="28"/>
@@ -3767,7 +3779,7 @@
       <x:c r="B20" s="31"/>
       <x:c r="C20" s="34"/>
       <x:c r="D20" s="47" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="E20" s="47"/>
       <x:c r="F20" s="47"/>
@@ -3799,7 +3811,7 @@
       <x:c r="B21" s="31"/>
       <x:c r="C21" s="34"/>
       <x:c r="D21" s="47" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E21" s="47"/>
       <x:c r="F21" s="47"/>
@@ -3831,7 +3843,7 @@
       <x:c r="B22" s="32"/>
       <x:c r="C22" s="35"/>
       <x:c r="D22" s="47" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="E22" s="47"/>
       <x:c r="F22" s="47"/>
@@ -3861,10 +3873,10 @@
     <x:row r="23" spans="1:28">
       <x:c r="A23" s="39"/>
       <x:c r="B23" s="37" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C23" s="47" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D23" s="47"/>
       <x:c r="E23" s="47"/>
@@ -3896,7 +3908,7 @@
       <x:c r="A24" s="39"/>
       <x:c r="B24" s="31"/>
       <x:c r="C24" s="47" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D24" s="47"/>
       <x:c r="E24" s="47"/>
@@ -3928,7 +3940,7 @@
       <x:c r="A25" s="39"/>
       <x:c r="B25" s="31"/>
       <x:c r="C25" s="47" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D25" s="47"/>
       <x:c r="E25" s="47"/>
@@ -3960,13 +3972,13 @@
       <x:c r="A26" s="39"/>
       <x:c r="B26" s="31"/>
       <x:c r="C26" s="36" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D26" s="47" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="E26" s="47" t="s">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F26" s="47"/>
       <x:c r="G26" s="47"/>
@@ -4056,10 +4068,10 @@
       <x:c r="B27" s="37"/>
       <x:c r="C27" s="34"/>
       <x:c r="D27" s="36" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="E27" s="47" t="s">
-        <x:v>207</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="F27" s="47" t="s">
         <x:v>49</x:v>
@@ -4152,7 +4164,7 @@
       <x:c r="C28" s="34"/>
       <x:c r="D28" s="35"/>
       <x:c r="E28" s="47" t="s">
-        <x:v>226</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F28" s="47" t="s">
         <x:v>49</x:v>
@@ -4244,10 +4256,10 @@
       <x:c r="B29" s="31"/>
       <x:c r="C29" s="34"/>
       <x:c r="D29" s="47" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="E29" s="49" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F29" s="49"/>
       <x:c r="G29" s="47"/>
@@ -4337,10 +4349,10 @@
       <x:c r="B30" s="31"/>
       <x:c r="C30" s="34"/>
       <x:c r="D30" s="47" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="E30" s="47" t="s">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F30" s="47"/>
       <x:c r="G30" s="47"/>
@@ -4431,7 +4443,7 @@
       <x:c r="C31" s="34"/>
       <x:c r="D31" s="47"/>
       <x:c r="E31" s="47" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F31" s="47"/>
       <x:c r="G31" s="47"/>
@@ -4521,10 +4533,10 @@
       <x:c r="B32" s="31"/>
       <x:c r="C32" s="34"/>
       <x:c r="D32" s="47" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="E32" s="47" t="s">
-        <x:v>200</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F32" s="47"/>
       <x:c r="G32" s="47"/>
@@ -4614,7 +4626,7 @@
       <x:c r="B33" s="31"/>
       <x:c r="C33" s="35"/>
       <x:c r="D33" s="47" t="s">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="E33" s="47"/>
       <x:c r="F33" s="47"/>
@@ -4707,7 +4719,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="D34" s="47" t="s">
-        <x:v>229</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="E34" s="47"/>
       <x:c r="F34" s="47"/>
@@ -4798,7 +4810,7 @@
       <x:c r="B35" s="31"/>
       <x:c r="C35" s="34"/>
       <x:c r="D35" s="47" t="s">
-        <x:v>202</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="E35" s="47"/>
       <x:c r="F35" s="47"/>
@@ -4889,7 +4901,7 @@
       <x:c r="B36" s="31"/>
       <x:c r="C36" s="34"/>
       <x:c r="D36" s="47" t="s">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="E36" s="47"/>
       <x:c r="F36" s="47"/>
@@ -4980,7 +4992,7 @@
       <x:c r="B37" s="31"/>
       <x:c r="C37" s="34"/>
       <x:c r="D37" s="47" t="s">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="E37" s="47"/>
       <x:c r="F37" s="47"/>
@@ -5071,7 +5083,7 @@
       <x:c r="B38" s="31"/>
       <x:c r="C38" s="34"/>
       <x:c r="D38" s="47" t="s">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="E38" s="47"/>
       <x:c r="F38" s="47"/>
@@ -5162,7 +5174,7 @@
       <x:c r="B39" s="37"/>
       <x:c r="C39" s="35"/>
       <x:c r="D39" s="47" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="E39" s="47"/>
       <x:c r="F39" s="47"/>
@@ -5251,10 +5263,10 @@
     <x:row r="40" spans="1:87">
       <x:c r="A40" s="39"/>
       <x:c r="B40" s="37" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C40" s="47" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="D40" s="47"/>
       <x:c r="E40" s="47"/>
@@ -5345,7 +5357,7 @@
       <x:c r="A41" s="39"/>
       <x:c r="B41" s="31"/>
       <x:c r="C41" s="47" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D41" s="47"/>
       <x:c r="E41" s="47"/>
@@ -5436,7 +5448,7 @@
       <x:c r="A42" s="39"/>
       <x:c r="B42" s="31"/>
       <x:c r="C42" s="47" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D42" s="47"/>
       <x:c r="E42" s="47"/>
@@ -5527,7 +5539,7 @@
       <x:c r="A43" s="39"/>
       <x:c r="B43" s="31"/>
       <x:c r="C43" s="47" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="D43" s="47"/>
       <x:c r="E43" s="47"/>
@@ -5618,7 +5630,7 @@
       <x:c r="A44" s="39"/>
       <x:c r="B44" s="31"/>
       <x:c r="C44" s="47" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D44" s="47"/>
       <x:c r="E44" s="47"/>
@@ -5709,7 +5721,7 @@
       <x:c r="A45" s="39"/>
       <x:c r="B45" s="32"/>
       <x:c r="C45" s="47" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="D45" s="47"/>
       <x:c r="E45" s="47"/>
@@ -5799,10 +5811,10 @@
     <x:row r="46" spans="1:87">
       <x:c r="A46" s="39"/>
       <x:c r="B46" s="37" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C46" s="47" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="D46" s="47"/>
       <x:c r="E46" s="47"/>
@@ -5893,7 +5905,7 @@
       <x:c r="A47" s="39"/>
       <x:c r="B47" s="31"/>
       <x:c r="C47" s="47" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D47" s="47"/>
       <x:c r="E47" s="47"/>
@@ -5984,7 +5996,7 @@
       <x:c r="A48" s="39"/>
       <x:c r="B48" s="31"/>
       <x:c r="C48" s="47" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D48" s="47"/>
       <x:c r="E48" s="47"/>
@@ -6075,7 +6087,7 @@
       <x:c r="A49" s="39"/>
       <x:c r="B49" s="32"/>
       <x:c r="C49" s="47" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="D49" s="47"/>
       <x:c r="E49" s="47"/>
@@ -6165,13 +6177,13 @@
     <x:row r="50" spans="1:87">
       <x:c r="A50" s="39"/>
       <x:c r="B50" s="37" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C50" s="36" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D50" s="47" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="E50" s="47"/>
       <x:c r="F50" s="47"/>
@@ -6262,7 +6274,7 @@
       <x:c r="B51" s="31"/>
       <x:c r="C51" s="35"/>
       <x:c r="D51" s="47" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E51" s="47"/>
       <x:c r="F51" s="47"/>
@@ -6352,10 +6364,10 @@
       <x:c r="A52" s="39"/>
       <x:c r="B52" s="31"/>
       <x:c r="C52" s="36" t="s">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D52" s="47" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="E52" s="47"/>
       <x:c r="F52" s="47"/>
@@ -6446,7 +6458,7 @@
       <x:c r="B53" s="31"/>
       <x:c r="C53" s="35"/>
       <x:c r="D53" s="47" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="E53" s="47"/>
       <x:c r="F53" s="47"/>
@@ -6536,10 +6548,10 @@
       <x:c r="A54" s="39"/>
       <x:c r="B54" s="31"/>
       <x:c r="C54" s="36" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="D54" s="47" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="E54" s="47"/>
       <x:c r="F54" s="47"/>
@@ -6630,7 +6642,7 @@
       <x:c r="B55" s="31"/>
       <x:c r="C55" s="34"/>
       <x:c r="D55" s="47" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="E55" s="47"/>
       <x:c r="F55" s="47"/>
@@ -6721,7 +6733,7 @@
       <x:c r="B56" s="31"/>
       <x:c r="C56" s="35"/>
       <x:c r="D56" s="47" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="E56" s="47"/>
       <x:c r="F56" s="47"/>
@@ -6811,10 +6823,10 @@
       <x:c r="A57" s="39"/>
       <x:c r="B57" s="31"/>
       <x:c r="C57" s="36" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="D57" s="47" t="s">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E57" s="47"/>
       <x:c r="F57" s="47"/>
@@ -6905,7 +6917,7 @@
       <x:c r="B58" s="31"/>
       <x:c r="C58" s="35"/>
       <x:c r="D58" s="47" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="E58" s="47"/>
       <x:c r="F58" s="47"/>
@@ -6995,10 +7007,10 @@
       <x:c r="A59" s="39"/>
       <x:c r="B59" s="31"/>
       <x:c r="C59" s="36" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="D59" s="47" t="s">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E59" s="47"/>
       <x:c r="F59" s="47"/>
@@ -7089,7 +7101,7 @@
       <x:c r="B60" s="31"/>
       <x:c r="C60" s="35"/>
       <x:c r="D60" s="47" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E60" s="47"/>
       <x:c r="F60" s="47"/>
@@ -7179,10 +7191,10 @@
       <x:c r="A61" s="39"/>
       <x:c r="B61" s="31"/>
       <x:c r="C61" s="36" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="D61" s="47" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="E61" s="47"/>
       <x:c r="F61" s="47"/>
@@ -7273,7 +7285,7 @@
       <x:c r="B62" s="32"/>
       <x:c r="C62" s="35"/>
       <x:c r="D62" s="47" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="E62" s="47"/>
       <x:c r="F62" s="47"/>
@@ -9297,9 +9309,9 @@
   <x:sheetPr codeName="Sheet3"/>
   <x:dimension ref="A1:H60"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <x:sheetView topLeftCell="A1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="F26" activeCellId="0" sqref="F26:F26"/>
+      <x:selection pane="bottomLeft" activeCell="F35" activeCellId="0" sqref="F35:F35"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
@@ -9315,28 +9327,28 @@
   <x:sheetData>
     <x:row r="1" spans="1:8" ht="17.149999999999999">
       <x:c r="A1" s="42" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B1" s="43" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C1" s="44" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D1" s="44" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E1" s="44" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="F1" s="44" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G1" s="44" t="s">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="H1" s="45" t="s">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8" ht="16.75" customHeight="1">
@@ -9347,13 +9359,13 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C2" s="74" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D2" s="79" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="E2" s="80" t="s">
-        <x:v>210</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="F2" s="80"/>
       <x:c r="G2" s="80"/>
@@ -9367,12 +9379,12 @@
       <x:c r="C3" s="75"/>
       <x:c r="D3" s="81"/>
       <x:c r="E3" s="82" t="s">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F3" s="82"/>
       <x:c r="G3" s="82"/>
       <x:c r="H3" s="82" t="s">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -9381,7 +9393,7 @@
       <x:c r="C4" s="75"/>
       <x:c r="D4" s="83"/>
       <x:c r="E4" s="82" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="F4" s="82"/>
       <x:c r="G4" s="82"/>
@@ -9394,15 +9406,15 @@
       <x:c r="B5" s="31"/>
       <x:c r="C5" s="75"/>
       <x:c r="D5" s="84" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="E5" s="85" t="s">
-        <x:v>224</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F5" s="82"/>
       <x:c r="G5" s="82"/>
       <x:c r="H5" s="82" t="s">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -9411,7 +9423,7 @@
       <x:c r="C6" s="54"/>
       <x:c r="D6" s="83"/>
       <x:c r="E6" s="85" t="s">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F6" s="82"/>
       <x:c r="G6" s="82"/>
@@ -9423,16 +9435,16 @@
       <x:c r="A7" s="39"/>
       <x:c r="B7" s="31"/>
       <x:c r="C7" s="53" t="s">
-        <x:v>218</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="D7" s="84" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="E7" s="84" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F7" s="82" t="s">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="G7" s="82"/>
       <x:c r="H7" s="82"/>
@@ -9444,7 +9456,7 @@
       <x:c r="D8" s="81"/>
       <x:c r="E8" s="81"/>
       <x:c r="F8" s="82" t="s">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G8" s="82"/>
       <x:c r="H8" s="82"/>
@@ -9456,7 +9468,7 @@
       <x:c r="D9" s="81"/>
       <x:c r="E9" s="81"/>
       <x:c r="F9" s="82" t="s">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="G9" s="82"/>
       <x:c r="H9" s="82"/>
@@ -9468,7 +9480,7 @@
       <x:c r="D10" s="81"/>
       <x:c r="E10" s="81"/>
       <x:c r="F10" s="82" t="s">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="G10" s="82"/>
       <x:c r="H10" s="82"/>
@@ -9480,7 +9492,7 @@
       <x:c r="D11" s="88"/>
       <x:c r="E11" s="88"/>
       <x:c r="F11" s="89" t="s">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="G11" s="89"/>
       <x:c r="H11" s="89"/>
@@ -9491,10 +9503,10 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C12" s="75" t="s">
-        <x:v>225</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="D12" s="80" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="E12" s="81" t="s">
         <x:v>19</x:v>
@@ -9508,7 +9520,7 @@
       <x:c r="B13" s="31"/>
       <x:c r="C13" s="75"/>
       <x:c r="D13" s="85" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="E13" s="81"/>
       <x:c r="F13" s="82"/>
@@ -9520,7 +9532,7 @@
       <x:c r="B14" s="31"/>
       <x:c r="C14" s="75"/>
       <x:c r="D14" s="85" t="s">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="E14" s="81"/>
       <x:c r="F14" s="82"/>
@@ -9532,7 +9544,7 @@
       <x:c r="B15" s="31"/>
       <x:c r="C15" s="54"/>
       <x:c r="D15" s="85" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="E15" s="83"/>
       <x:c r="F15" s="82"/>
@@ -9549,14 +9561,14 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="E16" s="84" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F16" s="82" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="G16" s="82"/>
       <x:c r="H16" s="84" t="s">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -9564,11 +9576,11 @@
       <x:c r="B17" s="31"/>
       <x:c r="C17" s="54"/>
       <x:c r="D17" s="82" t="s">
-        <x:v>205</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="E17" s="83"/>
       <x:c r="F17" s="82" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G17" s="82"/>
       <x:c r="H17" s="83"/>
@@ -9590,13 +9602,13 @@
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="39"/>
       <x:c r="B19" s="31" t="s">
-        <x:v>232</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="C19" s="75" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D19" s="80" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="E19" s="80"/>
       <x:c r="F19" s="80"/>
@@ -9608,7 +9620,7 @@
       <x:c r="B20" s="31"/>
       <x:c r="C20" s="75"/>
       <x:c r="D20" s="82" t="s">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="E20" s="82"/>
       <x:c r="F20" s="82"/>
@@ -9620,7 +9632,7 @@
       <x:c r="B21" s="31"/>
       <x:c r="C21" s="75"/>
       <x:c r="D21" s="82" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E21" s="82"/>
       <x:c r="F21" s="82"/>
@@ -9632,7 +9644,7 @@
       <x:c r="B22" s="31"/>
       <x:c r="C22" s="75"/>
       <x:c r="D22" s="82" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="E22" s="82"/>
       <x:c r="F22" s="82"/>
@@ -9644,7 +9656,7 @@
       <x:c r="B23" s="31"/>
       <x:c r="C23" s="54"/>
       <x:c r="D23" s="82" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="E23" s="82"/>
       <x:c r="F23" s="82"/>
@@ -9655,13 +9667,13 @@
       <x:c r="A24" s="38"/>
       <x:c r="B24" s="37"/>
       <x:c r="C24" s="53" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="D24" s="84" t="s">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="E24" s="82" t="s">
-        <x:v>222</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F24" s="82"/>
       <x:c r="G24" s="82"/>
@@ -9673,7 +9685,7 @@
       <x:c r="C25" s="75"/>
       <x:c r="D25" s="83"/>
       <x:c r="E25" s="82" t="s">
-        <x:v>235</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F25" s="82"/>
       <x:c r="G25" s="82"/>
@@ -9687,7 +9699,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="E26" s="82" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F26" s="82"/>
       <x:c r="G26" s="82"/>
@@ -9699,7 +9711,7 @@
       <x:c r="C27" s="75"/>
       <x:c r="D27" s="81"/>
       <x:c r="E27" s="82" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F27" s="82"/>
       <x:c r="G27" s="82"/>
@@ -9711,7 +9723,7 @@
       <x:c r="C28" s="75"/>
       <x:c r="D28" s="81"/>
       <x:c r="E28" s="82" t="s">
-        <x:v>220</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="F28" s="82"/>
       <x:c r="G28" s="82"/>
@@ -9723,7 +9735,7 @@
       <x:c r="C29" s="87"/>
       <x:c r="D29" s="88"/>
       <x:c r="E29" s="89" t="s">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F29" s="89"/>
       <x:c r="G29" s="89"/>
@@ -9732,10 +9744,10 @@
     <x:row r="30" spans="1:8">
       <x:c r="A30" s="39"/>
       <x:c r="B30" s="31" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C30" s="91" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="D30" s="80"/>
       <x:c r="E30" s="80"/>
@@ -9747,7 +9759,7 @@
       <x:c r="A31" s="39"/>
       <x:c r="B31" s="31"/>
       <x:c r="C31" s="76" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D31" s="82"/>
       <x:c r="E31" s="82"/>
@@ -9759,7 +9771,7 @@
       <x:c r="A32" s="39"/>
       <x:c r="B32" s="31"/>
       <x:c r="C32" s="76" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D32" s="82"/>
       <x:c r="E32" s="82"/>
@@ -9771,7 +9783,7 @@
       <x:c r="A33" s="39"/>
       <x:c r="B33" s="69"/>
       <x:c r="C33" s="92" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="D33" s="89"/>
       <x:c r="E33" s="89"/>
@@ -9782,10 +9794,10 @@
     <x:row r="34" spans="1:8">
       <x:c r="A34" s="39"/>
       <x:c r="B34" s="31" t="s">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="C34" s="91" t="s">
-        <x:v>233</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="D34" s="80"/>
       <x:c r="E34" s="80"/>
@@ -9797,10 +9809,10 @@
       <x:c r="A35" s="39"/>
       <x:c r="B35" s="31"/>
       <x:c r="C35" s="53" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="D35" s="82" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="E35" s="82"/>
       <x:c r="F35" s="82"/>
@@ -9812,7 +9824,7 @@
       <x:c r="B36" s="31"/>
       <x:c r="C36" s="75"/>
       <x:c r="D36" s="82" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="E36" s="82"/>
       <x:c r="F36" s="82"/>
@@ -9824,7 +9836,7 @@
       <x:c r="B37" s="69"/>
       <x:c r="C37" s="87"/>
       <x:c r="D37" s="89" t="s">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="E37" s="89"/>
       <x:c r="F37" s="89"/>
@@ -10148,7 +10160,7 @@
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="62"/>
       <x:c r="B2" s="46" t="s">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="C2" s="46" t="s">
         <x:v>20</x:v>
@@ -10157,22 +10169,22 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="E2" s="46" t="s">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F2" s="46" t="s">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="62"/>
       <x:c r="B3" s="30" t="s">
-        <x:v>234</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="C3" s="33" t="s">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="D3" s="33" t="s">
-        <x:v>206</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="E3" s="63" t="s">
         <x:v>57</x:v>
@@ -10185,7 +10197,7 @@
       <x:c r="C4" s="34"/>
       <x:c r="D4" s="34"/>
       <x:c r="E4" s="64" t="s">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F4" s="94"/>
     </x:row>
@@ -10195,7 +10207,7 @@
       <x:c r="C5" s="34"/>
       <x:c r="D5" s="34"/>
       <x:c r="E5" s="64" t="s">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F5" s="94"/>
     </x:row>
@@ -10205,7 +10217,7 @@
       <x:c r="C6" s="34"/>
       <x:c r="D6" s="34"/>
       <x:c r="E6" s="64" t="s">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="F6" s="94"/>
     </x:row>
@@ -10224,7 +10236,7 @@
       <x:c r="B8" s="31"/>
       <x:c r="C8" s="34"/>
       <x:c r="D8" s="36" t="s">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="E8" s="66" t="s">
         <x:v>58</x:v>
@@ -10247,7 +10259,7 @@
       <x:c r="C10" s="34"/>
       <x:c r="D10" s="35"/>
       <x:c r="E10" s="67" t="s">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F10" s="94"/>
     </x:row>
@@ -10256,7 +10268,7 @@
       <x:c r="B11" s="31"/>
       <x:c r="C11" s="34"/>
       <x:c r="D11" s="36" t="s">
-        <x:v>219</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="E11" s="66" t="s">
         <x:v>24</x:v>
@@ -10277,13 +10289,13 @@
       <x:c r="A13" s="62"/>
       <x:c r="B13" s="31"/>
       <x:c r="C13" s="36" t="s">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="D13" s="36" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E13" s="66" t="s">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F13" s="94"/>
     </x:row>
@@ -10303,7 +10315,7 @@
       <x:c r="C15" s="34"/>
       <x:c r="D15" s="34"/>
       <x:c r="E15" s="64" t="s">
-        <x:v>177</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F15" s="94"/>
     </x:row>
@@ -10322,7 +10334,7 @@
       <x:c r="B17" s="31"/>
       <x:c r="C17" s="34"/>
       <x:c r="D17" s="36" t="s">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="E17" s="66" t="s">
         <x:v>4</x:v>
@@ -10335,7 +10347,7 @@
       <x:c r="C18" s="35"/>
       <x:c r="D18" s="35"/>
       <x:c r="E18" s="65" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F18" s="94"/>
     </x:row>
@@ -10343,13 +10355,13 @@
       <x:c r="A19" s="62"/>
       <x:c r="B19" s="31"/>
       <x:c r="C19" s="36" t="s">
-        <x:v>214</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D19" s="36" t="s">
-        <x:v>238</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="E19" s="66" t="s">
-        <x:v>239</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="F19" s="94"/>
     </x:row>
@@ -10359,7 +10371,7 @@
       <x:c r="C20" s="34"/>
       <x:c r="D20" s="35"/>
       <x:c r="E20" s="67" t="s">
-        <x:v>230</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F20" s="94"/>
     </x:row>
@@ -10368,10 +10380,10 @@
       <x:c r="B21" s="31"/>
       <x:c r="C21" s="34"/>
       <x:c r="D21" s="36" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E21" s="66" t="s">
-        <x:v>223</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F21" s="94"/>
     </x:row>
@@ -10390,7 +10402,7 @@
       <x:c r="B23" s="31"/>
       <x:c r="C23" s="34"/>
       <x:c r="D23" s="47" t="s">
-        <x:v>205</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="E23" s="68" t="s">
         <x:v>27</x:v>
@@ -10402,10 +10414,10 @@
       <x:c r="B24" s="31"/>
       <x:c r="C24" s="34"/>
       <x:c r="D24" s="36" t="s">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="E24" s="66" t="s">
-        <x:v>212</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F24" s="94"/>
     </x:row>
@@ -10435,7 +10447,7 @@
       <x:c r="C27" s="70"/>
       <x:c r="D27" s="70"/>
       <x:c r="E27" s="71" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F27" s="95"/>
     </x:row>
@@ -10445,13 +10457,13 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="C28" s="96" t="s">
-        <x:v>228</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="D28" s="96" t="s">
-        <x:v>231</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="E28" s="97" t="s">
-        <x:v>237</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F28" s="93"/>
     </x:row>
@@ -10459,10 +10471,10 @@
       <x:c r="A29" s="62"/>
       <x:c r="B29" s="31"/>
       <x:c r="C29" s="36" t="s">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="D29" s="47" t="s">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="E29" s="68" t="s">
         <x:v>25</x:v>
@@ -10474,10 +10486,10 @@
       <x:c r="B30" s="31"/>
       <x:c r="C30" s="34"/>
       <x:c r="D30" s="36" t="s">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="E30" s="66" t="s">
-        <x:v>199</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F30" s="94"/>
     </x:row>
@@ -10507,19 +10519,19 @@
       <x:c r="C33" s="70"/>
       <x:c r="D33" s="70"/>
       <x:c r="E33" s="71" t="s">
-        <x:v>227</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F33" s="95"/>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="62"/>
       <x:c r="B34" s="31" t="s">
-        <x:v>208</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="C34" s="34"/>
       <x:c r="D34" s="34"/>
       <x:c r="E34" s="64" t="s">
-        <x:v>236</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F34" s="94"/>
     </x:row>
@@ -10529,7 +10541,7 @@
       <x:c r="C35" s="70"/>
       <x:c r="D35" s="70"/>
       <x:c r="E35" s="71" t="s">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F35" s="95"/>
     </x:row>

</xml_diff>

<commit_message>
add 0712 comment, 0713 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8568"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8568" activeTab="2"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Datebook" sheetId="1" r:id="rId4"/>
@@ -718,122 +718,123 @@
     <x:t>봄</x:t>
   </x:si>
   <x:si>
+    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어샵</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>편집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>달력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오늘 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수익적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALL*</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 기본 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고장사례(리콜사례)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상황별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보안성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>겨울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>무결성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오너들의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가을</x:t>
+  </x:si>
+  <x:si>
+    <x:t>여름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>장마철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록 및 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>함수의 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공식 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폭설철</x:t>
+  </x:si>
+  <x:si>
     <x:t>1. 플로우 차트 작성
-2. 설계 계획서 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어샵</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>편집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>달력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오늘 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수익적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALL*</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 기본 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고장사례(리콜사례)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상황별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보안성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>겨울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>무결성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오너들의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가을</x:t>
-  </x:si>
-  <x:si>
-    <x:t>여름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>장마철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록 및 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>함수의 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공식 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폭설철</x:t>
+2. 설계 계획서 작성
+3. Menu_Tree 도식화 수정</x:t>
   </x:si>
   <x:si>
     <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
@@ -2875,7 +2876,7 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="B2:E42"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <x:sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="2" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
       <x:selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18:D18"/>
     </x:sheetView>
@@ -3101,13 +3102,13 @@
         <x:v>60</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="2:5" ht="26.350000000000001">
+    <x:row r="17" spans="2:5" ht="39.549999999999997">
       <x:c r="B17" s="12">
         <x:v>44389</x:v>
       </x:c>
       <x:c r="C17" s="9"/>
       <x:c r="D17" s="11" t="s">
-        <x:v>199</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="E17" s="10"/>
     </x:row>
@@ -3527,7 +3528,7 @@
       <x:c r="D12" s="34"/>
       <x:c r="E12" s="34"/>
       <x:c r="F12" s="47" t="s">
-        <x:v>205</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="G12" s="47"/>
       <x:c r="H12" s="47"/>
@@ -4071,7 +4072,7 @@
         <x:v>147</x:v>
       </x:c>
       <x:c r="E27" s="47" t="s">
-        <x:v>209</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="F27" s="47" t="s">
         <x:v>49</x:v>
@@ -4164,7 +4165,7 @@
       <x:c r="C28" s="34"/>
       <x:c r="D28" s="35"/>
       <x:c r="E28" s="47" t="s">
-        <x:v>228</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F28" s="47" t="s">
         <x:v>49</x:v>
@@ -4536,7 +4537,7 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="E32" s="47" t="s">
-        <x:v>202</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F32" s="47"/>
       <x:c r="G32" s="47"/>
@@ -4719,7 +4720,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="D34" s="47" t="s">
-        <x:v>231</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="E34" s="47"/>
       <x:c r="F34" s="47"/>
@@ -4810,7 +4811,7 @@
       <x:c r="B35" s="31"/>
       <x:c r="C35" s="34"/>
       <x:c r="D35" s="47" t="s">
-        <x:v>204</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="E35" s="47"/>
       <x:c r="F35" s="47"/>
@@ -4901,7 +4902,7 @@
       <x:c r="B36" s="31"/>
       <x:c r="C36" s="34"/>
       <x:c r="D36" s="47" t="s">
-        <x:v>206</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="E36" s="47"/>
       <x:c r="F36" s="47"/>
@@ -5083,7 +5084,7 @@
       <x:c r="B38" s="31"/>
       <x:c r="C38" s="34"/>
       <x:c r="D38" s="47" t="s">
-        <x:v>203</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="E38" s="47"/>
       <x:c r="F38" s="47"/>
@@ -9309,9 +9310,9 @@
   <x:sheetPr codeName="Sheet3"/>
   <x:dimension ref="A1:H60"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="F35" activeCellId="0" sqref="F35:F35"/>
+      <x:selection pane="bottomLeft" activeCell="F21" activeCellId="0" sqref="F21:F21"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
@@ -9365,7 +9366,7 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="E2" s="80" t="s">
-        <x:v>212</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="F2" s="80"/>
       <x:c r="G2" s="80"/>
@@ -9409,7 +9410,7 @@
         <x:v>108</x:v>
       </x:c>
       <x:c r="E5" s="85" t="s">
-        <x:v>226</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F5" s="82"/>
       <x:c r="G5" s="82"/>
@@ -9435,7 +9436,7 @@
       <x:c r="A7" s="39"/>
       <x:c r="B7" s="31"/>
       <x:c r="C7" s="53" t="s">
-        <x:v>220</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="D7" s="84" t="s">
         <x:v>31</x:v>
@@ -9456,7 +9457,7 @@
       <x:c r="D8" s="81"/>
       <x:c r="E8" s="81"/>
       <x:c r="F8" s="82" t="s">
-        <x:v>213</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="G8" s="82"/>
       <x:c r="H8" s="82"/>
@@ -9503,7 +9504,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C12" s="75" t="s">
-        <x:v>227</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="D12" s="80" t="s">
         <x:v>147</x:v>
@@ -9576,7 +9577,7 @@
       <x:c r="B17" s="31"/>
       <x:c r="C17" s="54"/>
       <x:c r="D17" s="82" t="s">
-        <x:v>207</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="E17" s="83"/>
       <x:c r="F17" s="82" t="s">
@@ -9602,7 +9603,7 @@
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="39"/>
       <x:c r="B19" s="31" t="s">
-        <x:v>234</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="C19" s="75" t="s">
         <x:v>151</x:v>
@@ -9670,10 +9671,10 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="D24" s="84" t="s">
-        <x:v>215</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="E24" s="82" t="s">
-        <x:v>224</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F24" s="82"/>
       <x:c r="G24" s="82"/>
@@ -9685,7 +9686,7 @@
       <x:c r="C25" s="75"/>
       <x:c r="D25" s="83"/>
       <x:c r="E25" s="82" t="s">
-        <x:v>237</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F25" s="82"/>
       <x:c r="G25" s="82"/>
@@ -9711,7 +9712,7 @@
       <x:c r="C27" s="75"/>
       <x:c r="D27" s="81"/>
       <x:c r="E27" s="82" t="s">
-        <x:v>223</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="F27" s="82"/>
       <x:c r="G27" s="82"/>
@@ -9723,7 +9724,7 @@
       <x:c r="C28" s="75"/>
       <x:c r="D28" s="81"/>
       <x:c r="E28" s="82" t="s">
-        <x:v>222</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F28" s="82"/>
       <x:c r="G28" s="82"/>
@@ -9735,7 +9736,7 @@
       <x:c r="C29" s="87"/>
       <x:c r="D29" s="88"/>
       <x:c r="E29" s="89" t="s">
-        <x:v>218</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F29" s="89"/>
       <x:c r="G29" s="89"/>
@@ -9797,7 +9798,7 @@
         <x:v>194</x:v>
       </x:c>
       <x:c r="C34" s="91" t="s">
-        <x:v>235</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="D34" s="80"/>
       <x:c r="E34" s="80"/>
@@ -10178,13 +10179,13 @@
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="62"/>
       <x:c r="B3" s="30" t="s">
-        <x:v>236</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="C3" s="33" t="s">
         <x:v>191</x:v>
       </x:c>
       <x:c r="D3" s="33" t="s">
-        <x:v>208</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="E3" s="63" t="s">
         <x:v>57</x:v>
@@ -10197,7 +10198,7 @@
       <x:c r="C4" s="34"/>
       <x:c r="D4" s="34"/>
       <x:c r="E4" s="64" t="s">
-        <x:v>200</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F4" s="94"/>
     </x:row>
@@ -10268,7 +10269,7 @@
       <x:c r="B11" s="31"/>
       <x:c r="C11" s="34"/>
       <x:c r="D11" s="36" t="s">
-        <x:v>221</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="E11" s="66" t="s">
         <x:v>24</x:v>
@@ -10355,7 +10356,7 @@
       <x:c r="A19" s="62"/>
       <x:c r="B19" s="31"/>
       <x:c r="C19" s="36" t="s">
-        <x:v>216</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="D19" s="36" t="s">
         <x:v>240</x:v>
@@ -10371,7 +10372,7 @@
       <x:c r="C20" s="34"/>
       <x:c r="D20" s="35"/>
       <x:c r="E20" s="67" t="s">
-        <x:v>232</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="F20" s="94"/>
     </x:row>
@@ -10383,7 +10384,7 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="E21" s="66" t="s">
-        <x:v>225</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="F21" s="94"/>
     </x:row>
@@ -10402,7 +10403,7 @@
       <x:c r="B23" s="31"/>
       <x:c r="C23" s="34"/>
       <x:c r="D23" s="47" t="s">
-        <x:v>207</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="E23" s="68" t="s">
         <x:v>27</x:v>
@@ -10417,7 +10418,7 @@
         <x:v>176</x:v>
       </x:c>
       <x:c r="E24" s="66" t="s">
-        <x:v>214</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="F24" s="94"/>
     </x:row>
@@ -10457,10 +10458,10 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="C28" s="96" t="s">
-        <x:v>230</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="D28" s="96" t="s">
-        <x:v>233</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="E28" s="97" t="s">
         <x:v>239</x:v>
@@ -10471,10 +10472,10 @@
       <x:c r="A29" s="62"/>
       <x:c r="B29" s="31"/>
       <x:c r="C29" s="36" t="s">
-        <x:v>211</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="D29" s="47" t="s">
-        <x:v>217</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="E29" s="68" t="s">
         <x:v>25</x:v>
@@ -10486,10 +10487,10 @@
       <x:c r="B30" s="31"/>
       <x:c r="C30" s="34"/>
       <x:c r="D30" s="36" t="s">
-        <x:v>219</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="E30" s="66" t="s">
-        <x:v>201</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F30" s="94"/>
     </x:row>
@@ -10519,14 +10520,14 @@
       <x:c r="C33" s="70"/>
       <x:c r="D33" s="70"/>
       <x:c r="E33" s="71" t="s">
-        <x:v>229</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F33" s="95"/>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="62"/>
       <x:c r="B34" s="31" t="s">
-        <x:v>210</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="C34" s="34"/>
       <x:c r="D34" s="34"/>

</xml_diff>

<commit_message>
add 0714 comment, 0715 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8568"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="10956" windowHeight="8568"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Datebook" sheetId="1" r:id="rId4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="248">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="249">
   <x:si>
     <x:t>1. 요구사항 분석 (실현성 확인)
 2. 데이터 흐름도 수정
@@ -33,30 +33,37 @@
  -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 필요 자료 추가 조사
-2. 한계점 및 필요기술 추가
- - 차량 블루투스와 어플 연결 어떻게?
- - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리에 메모한 사항 달력에 날짜 표시</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1-1. Datebook Comment 부분 요약
-1-2. GIT 보고서 다시 작성
-1-3. PPT 머릿글 요약 작성
-1-4. 파일명 수정
-1-5 최종 아이디어 선정 이유 작성
-2. 요구사항 수집 및 분석</x:t>
+    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
+2. 블루투스 관련 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 현장실습 OT
+ - 기업 소개 및 업무 설명
+ - 앞으로 수행하게 될 프로젝트 설명
+2. 기존에 진행했던 캡스톤프로젝트 첨언
+3. 제품 개발 과정 설명
+ - 제품 기획 
+ - 개발 기획  
+ - 개발 설계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사
+2. 요구사항 추가 조사
+3. 경쟁 어플 기능 비교 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
   </x:si>
   <x:si>
     <x:t>1. Git 목록 삭제
@@ -64,20 +71,11 @@
 3. 인터페이스 구상도 작성</x:t>
   </x:si>
   <x:si>
-    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 추가 자료조사(관련 코드)
 2. FlowChart 수정 및 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -91,10 +89,25 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>1. (2-2) 수익적 요소 추가
-2. (4-1) 기능정의 추가
-3. 추가 자료 조사
- - 비슷한 어플(마이클) 화면 구성 조사</x:t>
+    <x:t>1. 필요 자료 추가 조사
+2. 한계점 및 필요기술 추가
+ - 차량 블루투스와 어플 연결 어떻게?
+ - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1-1. Datebook Comment 부분 요약
+1-2. GIT 보고서 다시 작성
+1-3. PPT 머릿글 요약 작성
+1-4. 파일명 수정
+1-5 최종 아이디어 선정 이유 작성
+2. 요구사항 수집 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
   </x:si>
   <x:si>
     <x:t>1. 아이디어 도출
@@ -111,92 +124,25 @@
 블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
   </x:si>
   <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성 완료
-2. 요구사항 정의 및 분류
- - 기능적 요구사항
- - 비기능적 요구사항</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 앱 화면별 Sequence 작성
-2. 앱 화면별 어떻게 구성할 것인지 구상
-3. 추가 자료조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 별 남은 수명 보여줌</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차종, 차번호, 연식 등</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 무료 판매 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 찾아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소 포인트 적립 연동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>방문 정비소 기록, 메모</x:t>
-  </x:si>
-  <x:si>
-    <x:t>항목 및 정비 주기 추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검 스케쥴 및 일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이달의 정비/세차 혜택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험료 확인 및 갱신일 알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기아 커넥티드카 연동하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
+    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
+2. 요구사항 추가 및 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 플로우 차트 작성
+2. 설계 계획서 작성
+3. Menu_Tree 도식화 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
   </x:si>
   <x:si>
     <x:t>1. 07.02 회의록 작성
@@ -213,6 +159,599 @@
 5. vi사용법 설명</x:t>
   </x:si>
   <x:si>
+    <x:t>1. 앱 화면별 Sequence 작성
+2. 앱 화면별 어떻게 구성할 것인지 구상
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
+2. 추가 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성 완료
+2. 요구사항 정의 및 분류
+ - 기능적 요구사항
+ - 비기능적 요구사항</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
+로그인 버튼이 나와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
+비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검내역서(정비소 제공 문서)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리별 check list</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보(오너들의 평균 정보)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. (2-2) 수익적 요소 추가
+2. (4-1) 기능정의 추가
+3. 추가 자료 조사
+ - 비슷한 어플(마이클) 화면 구성 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 기본 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고장사례(리콜사례)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자주 하는 질문</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 판매견적 받기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 형태로 존재</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유사 모델 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 교체 예상 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 정보 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:40
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 추천 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:22
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>진행 방향 ---&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스 (메뉴)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 장착점 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소 지도 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약/견적 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험료 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰 보유 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인 쿠폰 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>데이터 연동 설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 선호도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>친구 초대 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필요 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 시기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차 정보 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균 연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 후기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연비 랭킹</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험사 선택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모두의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메모 입력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 시세</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결함/리콜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>엔진오일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>첫예약할인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카카오톡 문의</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>setting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용 가이드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨 필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>디테일링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어샵</x:t>
+  </x:si>
+  <x:si>
+    <x:t>글 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수리견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tips</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 방문 장소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공유게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 메뉴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>경기/인천</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>견적 요청</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고객상담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연차, 보험료</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 검사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>최신 글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록 및 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자차 게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>함수의 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALL*</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오늘 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>더 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오너들의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Menu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공식 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수익적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 주변 검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
+  </x:si>
+  <x:si>
+    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q&amp;A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>장마철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>여름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>만족도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상황별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클</x:t>
+  </x:si>
+  <x:si>
+    <x:t>검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가을</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평점</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보안성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>편집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>겨울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>무결성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>달력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폭설철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>홈</x:t>
+  </x:si>
+  <x:si>
+    <x:t>봄</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인기글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>계절별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>광고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어</x:t>
+  </x:si>
+  <x:si>
     <x:t>로그인</x:t>
   </x:si>
   <x:si>
@@ -225,424 +764,56 @@
     <x:t>최신글</x:t>
   </x:si>
   <x:si>
-    <x:t>타이어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>만족도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>봄</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>달력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상황별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보안성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>홈</x:t>
-  </x:si>
-  <x:si>
-    <x:t>편집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>겨울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>무결성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Q&amp;A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>장마철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폭설철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>채팅창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>여름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가을</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평점</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인기글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>광고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>계절별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 현장실습 OT
- - 기업 소개 및 업무 설명
- - 앞으로 수행하게 될 프로젝트 설명
-2. 기존에 진행했던 캡스톤프로젝트 첨언
-3. 제품 개발 과정 설명
- - 제품 기획 
- - 개발 기획  
- - 개발 설계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리별 check list</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검내역서(정비소 제공 문서)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보(오너들의 평균 정보)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오너들의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록 및 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수익적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>함수의 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALL*</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오늘 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공식 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>더 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Menu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자차 게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 주변 검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연비 랭킹</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차 정보 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모두의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 후기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험사 선택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Home</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필요 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 시기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균 연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>경기/인천</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>디테일링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 시세</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메모 입력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>글 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용 가이드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수리견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>카카오톡 문의</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>엔진오일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 방문 장소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결함/리콜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>첫예약할인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>setting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨 필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어샵</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공유게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 메뉴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연차, 보험료</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>최신 글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고객상담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>견적 요청</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 검사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성
+    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 계약서 작성
+2. 현장실습 오리엔테이션</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 보완
+2. 기능정의 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Menu_Tree 수정(완료)
 2. 추가 자료 조사</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
-2. 요구사항 추가 및 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 플로우 차트 작성
-2. 설계 계획서 작성
-3. Menu_Tree 도식화 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 추가 자료조사
-2. 요구사항 추가 조사
-3. 경쟁 어플 기능 비교 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
+    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
   </x:si>
   <x:si>
     <x:t>1. 인터페이스 구상도 작성
@@ -650,227 +821,60 @@
 3. 추가 자료조사</x:t>
   </x:si>
   <x:si>
-    <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
-비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 정보 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스 (메뉴)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:40
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 장착점 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:22
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소 지도 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 추천 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>진행 방향 ---&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>데이터 연동 설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험료 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:25
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 선호도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰 보유 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인 쿠폰 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약/견적 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>친구 초대 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유사 모델 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 교체 예상 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 판매견적 받기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자주 하는 질문</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 기본 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고장사례(리콜사례)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Menu_Tree 수정(완료)
+    <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이달의 정비/세차 혜택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기아 커넥티드카 연동하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소 포인트 적립 연동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 무료 판매 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 별 남은 수명 보여줌</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검 스케쥴 및 일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험료 확인 및 갱신일 알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 찾아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차종, 차번호, 연식 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>방문 정비소 기록, 메모</x:t>
+  </x:si>
+  <x:si>
+    <x:t>항목 및 정비 주기 추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리에 메모한 사항 달력에 날짜 표시</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 시퀀스 작성
 2. 추가 자료 조사</x:t>
   </x:si>
   <x:si>
-    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 보완
-2. 기능정의 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
-로그인 버튼이 나와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
-2. 블루투스 관련 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 계약서 작성
-2. 현장실습 오리엔테이션</x:t>
-  </x:si>
-  <x:si>
-    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴 시퀀스 작성
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
+    <x:t>1. 메뉴시퀀스 작성 (미완)
+2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1463,7 +1467,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="100">
+  <x:cellXfs count="101">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -2224,6 +2228,19 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2917,8 +2934,8 @@
   <x:dimension ref="B2:E42"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:pane xSplit="0" ySplit="2" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20:D20"/>
+      <x:pane xSplit="0" ySplit="2" topLeftCell="C15" activePane="bottomLeft" state="frozen"/>
+      <x:selection pane="bottomLeft" activeCell="E20" activeCellId="0" sqref="E20:E20"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -2934,16 +2951,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="5" t="s">
-        <x:v>154</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C2" s="6" t="s">
-        <x:v>120</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D2" s="6" t="s">
-        <x:v>140</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="E2" s="7" t="s">
-        <x:v>142</x:v>
+        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -2951,13 +2968,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="15" t="s">
-        <x:v>207</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D3" s="9" t="s">
-        <x:v>241</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="E3" s="9" t="s">
-        <x:v>90</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -2965,13 +2982,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="14" t="s">
-        <x:v>207</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D4" s="12" t="s">
-        <x:v>95</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E4" s="12" t="s">
-        <x:v>13</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -2979,10 +2996,10 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="16" t="s">
-        <x:v>211</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="D5" s="12" t="s">
-        <x:v>237</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E5" s="12" t="s">
         <x:v>15</x:v>
@@ -2993,13 +3010,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="18" t="s">
-        <x:v>211</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="D6" s="12" t="s">
-        <x:v>6</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E6" s="17" t="s">
-        <x:v>17</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -3007,13 +3024,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="14" t="s">
-        <x:v>189</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D7" s="12" t="s">
-        <x:v>229</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="E7" s="12" t="s">
-        <x:v>43</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -3021,13 +3038,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="14" t="s">
-        <x:v>205</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D8" s="12" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E8" s="12" t="s">
-        <x:v>18</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -3035,13 +3052,13 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="19" t="s">
-        <x:v>196</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D9" s="12" t="s">
-        <x:v>96</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E9" s="12" t="s">
-        <x:v>236</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -3049,13 +3066,13 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="20" t="s">
-        <x:v>203</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D10" s="12" t="s">
-        <x:v>177</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E10" s="12" t="s">
-        <x:v>19</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
@@ -3063,13 +3080,13 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="22" t="s">
-        <x:v>187</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="D11" s="12" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E11" s="12" t="s">
-        <x:v>42</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:5" ht="105.40000000000001">
@@ -3077,10 +3094,10 @@
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="21" t="s">
-        <x:v>201</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="D12" s="12" t="s">
-        <x:v>181</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="E12" s="12" t="s">
         <x:v>0</x:v>
@@ -3091,13 +3108,13 @@
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="23" t="s">
-        <x:v>203</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D13" s="12" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E13" s="12" t="s">
         <x:v>12</x:v>
-      </x:c>
-      <x:c r="E13" s="12" t="s">
-        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5" ht="52.700000000000003">
@@ -3105,13 +3122,13 @@
         <x:v>44384</x:v>
       </x:c>
       <x:c r="C14" s="24" t="s">
-        <x:v>193</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D14" s="12" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E14" s="12" t="s">
-        <x:v>14</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:5" ht="52.700000000000003">
@@ -3119,10 +3136,10 @@
         <x:v>44385</x:v>
       </x:c>
       <x:c r="C15" s="30" t="s">
-        <x:v>212</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D15" s="12" t="s">
-        <x:v>178</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
         <x:v>16</x:v>
@@ -3133,13 +3150,13 @@
         <x:v>44386</x:v>
       </x:c>
       <x:c r="C16" s="31" t="s">
-        <x:v>191</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D16" s="12" t="s">
-        <x:v>230</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="E16" s="12" t="s">
-        <x:v>175</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="2:5" ht="39.549999999999997">
@@ -3147,45 +3164,51 @@
         <x:v>44389</x:v>
       </x:c>
       <x:c r="C17" s="74" t="s">
-        <x:v>226</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D17" s="12" t="s">
-        <x:v>176</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>227</x:v>
+        <x:v>224</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:5" ht="26.350000000000001">
       <x:c r="B18" s="13">
         <x:v>44390</x:v>
       </x:c>
-      <x:c r="C18" s="14" t="s">
-        <x:v>225</x:v>
+      <x:c r="C18" s="100" t="s">
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D18" s="12" t="s">
-        <x:v>244</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="E18" s="12" t="s">
-        <x:v>239</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="2:5" ht="26.350000000000001">
       <x:c r="B19" s="13">
         <x:v>44391</x:v>
       </x:c>
-      <x:c r="C19" s="10"/>
+      <x:c r="C19" s="100" t="s">
+        <x:v>78</x:v>
+      </x:c>
       <x:c r="D19" s="12" t="s">
-        <x:v>174</x:v>
-      </x:c>
-      <x:c r="E19" s="11"/>
-    </x:row>
-    <x:row r="20" spans="2:5">
+        <x:v>247</x:v>
+      </x:c>
+      <x:c r="E19" s="12" t="s">
+        <x:v>248</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="2:5" ht="26.350000000000001">
       <x:c r="B20" s="13">
         <x:v>44392</x:v>
       </x:c>
       <x:c r="C20" s="10"/>
-      <x:c r="D20" s="11"/>
+      <x:c r="D20" s="12" t="s">
+        <x:v>28</x:v>
+      </x:c>
       <x:c r="E20" s="11"/>
     </x:row>
     <x:row r="21" spans="2:5">
@@ -3392,54 +3415,54 @@
   <x:sheetData>
     <x:row r="1" spans="1:9" ht="17.149999999999999">
       <x:c r="A1" s="26" t="s">
-        <x:v>198</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>108</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
-        <x:v>117</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="D1" s="34" t="s">
-        <x:v>106</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E1" s="34" t="s">
-        <x:v>159</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F1" s="34" t="s">
-        <x:v>125</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>128</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="H1" s="34" t="s">
-        <x:v>88</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="I1" s="35" t="s">
-        <x:v>56</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:9">
       <x:c r="A2" s="83" t="s">
-        <x:v>59</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B2" s="77" t="s">
-        <x:v>69</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C2" s="80" t="s">
-        <x:v>131</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D2" s="80" t="s">
-        <x:v>115</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="E2" s="38" t="s">
-        <x:v>135</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F2" s="38"/>
       <x:c r="G2" s="38"/>
       <x:c r="H2" s="38"/>
       <x:c r="I2" s="38" t="s">
-        <x:v>217</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9">
@@ -3448,13 +3471,13 @@
       <x:c r="C3" s="81"/>
       <x:c r="D3" s="81"/>
       <x:c r="E3" s="37" t="s">
-        <x:v>213</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F3" s="37"/>
       <x:c r="G3" s="37"/>
       <x:c r="H3" s="37"/>
       <x:c r="I3" s="37" t="s">
-        <x:v>30</x:v>
+        <x:v>238</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
@@ -3463,7 +3486,7 @@
       <x:c r="C4" s="81"/>
       <x:c r="D4" s="81"/>
       <x:c r="E4" s="37" t="s">
-        <x:v>136</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F4" s="37"/>
       <x:c r="G4" s="37"/>
@@ -3476,10 +3499,10 @@
       <x:c r="C5" s="81"/>
       <x:c r="D5" s="81"/>
       <x:c r="E5" s="75" t="s">
-        <x:v>148</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F5" s="37" t="s">
-        <x:v>146</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G5" s="37"/>
       <x:c r="H5" s="37"/>
@@ -3492,7 +3515,7 @@
       <x:c r="D6" s="76"/>
       <x:c r="E6" s="76"/>
       <x:c r="F6" s="37" t="s">
-        <x:v>188</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G6" s="37"/>
       <x:c r="H6" s="37"/>
@@ -3503,10 +3526,10 @@
       <x:c r="B7" s="78"/>
       <x:c r="C7" s="81"/>
       <x:c r="D7" s="75" t="s">
-        <x:v>161</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="E7" s="37" t="s">
-        <x:v>66</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="F7" s="37"/>
       <x:c r="G7" s="37"/>
@@ -3519,13 +3542,13 @@
       <x:c r="C8" s="81"/>
       <x:c r="D8" s="81"/>
       <x:c r="E8" s="37" t="s">
-        <x:v>57</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F8" s="37"/>
       <x:c r="G8" s="37"/>
       <x:c r="H8" s="37"/>
       <x:c r="I8" s="37" t="s">
-        <x:v>35</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:9">
@@ -3534,13 +3557,13 @@
       <x:c r="C9" s="81"/>
       <x:c r="D9" s="81"/>
       <x:c r="E9" s="37" t="s">
-        <x:v>50</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F9" s="37"/>
       <x:c r="G9" s="37"/>
       <x:c r="H9" s="37"/>
       <x:c r="I9" s="37" t="s">
-        <x:v>28</x:v>
+        <x:v>237</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
@@ -3549,10 +3572,10 @@
       <x:c r="C10" s="81"/>
       <x:c r="D10" s="81"/>
       <x:c r="E10" s="75" t="s">
-        <x:v>169</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F10" s="37" t="s">
-        <x:v>133</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="G10" s="37"/>
       <x:c r="H10" s="37"/>
@@ -3565,12 +3588,12 @@
       <x:c r="D11" s="81"/>
       <x:c r="E11" s="81"/>
       <x:c r="F11" s="37" t="s">
-        <x:v>139</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="G11" s="37"/>
       <x:c r="H11" s="37"/>
       <x:c r="I11" s="37" t="s">
-        <x:v>233</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
@@ -3580,7 +3603,7 @@
       <x:c r="D12" s="81"/>
       <x:c r="E12" s="81"/>
       <x:c r="F12" s="37" t="s">
-        <x:v>70</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="G12" s="37"/>
       <x:c r="H12" s="37"/>
@@ -3593,12 +3616,12 @@
       <x:c r="D13" s="76"/>
       <x:c r="E13" s="76"/>
       <x:c r="F13" s="37" t="s">
-        <x:v>86</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="G13" s="37"/>
       <x:c r="H13" s="37"/>
       <x:c r="I13" s="37" t="s">
-        <x:v>27</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="J13" s="29"/>
       <x:c r="K13" s="29"/>
@@ -3624,19 +3647,19 @@
       <x:c r="A14" s="84"/>
       <x:c r="B14" s="78"/>
       <x:c r="C14" s="75" t="s">
-        <x:v>116</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="D14" s="75" t="s">
-        <x:v>144</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="E14" s="37" t="s">
-        <x:v>81</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="F14" s="37"/>
       <x:c r="G14" s="37"/>
       <x:c r="H14" s="37"/>
       <x:c r="I14" s="37" t="s">
-        <x:v>52</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="J14" s="29"/>
       <x:c r="K14" s="29"/>
@@ -3664,13 +3687,13 @@
       <x:c r="C15" s="81"/>
       <x:c r="D15" s="81"/>
       <x:c r="E15" s="37" t="s">
-        <x:v>129</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F15" s="37"/>
       <x:c r="G15" s="37"/>
       <x:c r="H15" s="37"/>
       <x:c r="I15" s="37" t="s">
-        <x:v>113</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="J15" s="29"/>
       <x:c r="K15" s="29"/>
@@ -3698,7 +3721,7 @@
       <x:c r="C16" s="81"/>
       <x:c r="D16" s="81"/>
       <x:c r="E16" s="37" t="s">
-        <x:v>118</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F16" s="37"/>
       <x:c r="G16" s="37"/>
@@ -3729,13 +3752,13 @@
       <x:c r="C17" s="81"/>
       <x:c r="D17" s="76"/>
       <x:c r="E17" s="37" t="s">
-        <x:v>147</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F17" s="37"/>
       <x:c r="G17" s="37"/>
       <x:c r="H17" s="37"/>
       <x:c r="I17" s="37" t="s">
-        <x:v>5</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="J17" s="29"/>
       <x:c r="K17" s="29"/>
@@ -3762,13 +3785,13 @@
       <x:c r="B18" s="78"/>
       <x:c r="C18" s="81"/>
       <x:c r="D18" s="37" t="s">
-        <x:v>202</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="E18" s="37" t="s">
-        <x:v>200</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F18" s="37" t="s">
-        <x:v>119</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="G18" s="37"/>
       <x:c r="H18" s="37"/>
@@ -3798,14 +3821,14 @@
       <x:c r="B19" s="78"/>
       <x:c r="C19" s="81"/>
       <x:c r="D19" s="37" t="s">
-        <x:v>46</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="E19" s="37"/>
       <x:c r="F19" s="37"/>
       <x:c r="G19" s="37"/>
       <x:c r="H19" s="37"/>
       <x:c r="I19" s="75" t="s">
-        <x:v>216</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="J19" s="29"/>
       <x:c r="K19" s="29"/>
@@ -3832,7 +3855,7 @@
       <x:c r="B20" s="78"/>
       <x:c r="C20" s="81"/>
       <x:c r="D20" s="37" t="s">
-        <x:v>147</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="E20" s="37"/>
       <x:c r="F20" s="37"/>
@@ -3864,7 +3887,7 @@
       <x:c r="B21" s="78"/>
       <x:c r="C21" s="81"/>
       <x:c r="D21" s="37" t="s">
-        <x:v>118</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="E21" s="37"/>
       <x:c r="F21" s="37"/>
@@ -3896,7 +3919,7 @@
       <x:c r="B22" s="79"/>
       <x:c r="C22" s="76"/>
       <x:c r="D22" s="37" t="s">
-        <x:v>214</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E22" s="37"/>
       <x:c r="F22" s="37"/>
@@ -3926,10 +3949,10 @@
     <x:row r="23" spans="1:28">
       <x:c r="A23" s="84"/>
       <x:c r="B23" s="82" t="s">
-        <x:v>149</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C23" s="37" t="s">
-        <x:v>209</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D23" s="37"/>
       <x:c r="E23" s="37"/>
@@ -3961,7 +3984,7 @@
       <x:c r="A24" s="84"/>
       <x:c r="B24" s="78"/>
       <x:c r="C24" s="37" t="s">
-        <x:v>82</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="D24" s="37"/>
       <x:c r="E24" s="37"/>
@@ -3993,7 +4016,7 @@
       <x:c r="A25" s="84"/>
       <x:c r="B25" s="78"/>
       <x:c r="C25" s="37" t="s">
-        <x:v>68</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D25" s="37"/>
       <x:c r="E25" s="37"/>
@@ -4025,13 +4048,13 @@
       <x:c r="A26" s="84"/>
       <x:c r="B26" s="78"/>
       <x:c r="C26" s="75" t="s">
-        <x:v>149</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="D26" s="37" t="s">
-        <x:v>145</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="E26" s="37" t="s">
-        <x:v>218</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F26" s="37"/>
       <x:c r="G26" s="37"/>
@@ -4121,13 +4144,13 @@
       <x:c r="B27" s="82"/>
       <x:c r="C27" s="81"/>
       <x:c r="D27" s="75" t="s">
-        <x:v>48</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="E27" s="37" t="s">
-        <x:v>104</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F27" s="37" t="s">
-        <x:v>192</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G27" s="37"/>
       <x:c r="H27" s="37"/>
@@ -4217,10 +4240,10 @@
       <x:c r="C28" s="81"/>
       <x:c r="D28" s="76"/>
       <x:c r="E28" s="37" t="s">
-        <x:v>109</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F28" s="37" t="s">
-        <x:v>192</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="G28" s="37"/>
       <x:c r="H28" s="37"/>
@@ -4309,10 +4332,10 @@
       <x:c r="B29" s="78"/>
       <x:c r="C29" s="81"/>
       <x:c r="D29" s="37" t="s">
-        <x:v>141</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="E29" s="39" t="s">
-        <x:v>172</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F29" s="39"/>
       <x:c r="G29" s="37"/>
@@ -4402,10 +4425,10 @@
       <x:c r="B30" s="78"/>
       <x:c r="C30" s="81"/>
       <x:c r="D30" s="37" t="s">
-        <x:v>132</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="E30" s="37" t="s">
-        <x:v>54</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="F30" s="37"/>
       <x:c r="G30" s="37"/>
@@ -4586,10 +4609,10 @@
       <x:c r="B32" s="78"/>
       <x:c r="C32" s="81"/>
       <x:c r="D32" s="37" t="s">
-        <x:v>134</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="E32" s="37" t="s">
-        <x:v>151</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F32" s="37"/>
       <x:c r="G32" s="37"/>
@@ -4679,7 +4702,7 @@
       <x:c r="B33" s="78"/>
       <x:c r="C33" s="76"/>
       <x:c r="D33" s="37" t="s">
-        <x:v>150</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="E33" s="37"/>
       <x:c r="F33" s="37"/>
@@ -4769,10 +4792,10 @@
       <x:c r="A34" s="83"/>
       <x:c r="B34" s="82"/>
       <x:c r="C34" s="75" t="s">
-        <x:v>111</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="D34" s="37" t="s">
-        <x:v>105</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="E34" s="37"/>
       <x:c r="F34" s="37"/>
@@ -4863,7 +4886,7 @@
       <x:c r="B35" s="78"/>
       <x:c r="C35" s="81"/>
       <x:c r="D35" s="37" t="s">
-        <x:v>53</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="E35" s="37"/>
       <x:c r="F35" s="37"/>
@@ -4954,7 +4977,7 @@
       <x:c r="B36" s="78"/>
       <x:c r="C36" s="81"/>
       <x:c r="D36" s="37" t="s">
-        <x:v>60</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="E36" s="37"/>
       <x:c r="F36" s="37"/>
@@ -5045,7 +5068,7 @@
       <x:c r="B37" s="78"/>
       <x:c r="C37" s="81"/>
       <x:c r="D37" s="37" t="s">
-        <x:v>45</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="E37" s="37"/>
       <x:c r="F37" s="37"/>
@@ -5136,7 +5159,7 @@
       <x:c r="B38" s="78"/>
       <x:c r="C38" s="81"/>
       <x:c r="D38" s="37" t="s">
-        <x:v>157</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="E38" s="37"/>
       <x:c r="F38" s="37"/>
@@ -5227,7 +5250,7 @@
       <x:c r="B39" s="82"/>
       <x:c r="C39" s="76"/>
       <x:c r="D39" s="37" t="s">
-        <x:v>173</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="E39" s="37"/>
       <x:c r="F39" s="37"/>
@@ -5316,10 +5339,10 @@
     <x:row r="40" spans="1:87">
       <x:c r="A40" s="84"/>
       <x:c r="B40" s="82" t="s">
-        <x:v>89</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="C40" s="37" t="s">
-        <x:v>83</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="D40" s="37"/>
       <x:c r="E40" s="37"/>
@@ -5410,7 +5433,7 @@
       <x:c r="A41" s="84"/>
       <x:c r="B41" s="78"/>
       <x:c r="C41" s="37" t="s">
-        <x:v>168</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D41" s="37"/>
       <x:c r="E41" s="37"/>
@@ -5501,7 +5524,7 @@
       <x:c r="A42" s="84"/>
       <x:c r="B42" s="78"/>
       <x:c r="C42" s="37" t="s">
-        <x:v>110</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D42" s="37"/>
       <x:c r="E42" s="37"/>
@@ -5592,7 +5615,7 @@
       <x:c r="A43" s="84"/>
       <x:c r="B43" s="78"/>
       <x:c r="C43" s="37" t="s">
-        <x:v>155</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="D43" s="37"/>
       <x:c r="E43" s="37"/>
@@ -5683,7 +5706,7 @@
       <x:c r="A44" s="84"/>
       <x:c r="B44" s="78"/>
       <x:c r="C44" s="37" t="s">
-        <x:v>68</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D44" s="37"/>
       <x:c r="E44" s="37"/>
@@ -5774,7 +5797,7 @@
       <x:c r="A45" s="84"/>
       <x:c r="B45" s="79"/>
       <x:c r="C45" s="37" t="s">
-        <x:v>137</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="D45" s="37"/>
       <x:c r="E45" s="37"/>
@@ -5864,10 +5887,10 @@
     <x:row r="46" spans="1:87">
       <x:c r="A46" s="84"/>
       <x:c r="B46" s="82" t="s">
-        <x:v>55</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C46" s="37" t="s">
-        <x:v>84</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="D46" s="37"/>
       <x:c r="E46" s="37"/>
@@ -5958,7 +5981,7 @@
       <x:c r="A47" s="84"/>
       <x:c r="B47" s="78"/>
       <x:c r="C47" s="37" t="s">
-        <x:v>64</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="D47" s="37"/>
       <x:c r="E47" s="37"/>
@@ -6049,7 +6072,7 @@
       <x:c r="A48" s="84"/>
       <x:c r="B48" s="78"/>
       <x:c r="C48" s="37" t="s">
-        <x:v>127</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="D48" s="37"/>
       <x:c r="E48" s="37"/>
@@ -6140,7 +6163,7 @@
       <x:c r="A49" s="84"/>
       <x:c r="B49" s="79"/>
       <x:c r="C49" s="37" t="s">
-        <x:v>158</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="D49" s="37"/>
       <x:c r="E49" s="37"/>
@@ -6230,13 +6253,13 @@
     <x:row r="50" spans="1:87">
       <x:c r="A50" s="84"/>
       <x:c r="B50" s="82" t="s">
-        <x:v>107</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C50" s="75" t="s">
-        <x:v>209</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D50" s="37" t="s">
-        <x:v>167</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E50" s="37"/>
       <x:c r="F50" s="37"/>
@@ -6327,7 +6350,7 @@
       <x:c r="B51" s="78"/>
       <x:c r="C51" s="76"/>
       <x:c r="D51" s="37" t="s">
-        <x:v>143</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="E51" s="37"/>
       <x:c r="F51" s="37"/>
@@ -6417,10 +6440,10 @@
       <x:c r="A52" s="84"/>
       <x:c r="B52" s="78"/>
       <x:c r="C52" s="75" t="s">
-        <x:v>51</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="D52" s="37" t="s">
-        <x:v>206</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="E52" s="37"/>
       <x:c r="F52" s="37"/>
@@ -6511,7 +6534,7 @@
       <x:c r="B53" s="78"/>
       <x:c r="C53" s="76"/>
       <x:c r="D53" s="37" t="s">
-        <x:v>204</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E53" s="37"/>
       <x:c r="F53" s="37"/>
@@ -6601,10 +6624,10 @@
       <x:c r="A54" s="84"/>
       <x:c r="B54" s="78"/>
       <x:c r="C54" s="75" t="s">
-        <x:v>197</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D54" s="37" t="s">
-        <x:v>208</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E54" s="37"/>
       <x:c r="F54" s="37"/>
@@ -6695,7 +6718,7 @@
       <x:c r="B55" s="78"/>
       <x:c r="C55" s="81"/>
       <x:c r="D55" s="37" t="s">
-        <x:v>194</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E55" s="37"/>
       <x:c r="F55" s="37"/>
@@ -6786,7 +6809,7 @@
       <x:c r="B56" s="78"/>
       <x:c r="C56" s="76"/>
       <x:c r="D56" s="37" t="s">
-        <x:v>23</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="E56" s="37"/>
       <x:c r="F56" s="37"/>
@@ -6876,10 +6899,10 @@
       <x:c r="A57" s="84"/>
       <x:c r="B57" s="78"/>
       <x:c r="C57" s="75" t="s">
-        <x:v>165</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D57" s="37" t="s">
-        <x:v>29</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="E57" s="37"/>
       <x:c r="F57" s="37"/>
@@ -6970,7 +6993,7 @@
       <x:c r="B58" s="78"/>
       <x:c r="C58" s="76"/>
       <x:c r="D58" s="37" t="s">
-        <x:v>210</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="E58" s="37"/>
       <x:c r="F58" s="37"/>
@@ -7060,10 +7083,10 @@
       <x:c r="A59" s="84"/>
       <x:c r="B59" s="78"/>
       <x:c r="C59" s="75" t="s">
-        <x:v>199</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D59" s="37" t="s">
-        <x:v>31</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="E59" s="37"/>
       <x:c r="F59" s="37"/>
@@ -7154,7 +7177,7 @@
       <x:c r="B60" s="78"/>
       <x:c r="C60" s="76"/>
       <x:c r="D60" s="37" t="s">
-        <x:v>25</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="E60" s="37"/>
       <x:c r="F60" s="37"/>
@@ -7244,10 +7267,10 @@
       <x:c r="A61" s="84"/>
       <x:c r="B61" s="78"/>
       <x:c r="C61" s="75" t="s">
-        <x:v>138</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="D61" s="37" t="s">
-        <x:v>74</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="E61" s="37"/>
       <x:c r="F61" s="37"/>
@@ -7338,7 +7361,7 @@
       <x:c r="B62" s="79"/>
       <x:c r="C62" s="76"/>
       <x:c r="D62" s="37" t="s">
-        <x:v>170</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="E62" s="37"/>
       <x:c r="F62" s="37"/>
@@ -9364,7 +9387,7 @@
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="H23" activeCellId="0" sqref="H23:H23"/>
+      <x:selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31:D31"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
@@ -9380,50 +9403,50 @@
   <x:sheetData>
     <x:row r="1" spans="1:8" ht="17.149999999999999">
       <x:c r="A1" s="32" t="s">
-        <x:v>198</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>108</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
-        <x:v>117</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="D1" s="34" t="s">
-        <x:v>106</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E1" s="34" t="s">
-        <x:v>159</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F1" s="34" t="s">
-        <x:v>125</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>88</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="H1" s="35" t="s">
-        <x:v>67</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8" ht="16.75" customHeight="1">
       <x:c r="A2" s="83" t="s">
-        <x:v>114</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B2" s="77" t="s">
-        <x:v>121</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C2" s="90" t="s">
-        <x:v>131</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D2" s="88" t="s">
-        <x:v>144</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="E2" s="61" t="s">
-        <x:v>222</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F2" s="61"/>
       <x:c r="G2" s="61"/>
       <x:c r="H2" s="61" t="s">
-        <x:v>22</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -9432,12 +9455,12 @@
       <x:c r="C3" s="91"/>
       <x:c r="D3" s="89"/>
       <x:c r="E3" s="62" t="s">
-        <x:v>162</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="F3" s="62"/>
       <x:c r="G3" s="62"/>
       <x:c r="H3" s="62" t="s">
-        <x:v>166</x:v>
+        <x:v>136</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -9446,12 +9469,12 @@
       <x:c r="C4" s="91"/>
       <x:c r="D4" s="87"/>
       <x:c r="E4" s="62" t="s">
-        <x:v>148</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F4" s="62"/>
       <x:c r="G4" s="62"/>
       <x:c r="H4" s="62" t="s">
-        <x:v>26</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -9459,15 +9482,15 @@
       <x:c r="B5" s="78"/>
       <x:c r="C5" s="91"/>
       <x:c r="D5" s="86" t="s">
-        <x:v>161</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="E5" s="63" t="s">
-        <x:v>98</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F5" s="62"/>
       <x:c r="G5" s="62"/>
       <x:c r="H5" s="62" t="s">
-        <x:v>243</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -9476,28 +9499,28 @@
       <x:c r="C6" s="92"/>
       <x:c r="D6" s="87"/>
       <x:c r="E6" s="63" t="s">
-        <x:v>50</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F6" s="62"/>
       <x:c r="G6" s="62"/>
       <x:c r="H6" s="62" t="s">
-        <x:v>93</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="84"/>
       <x:c r="B7" s="78"/>
       <x:c r="C7" s="94" t="s">
-        <x:v>97</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="D7" s="86" t="s">
-        <x:v>94</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E7" s="86" t="s">
-        <x:v>144</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F7" s="62" t="s">
-        <x:v>81</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="G7" s="62"/>
       <x:c r="H7" s="62"/>
@@ -9509,7 +9532,7 @@
       <x:c r="D8" s="89"/>
       <x:c r="E8" s="89"/>
       <x:c r="F8" s="62" t="s">
-        <x:v>223</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G8" s="62"/>
       <x:c r="H8" s="62"/>
@@ -9521,7 +9544,7 @@
       <x:c r="D9" s="89"/>
       <x:c r="E9" s="89"/>
       <x:c r="F9" s="62" t="s">
-        <x:v>171</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G9" s="62"/>
       <x:c r="H9" s="62"/>
@@ -9533,7 +9556,7 @@
       <x:c r="D10" s="89"/>
       <x:c r="E10" s="89"/>
       <x:c r="F10" s="62" t="s">
-        <x:v>46</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="G10" s="62"/>
       <x:c r="H10" s="62"/>
@@ -9545,7 +9568,7 @@
       <x:c r="D11" s="93"/>
       <x:c r="E11" s="93"/>
       <x:c r="F11" s="65" t="s">
-        <x:v>160</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G11" s="65"/>
       <x:c r="H11" s="65"/>
@@ -9553,16 +9576,16 @@
     <x:row r="12" spans="1:8">
       <x:c r="A12" s="84"/>
       <x:c r="B12" s="78" t="s">
-        <x:v>87</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="C12" s="91" t="s">
-        <x:v>102</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D12" s="61" t="s">
-        <x:v>48</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="E12" s="89" t="s">
-        <x:v>24</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F12" s="61"/>
       <x:c r="G12" s="61"/>
@@ -9573,7 +9596,7 @@
       <x:c r="B13" s="78"/>
       <x:c r="C13" s="91"/>
       <x:c r="D13" s="63" t="s">
-        <x:v>145</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="E13" s="89"/>
       <x:c r="F13" s="62"/>
@@ -9585,7 +9608,7 @@
       <x:c r="B14" s="78"/>
       <x:c r="C14" s="91"/>
       <x:c r="D14" s="63" t="s">
-        <x:v>156</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="E14" s="89"/>
       <x:c r="F14" s="62"/>
@@ -9597,7 +9620,7 @@
       <x:c r="B15" s="78"/>
       <x:c r="C15" s="92"/>
       <x:c r="D15" s="63" t="s">
-        <x:v>173</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="E15" s="87"/>
       <x:c r="F15" s="62"/>
@@ -9608,20 +9631,20 @@
       <x:c r="A16" s="84"/>
       <x:c r="B16" s="78"/>
       <x:c r="C16" s="94" t="s">
-        <x:v>122</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="D16" s="63" t="s">
-        <x:v>112</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="E16" s="86" t="s">
-        <x:v>209</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F16" s="62" t="s">
-        <x:v>167</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="G16" s="62"/>
       <x:c r="H16" s="86" t="s">
-        <x:v>4</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -9629,11 +9652,11 @@
       <x:c r="B17" s="78"/>
       <x:c r="C17" s="92"/>
       <x:c r="D17" s="62" t="s">
-        <x:v>61</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="E17" s="87"/>
       <x:c r="F17" s="62" t="s">
-        <x:v>143</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="G17" s="62"/>
       <x:c r="H17" s="87"/>
@@ -9642,26 +9665,26 @@
       <x:c r="A18" s="84"/>
       <x:c r="B18" s="95"/>
       <x:c r="C18" s="66" t="s">
-        <x:v>123</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D18" s="65"/>
       <x:c r="E18" s="65"/>
       <x:c r="F18" s="65"/>
       <x:c r="G18" s="65"/>
       <x:c r="H18" s="65" t="s">
-        <x:v>21</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="84"/>
       <x:c r="B19" s="78" t="s">
-        <x:v>221</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C19" s="91" t="s">
-        <x:v>89</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="D19" s="61" t="s">
-        <x:v>83</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="E19" s="61"/>
       <x:c r="F19" s="61"/>
@@ -9673,7 +9696,7 @@
       <x:c r="B20" s="78"/>
       <x:c r="C20" s="91"/>
       <x:c r="D20" s="62" t="s">
-        <x:v>47</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="E20" s="62"/>
       <x:c r="F20" s="62"/>
@@ -9685,7 +9708,7 @@
       <x:c r="B21" s="78"/>
       <x:c r="C21" s="91"/>
       <x:c r="D21" s="62" t="s">
-        <x:v>110</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="E21" s="62"/>
       <x:c r="F21" s="62"/>
@@ -9697,7 +9720,7 @@
       <x:c r="B22" s="78"/>
       <x:c r="C22" s="91"/>
       <x:c r="D22" s="62" t="s">
-        <x:v>68</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="E22" s="62"/>
       <x:c r="F22" s="62"/>
@@ -9709,7 +9732,7 @@
       <x:c r="B23" s="78"/>
       <x:c r="C23" s="92"/>
       <x:c r="D23" s="62" t="s">
-        <x:v>137</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="E23" s="62"/>
       <x:c r="F23" s="62"/>
@@ -9720,13 +9743,13 @@
       <x:c r="A24" s="83"/>
       <x:c r="B24" s="82"/>
       <x:c r="C24" s="94" t="s">
-        <x:v>155</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="D24" s="86" t="s">
-        <x:v>62</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="E24" s="62" t="s">
-        <x:v>76</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F24" s="62"/>
       <x:c r="G24" s="62"/>
@@ -9738,7 +9761,7 @@
       <x:c r="C25" s="91"/>
       <x:c r="D25" s="87"/>
       <x:c r="E25" s="62" t="s">
-        <x:v>77</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F25" s="62"/>
       <x:c r="G25" s="62"/>
@@ -9749,10 +9772,10 @@
       <x:c r="B26" s="82"/>
       <x:c r="C26" s="91"/>
       <x:c r="D26" s="86" t="s">
-        <x:v>85</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="E26" s="62" t="s">
-        <x:v>58</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F26" s="62"/>
       <x:c r="G26" s="62"/>
@@ -9764,7 +9787,7 @@
       <x:c r="C27" s="91"/>
       <x:c r="D27" s="89"/>
       <x:c r="E27" s="62" t="s">
-        <x:v>79</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="F27" s="62"/>
       <x:c r="G27" s="62"/>
@@ -9776,7 +9799,7 @@
       <x:c r="C28" s="91"/>
       <x:c r="D28" s="89"/>
       <x:c r="E28" s="62" t="s">
-        <x:v>80</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F28" s="62"/>
       <x:c r="G28" s="62"/>
@@ -9788,7 +9811,7 @@
       <x:c r="C29" s="96"/>
       <x:c r="D29" s="93"/>
       <x:c r="E29" s="65" t="s">
-        <x:v>71</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F29" s="65"/>
       <x:c r="G29" s="65"/>
@@ -9797,10 +9820,10 @@
     <x:row r="30" spans="1:8">
       <x:c r="A30" s="84"/>
       <x:c r="B30" s="78" t="s">
-        <x:v>55</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C30" s="67" t="s">
-        <x:v>84</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="D30" s="61"/>
       <x:c r="E30" s="61"/>
@@ -9812,7 +9835,7 @@
       <x:c r="A31" s="84"/>
       <x:c r="B31" s="78"/>
       <x:c r="C31" s="58" t="s">
-        <x:v>64</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="D31" s="62"/>
       <x:c r="E31" s="62"/>
@@ -9824,7 +9847,7 @@
       <x:c r="A32" s="84"/>
       <x:c r="B32" s="78"/>
       <x:c r="C32" s="58" t="s">
-        <x:v>127</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="D32" s="62"/>
       <x:c r="E32" s="62"/>
@@ -9836,7 +9859,7 @@
       <x:c r="A33" s="84"/>
       <x:c r="B33" s="95"/>
       <x:c r="C33" s="68" t="s">
-        <x:v>158</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="D33" s="65"/>
       <x:c r="E33" s="65"/>
@@ -9847,10 +9870,10 @@
     <x:row r="34" spans="1:8">
       <x:c r="A34" s="84"/>
       <x:c r="B34" s="78" t="s">
-        <x:v>153</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C34" s="67" t="s">
-        <x:v>224</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D34" s="61"/>
       <x:c r="E34" s="61"/>
@@ -9862,10 +9885,10 @@
       <x:c r="A35" s="84"/>
       <x:c r="B35" s="78"/>
       <x:c r="C35" s="94" t="s">
-        <x:v>138</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="D35" s="62" t="s">
-        <x:v>74</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="E35" s="62"/>
       <x:c r="F35" s="62"/>
@@ -9877,7 +9900,7 @@
       <x:c r="B36" s="78"/>
       <x:c r="C36" s="91"/>
       <x:c r="D36" s="62" t="s">
-        <x:v>170</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="E36" s="62"/>
       <x:c r="F36" s="62"/>
@@ -9889,7 +9912,7 @@
       <x:c r="B37" s="95"/>
       <x:c r="C37" s="96"/>
       <x:c r="D37" s="65" t="s">
-        <x:v>219</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E37" s="65"/>
       <x:c r="F37" s="65"/>
@@ -10150,7 +10173,7 @@
     <x:mergeCell ref="C35:C37"/>
     <x:mergeCell ref="B34:B37"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51138889789581299" footer="0.51138889789581299"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -10213,34 +10236,34 @@
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="49"/>
       <x:c r="B2" s="36" t="s">
-        <x:v>49</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="C2" s="36" t="s">
-        <x:v>190</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D2" s="36" t="s">
-        <x:v>126</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E2" s="36" t="s">
-        <x:v>152</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F2" s="36" t="s">
-        <x:v>67</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" ht="16.75">
       <x:c r="A3" s="49"/>
       <x:c r="B3" s="77" t="s">
-        <x:v>99</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C3" s="80" t="s">
-        <x:v>164</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="D3" s="80" t="s">
-        <x:v>163</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="E3" s="50" t="s">
-        <x:v>185</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F3" s="69"/>
     </x:row>
@@ -10250,7 +10273,7 @@
       <x:c r="C4" s="81"/>
       <x:c r="D4" s="81"/>
       <x:c r="E4" s="51" t="s">
-        <x:v>3</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F4" s="70"/>
     </x:row>
@@ -10260,7 +10283,7 @@
       <x:c r="C5" s="81"/>
       <x:c r="D5" s="81"/>
       <x:c r="E5" s="51" t="s">
-        <x:v>179</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F5" s="70"/>
     </x:row>
@@ -10270,7 +10293,7 @@
       <x:c r="C6" s="81"/>
       <x:c r="D6" s="81"/>
       <x:c r="E6" s="51" t="s">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="F6" s="70"/>
     </x:row>
@@ -10280,7 +10303,7 @@
       <x:c r="C7" s="81"/>
       <x:c r="D7" s="76"/>
       <x:c r="E7" s="52" t="s">
-        <x:v>182</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F7" s="70"/>
     </x:row>
@@ -10289,10 +10312,10 @@
       <x:c r="B8" s="78"/>
       <x:c r="C8" s="81"/>
       <x:c r="D8" s="75" t="s">
-        <x:v>44</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="E8" s="53" t="s">
-        <x:v>183</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F8" s="70"/>
     </x:row>
@@ -10302,7 +10325,7 @@
       <x:c r="C9" s="81"/>
       <x:c r="D9" s="81"/>
       <x:c r="E9" s="51" t="s">
-        <x:v>231</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="F9" s="70"/>
     </x:row>
@@ -10312,7 +10335,7 @@
       <x:c r="C10" s="81"/>
       <x:c r="D10" s="76"/>
       <x:c r="E10" s="54" t="s">
-        <x:v>180</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="F10" s="70"/>
     </x:row>
@@ -10321,10 +10344,10 @@
       <x:c r="B11" s="78"/>
       <x:c r="C11" s="81"/>
       <x:c r="D11" s="75" t="s">
-        <x:v>75</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="E11" s="53" t="s">
-        <x:v>41</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F11" s="70"/>
     </x:row>
@@ -10334,7 +10357,7 @@
       <x:c r="C12" s="76"/>
       <x:c r="D12" s="76"/>
       <x:c r="E12" s="54" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F12" s="70"/>
     </x:row>
@@ -10342,13 +10365,13 @@
       <x:c r="A13" s="49"/>
       <x:c r="B13" s="78"/>
       <x:c r="C13" s="75" t="s">
-        <x:v>220</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D13" s="75" t="s">
-        <x:v>89</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="E13" s="53" t="s">
-        <x:v>240</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F13" s="70"/>
     </x:row>
@@ -10358,7 +10381,7 @@
       <x:c r="C14" s="81"/>
       <x:c r="D14" s="81"/>
       <x:c r="E14" s="51" t="s">
-        <x:v>184</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F14" s="70"/>
     </x:row>
@@ -10368,7 +10391,7 @@
       <x:c r="C15" s="81"/>
       <x:c r="D15" s="81"/>
       <x:c r="E15" s="51" t="s">
-        <x:v>232</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="F15" s="70"/>
     </x:row>
@@ -10378,7 +10401,7 @@
       <x:c r="C16" s="81"/>
       <x:c r="D16" s="76"/>
       <x:c r="E16" s="54" t="s">
-        <x:v>36</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F16" s="70"/>
     </x:row>
@@ -10387,10 +10410,10 @@
       <x:c r="B17" s="78"/>
       <x:c r="C17" s="81"/>
       <x:c r="D17" s="75" t="s">
-        <x:v>78</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="E17" s="53" t="s">
-        <x:v>228</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="F17" s="70"/>
     </x:row>
@@ -10400,7 +10423,7 @@
       <x:c r="C18" s="76"/>
       <x:c r="D18" s="76"/>
       <x:c r="E18" s="52" t="s">
-        <x:v>238</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F18" s="70"/>
     </x:row>
@@ -10408,13 +10431,13 @@
       <x:c r="A19" s="49"/>
       <x:c r="B19" s="78"/>
       <x:c r="C19" s="75" t="s">
-        <x:v>65</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="D19" s="75" t="s">
-        <x:v>91</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E19" s="53" t="s">
-        <x:v>246</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="F19" s="70"/>
     </x:row>
@@ -10424,7 +10447,7 @@
       <x:c r="C20" s="81"/>
       <x:c r="D20" s="76"/>
       <x:c r="E20" s="54" t="s">
-        <x:v>8</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F20" s="70"/>
     </x:row>
@@ -10433,10 +10456,10 @@
       <x:c r="B21" s="78"/>
       <x:c r="C21" s="81"/>
       <x:c r="D21" s="75" t="s">
-        <x:v>195</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E21" s="53" t="s">
-        <x:v>2</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="F21" s="70"/>
     </x:row>
@@ -10446,7 +10469,7 @@
       <x:c r="C22" s="81"/>
       <x:c r="D22" s="76"/>
       <x:c r="E22" s="54" t="s">
-        <x:v>40</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F22" s="70"/>
     </x:row>
@@ -10455,10 +10478,10 @@
       <x:c r="B23" s="78"/>
       <x:c r="C23" s="81"/>
       <x:c r="D23" s="37" t="s">
-        <x:v>61</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="E23" s="55" t="s">
-        <x:v>37</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F23" s="70"/>
     </x:row>
@@ -10467,10 +10490,10 @@
       <x:c r="B24" s="78"/>
       <x:c r="C24" s="81"/>
       <x:c r="D24" s="75" t="s">
-        <x:v>215</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E24" s="53" t="s">
-        <x:v>92</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F24" s="70"/>
     </x:row>
@@ -10480,7 +10503,7 @@
       <x:c r="C25" s="81"/>
       <x:c r="D25" s="81"/>
       <x:c r="E25" s="51" t="s">
-        <x:v>38</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F25" s="70"/>
     </x:row>
@@ -10490,7 +10513,7 @@
       <x:c r="C26" s="81"/>
       <x:c r="D26" s="81"/>
       <x:c r="E26" s="51" t="s">
-        <x:v>33</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F26" s="70"/>
     </x:row>
@@ -10500,23 +10523,23 @@
       <x:c r="C27" s="99"/>
       <x:c r="D27" s="99"/>
       <x:c r="E27" s="56" t="s">
-        <x:v>234</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F27" s="71"/>
     </x:row>
     <x:row r="28" spans="1:6" ht="16.75">
       <x:c r="A28" s="49"/>
       <x:c r="B28" s="77" t="s">
-        <x:v>124</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C28" s="72" t="s">
-        <x:v>101</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D28" s="72" t="s">
-        <x:v>73</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="E28" s="73" t="s">
-        <x:v>235</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="F28" s="69"/>
     </x:row>
@@ -10524,13 +10547,13 @@
       <x:c r="A29" s="49"/>
       <x:c r="B29" s="78"/>
       <x:c r="C29" s="75" t="s">
-        <x:v>103</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="D29" s="37" t="s">
-        <x:v>63</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="E29" s="55" t="s">
-        <x:v>39</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="F29" s="70"/>
     </x:row>
@@ -10539,10 +10562,10 @@
       <x:c r="B30" s="78"/>
       <x:c r="C30" s="81"/>
       <x:c r="D30" s="75" t="s">
-        <x:v>72</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="E30" s="53" t="s">
-        <x:v>242</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="F30" s="70"/>
     </x:row>
@@ -10552,7 +10575,7 @@
       <x:c r="C31" s="81"/>
       <x:c r="D31" s="81"/>
       <x:c r="E31" s="51" t="s">
-        <x:v>34</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F31" s="70"/>
     </x:row>
@@ -10562,7 +10585,7 @@
       <x:c r="C32" s="81"/>
       <x:c r="D32" s="81"/>
       <x:c r="E32" s="51" t="s">
-        <x:v>186</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F32" s="70"/>
     </x:row>
@@ -10572,19 +10595,19 @@
       <x:c r="C33" s="99"/>
       <x:c r="D33" s="99"/>
       <x:c r="E33" s="56" t="s">
-        <x:v>245</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F33" s="71"/>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="49"/>
       <x:c r="B34" s="78" t="s">
-        <x:v>100</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="C34" s="81"/>
       <x:c r="D34" s="81"/>
       <x:c r="E34" s="51" t="s">
-        <x:v>11</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F34" s="70"/>
     </x:row>
@@ -10594,7 +10617,7 @@
       <x:c r="C35" s="99"/>
       <x:c r="D35" s="99"/>
       <x:c r="E35" s="56" t="s">
-        <x:v>247</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F35" s="71"/>
     </x:row>
@@ -10669,7 +10692,7 @@
     <x:mergeCell ref="D34:D35"/>
     <x:mergeCell ref="C34:C35"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51138889789581299" footer="0.51138889789581299"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
add 0715 comment, 0716 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="10956" windowHeight="8568"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8568"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Datebook" sheetId="1" r:id="rId4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="249">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="252">
   <x:si>
     <x:t>1. 요구사항 분석 (실현성 확인)
 2. 데이터 흐름도 수정
@@ -33,49 +33,79 @@
  -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
-2. 블루투스 관련 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 현장실습 OT
- - 기업 소개 및 업무 설명
- - 앞으로 수행하게 될 프로젝트 설명
-2. 기존에 진행했던 캡스톤프로젝트 첨언
-3. 제품 개발 과정 설명
- - 제품 기획 
- - 개발 기획  
- - 개발 설계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
 2. 요구사항 분석
 3. 구현 가능 여부 확인</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 추가 자료조사
-2. 요구사항 추가 조사
-3. 경쟁 어플 기능 비교 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Git 목록 삭제
-2. 요구사항 분석
-3. 인터페이스 구상도 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 추가 자료조사(관련 코드)
-2. FlowChart 수정 및 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 필요 자료 추가 조사
+2. 한계점 및 필요기술 추가
+ - 차량 블루투스와 어플 연결 어떻게?
+ - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
+2. 추가 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 경쟁 어플 메뉴트리 수정
+2. 요구사항, 기능정의 순서 수정
+3. 한계점 수정
+블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+ - 컴퓨터 견적 추천 앱
+ - 주차시 사고발생 알림 앱
+2. 주제 아이디어 최종 선정
+ - 차량 관리 어플
+3. 개발 계획서 및 요구사항 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 07.02 회의록 작성
+2. Git 업로드 한 것 중 중복된 것들 삭제
+3. 어플 흐름 구상도 작성
+4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -89,12 +119,6 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 필요 자료 추가 조사
-2. 한계점 및 필요기술 추가
- - 차량 블루투스와 어플 연결 어떻게?
- - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
-  </x:si>
-  <x:si>
     <x:t>1-1. Datebook Comment 부분 요약
 1-2. GIT 보고서 다시 작성
 1-3. PPT 머릿글 요약 작성
@@ -103,25 +127,45 @@
 2. 요구사항 수집 및 분석</x:t>
   </x:si>
   <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
- - 컴퓨터 견적 추천 앱
- - 주차시 사고발생 알림 앱
-2. 주제 아이디어 최종 선정
- - 차량 관리 어플
-3. 개발 계획서 및 요구사항 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 경쟁 어플 메뉴트리 수정
-2. 요구사항, 기능정의 순서 수정
-3. 한계점 수정
-블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
+    <x:t>1. 현장실습 OT
+ - 기업 소개 및 업무 설명
+ - 앞으로 수행하게 될 프로젝트 설명
+2. 기존에 진행했던 캡스톤프로젝트 첨언
+3. 제품 개발 과정 설명
+ - 제품 기획 
+ - 개발 기획  
+ - 개발 설계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성 (미완)
+2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사(관련 코드)
+2. FlowChart 수정 및 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. (2-2) 수익적 요소 추가
+2. (4-1) 기능정의 추가
+3. 추가 자료 조사
+ - 비슷한 어플(마이클) 화면 구성 조사</x:t>
   </x:si>
   <x:si>
     <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
@@ -133,54 +177,425 @@
 3. Menu_Tree 도식화 수정</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 07.02 회의록 작성
-2. Git 업로드 한 것 중 중복된 것들 삭제
-3. 어플 흐름 구상도 작성
-4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 진행사항 체크 및 2주차 목표 설정
-2. 06.28 회의록 작성
-3. 상용화 된 타 앱 기능 분석
-4. 요구사항 정의
- - 회원가입, DB, 무결성 (미완)
-5. vi사용법 설명</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 앱 화면별 Sequence 작성
 2. 앱 화면별 어떻게 구성할 것인지 구상
 3. 추가 자료조사</x:t>
   </x:si>
   <x:si>
-    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
+로그인 버튼이 나와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
+2. 블루투스 관련 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검내역서(정비소 제공 문서)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리별 check list</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보(오너들의 평균 정보)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
+비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>경기/인천</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오너들의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수리견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 메뉴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>견적 요청</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고객상담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>최신 글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록 및 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오늘 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연차, 보험료</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tips</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공유게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>더 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>글 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 방문 장소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Menu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 검사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자차 게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>함수의 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALL*</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공식 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 주변 검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수익적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험사 선택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메모 입력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 시기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결함/리콜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균 연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>첫예약할인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카카오톡 문의</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>setting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 후기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모두의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>엔진오일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 시세</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필요 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차 정보 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연비 랭킹</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용 가이드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨 필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>디테일링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어샵</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 장착점 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 추천 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소 지도 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 정보 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:22
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>진행 방향 ---&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:40
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스 (메뉴)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 기본 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 형태로 존재</x:t>
+  </x:si>
+  <x:si>
+    <x:t>community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고장사례(리콜사례)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 판매견적 받기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자주 하는 질문</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유사 모델 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 교체 예상 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약/견적 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험료 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰 보유 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성</x:t>
   </x:si>
   <x:si>
     <x:t>1. vi 명령어 설명서 작성 완료
@@ -189,631 +604,8 @@
  - 비기능적 요구사항</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
-로그인 버튼이 나와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
-비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검내역서(정비소 제공 문서)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리별 check list</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보(오너들의 평균 정보)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. (2-2) 수익적 요소 추가
-2. (4-1) 기능정의 추가
-3. 추가 자료 조사
- - 비슷한 어플(마이클) 화면 구성 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 기본 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고장사례(리콜사례)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자주 하는 질문</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 판매견적 받기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유사 모델 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 교체 예상 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 정보 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:40
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 추천 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:22
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>진행 방향 ---&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스 (메뉴)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 장착점 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소 지도 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:25
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약/견적 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험료 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰 보유 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인 쿠폰 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>데이터 연동 설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 선호도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>친구 초대 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필요 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 시기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차 정보 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균 연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 후기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Home</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연비 랭킹</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험사 선택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모두의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메모 입력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 시세</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결함/리콜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>엔진오일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>첫예약할인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>카카오톡 문의</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>setting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용 가이드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨 필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>디테일링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어샵</x:t>
-  </x:si>
-  <x:si>
-    <x:t>글 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수리견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 방문 장소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공유게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 메뉴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>경기/인천</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>견적 요청</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고객상담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연차, 보험료</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 검사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>최신 글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록 및 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자차 게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>함수의 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALL*</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오늘 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>더 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오너들의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Menu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공식 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수익적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 주변 검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
-  </x:si>
-  <x:si>
-    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Q&amp;A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>장마철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>여름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>만족도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상황별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클</x:t>
-  </x:si>
-  <x:si>
-    <x:t>검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가을</x:t>
-  </x:si>
-  <x:si>
-    <x:t>채팅창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평점</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보안성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>편집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>겨울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>무결성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>달력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폭설철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>홈</x:t>
-  </x:si>
-  <x:si>
-    <x:t>봄</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인기글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>계절별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>광고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>손세차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>리뷰</x:t>
-  </x:si>
-  <x:si>
-    <x:t>최신글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 계약서 작성
-2. 현장실습 오리엔테이션</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 보완
-2. 기능정의 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Menu_Tree 수정(완료)
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
+    <x:t>1. 메뉴시퀀스 작성(설명,컨테이너등 정보 채우기)
+2. 기능플로우 작성</x:t>
   </x:si>
   <x:si>
     <x:t>1. 인터페이스 구상도 작성
@@ -821,60 +613,279 @@
 3. 추가 자료조사</x:t>
   </x:si>
   <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사
+2. 요구사항 추가 조사
+3. 경쟁 어플 기능 비교 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
     <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
   </x:si>
   <x:si>
+    <x:t>데이터 연동 설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>친구 초대 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 선호도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인 쿠폰 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가을</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>장마철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>만족도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>여름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q&amp;A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상황별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평점</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폭설철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>광고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>홈</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>달력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>봄</x:t>
+  </x:si>
+  <x:si>
+    <x:t>편집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보안성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인기글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>손세차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>리뷰</x:t>
+  </x:si>
+  <x:si>
+    <x:t>겨울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>계절별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>무결성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>최신글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>방문 정비소 기록, 메모</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차종, 차번호, 연식 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>항목 및 정비 주기 추가</x:t>
+  </x:si>
+  <x:si>
     <x:t>이달의 정비/세차 혜택</x:t>
   </x:si>
   <x:si>
+    <x:t>부품 별 남은 수명 보여줌</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소 포인트 적립 연동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 무료 판매 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검 스케쥴 및 일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 찾아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험료 확인 및 갱신일 알림</x:t>
+  </x:si>
+  <x:si>
     <x:t>기아 커넥티드카 연동하기</x:t>
   </x:si>
   <x:si>
-    <x:t>주유소 포인트 적립 연동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 무료 판매 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 별 남은 수명 보여줌</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검 스케쥴 및 일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험료 확인 및 갱신일 알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 찾아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차종, 차번호, 연식 등</x:t>
-  </x:si>
-  <x:si>
-    <x:t>방문 정비소 기록, 메모</x:t>
-  </x:si>
-  <x:si>
-    <x:t>항목 및 정비 주기 추가</x:t>
+    <x:t>1. Menu_Tree 수정(완료)
+2. 추가 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 보완
+2. 기능정의 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리에 메모한 사항 달력에 날짜 표시</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
   </x:si>
   <x:si>
     <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
   </x:si>
   <x:si>
-    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리에 메모한 사항 달력에 날짜 표시</x:t>
+    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
   </x:si>
   <x:si>
     <x:t>1. 화면 시퀀스 작성
 2. 추가 자료 조사</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 메뉴시퀀스 작성 (미완)
-2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
+    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 계약서 작성
+2. 현장실습 오리엔테이션</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2005,6 +2016,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
           <x:alignment horizontal="center" vertical="center"/>
           <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
@@ -2225,19 +2249,6 @@
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -2934,8 +2945,8 @@
   <x:dimension ref="B2:E42"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:pane xSplit="0" ySplit="2" topLeftCell="C15" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="E20" activeCellId="0" sqref="E20:E20"/>
+      <x:pane xSplit="0" ySplit="2" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
+      <x:selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21:D21"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -2951,16 +2962,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="5" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C2" s="6" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="D2" s="6" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E2" s="7" t="s">
         <x:v>117</x:v>
-      </x:c>
-      <x:c r="C2" s="6" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="D2" s="6" t="s">
-        <x:v>131</x:v>
-      </x:c>
-      <x:c r="E2" s="7" t="s">
-        <x:v>118</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -2968,13 +2979,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="15" t="s">
-        <x:v>77</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D3" s="9" t="s">
-        <x:v>216</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="E3" s="9" t="s">
-        <x:v>2</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -2982,13 +2993,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="14" t="s">
-        <x:v>77</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D4" s="12" t="s">
-        <x:v>19</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E4" s="12" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -2996,13 +3007,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="16" t="s">
-        <x:v>74</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D5" s="12" t="s">
-        <x:v>32</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E5" s="12" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -3010,13 +3021,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="18" t="s">
-        <x:v>74</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D6" s="12" t="s">
-        <x:v>13</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E6" s="17" t="s">
-        <x:v>14</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -3024,13 +3035,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="14" t="s">
-        <x:v>63</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="D7" s="12" t="s">
-        <x:v>222</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="E7" s="12" t="s">
-        <x:v>22</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -3038,13 +3049,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="14" t="s">
-        <x:v>69</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="D8" s="12" t="s">
-        <x:v>35</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E8" s="12" t="s">
-        <x:v>30</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -3052,13 +3063,13 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="19" t="s">
-        <x:v>62</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="D9" s="12" t="s">
-        <x:v>20</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E9" s="12" t="s">
-        <x:v>31</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -3066,13 +3077,13 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="20" t="s">
-        <x:v>78</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="D10" s="12" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="E10" s="12" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="E10" s="12" t="s">
-        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
@@ -3080,13 +3091,13 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="22" t="s">
-        <x:v>65</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="D11" s="12" t="s">
-        <x:v>8</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E11" s="12" t="s">
-        <x:v>21</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:5" ht="105.40000000000001">
@@ -3094,10 +3105,10 @@
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="21" t="s">
-        <x:v>71</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="D12" s="12" t="s">
-        <x:v>230</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="E12" s="12" t="s">
         <x:v>0</x:v>
@@ -3108,13 +3119,13 @@
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="23" t="s">
-        <x:v>78</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="D13" s="12" t="s">
-        <x:v>9</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E13" s="12" t="s">
-        <x:v>12</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5" ht="52.700000000000003">
@@ -3122,13 +3133,13 @@
         <x:v>44384</x:v>
       </x:c>
       <x:c r="C14" s="24" t="s">
-        <x:v>60</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="D14" s="12" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E14" s="12" t="s">
-        <x:v>42</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:5" ht="52.700000000000003">
@@ -3136,13 +3147,13 @@
         <x:v>44385</x:v>
       </x:c>
       <x:c r="C15" s="30" t="s">
-        <x:v>75</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="D15" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="2:5" ht="26.350000000000001">
@@ -3150,13 +3161,13 @@
         <x:v>44386</x:v>
       </x:c>
       <x:c r="C16" s="31" t="s">
-        <x:v>58</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D16" s="12" t="s">
-        <x:v>223</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="E16" s="12" t="s">
-        <x:v>17</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="2:5" ht="39.549999999999997">
@@ -3164,59 +3175,65 @@
         <x:v>44389</x:v>
       </x:c>
       <x:c r="C17" s="74" t="s">
-        <x:v>44</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D17" s="12" t="s">
-        <x:v>18</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>224</x:v>
+        <x:v>230</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:5" ht="26.350000000000001">
       <x:c r="B18" s="13">
         <x:v>44390</x:v>
       </x:c>
-      <x:c r="C18" s="100" t="s">
-        <x:v>37</x:v>
+      <x:c r="C18" s="75" t="s">
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D18" s="12" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="E18" s="12" t="s">
-        <x:v>1</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="2:5" ht="26.350000000000001">
       <x:c r="B19" s="13">
         <x:v>44391</x:v>
       </x:c>
-      <x:c r="C19" s="100" t="s">
-        <x:v>78</x:v>
+      <x:c r="C19" s="75" t="s">
+        <x:v>170</x:v>
       </x:c>
       <x:c r="D19" s="12" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="E19" s="12" t="s">
-        <x:v>248</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="2:5" ht="26.350000000000001">
       <x:c r="B20" s="13">
         <x:v>44392</x:v>
       </x:c>
-      <x:c r="C20" s="10"/>
+      <x:c r="C20" s="14" t="s">
+        <x:v>239</x:v>
+      </x:c>
       <x:c r="D20" s="12" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E20" s="11"/>
-    </x:row>
-    <x:row r="21" spans="2:5">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E20" s="11" t="s">
+        <x:v>160</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="2:5" ht="26.350000000000001">
       <x:c r="B21" s="13">
         <x:v>44393</x:v>
       </x:c>
       <x:c r="C21" s="10"/>
-      <x:c r="D21" s="11"/>
+      <x:c r="D21" s="12" t="s">
+        <x:v>162</x:v>
+      </x:c>
       <x:c r="E21" s="11"/>
     </x:row>
     <x:row r="22" spans="2:5">
@@ -3415,78 +3432,78 @@
   <x:sheetData>
     <x:row r="1" spans="1:9" ht="17.149999999999999">
       <x:c r="A1" s="26" t="s">
-        <x:v>64</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>154</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="D1" s="34" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="E1" s="34" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="F1" s="34" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="D1" s="34" t="s">
-        <x:v>151</x:v>
-      </x:c>
-      <x:c r="E1" s="34" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F1" s="34" t="s">
-        <x:v>87</x:v>
-      </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>90</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="H1" s="34" t="s">
-        <x:v>206</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="I1" s="35" t="s">
-        <x:v>184</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:9">
-      <x:c r="A2" s="83" t="s">
-        <x:v>178</x:v>
-      </x:c>
-      <x:c r="B2" s="77" t="s">
-        <x:v>198</x:v>
-      </x:c>
-      <x:c r="C2" s="80" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="D2" s="80" t="s">
-        <x:v>86</x:v>
+      <x:c r="A2" s="84" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="B2" s="78" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="C2" s="81" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="D2" s="81" t="s">
+        <x:v>112</x:v>
       </x:c>
       <x:c r="E2" s="38" t="s">
-        <x:v>102</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F2" s="38"/>
       <x:c r="G2" s="38"/>
       <x:c r="H2" s="38"/>
       <x:c r="I2" s="38" t="s">
-        <x:v>51</x:v>
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9">
-      <x:c r="A3" s="84"/>
-      <x:c r="B3" s="78"/>
-      <x:c r="C3" s="81"/>
-      <x:c r="D3" s="81"/>
+      <x:c r="A3" s="85"/>
+      <x:c r="B3" s="79"/>
+      <x:c r="C3" s="82"/>
+      <x:c r="D3" s="82"/>
       <x:c r="E3" s="37" t="s">
-        <x:v>47</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="F3" s="37"/>
       <x:c r="G3" s="37"/>
       <x:c r="H3" s="37"/>
       <x:c r="I3" s="37" t="s">
-        <x:v>238</x:v>
+        <x:v>228</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
-      <x:c r="A4" s="84"/>
-      <x:c r="B4" s="78"/>
-      <x:c r="C4" s="81"/>
-      <x:c r="D4" s="81"/>
+      <x:c r="A4" s="85"/>
+      <x:c r="B4" s="79"/>
+      <x:c r="C4" s="82"/>
+      <x:c r="D4" s="82"/>
       <x:c r="E4" s="37" t="s">
-        <x:v>101</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F4" s="37"/>
       <x:c r="G4" s="37"/>
@@ -3494,42 +3511,42 @@
       <x:c r="I4" s="37"/>
     </x:row>
     <x:row r="5" spans="1:9">
-      <x:c r="A5" s="84"/>
-      <x:c r="B5" s="78"/>
-      <x:c r="C5" s="81"/>
-      <x:c r="D5" s="81"/>
-      <x:c r="E5" s="75" t="s">
-        <x:v>105</x:v>
+      <x:c r="A5" s="85"/>
+      <x:c r="B5" s="79"/>
+      <x:c r="C5" s="82"/>
+      <x:c r="D5" s="82"/>
+      <x:c r="E5" s="76" t="s">
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F5" s="37" t="s">
-        <x:v>127</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="G5" s="37"/>
       <x:c r="H5" s="37"/>
       <x:c r="I5" s="37"/>
     </x:row>
     <x:row r="6" spans="1:9">
-      <x:c r="A6" s="84"/>
-      <x:c r="B6" s="78"/>
-      <x:c r="C6" s="81"/>
-      <x:c r="D6" s="76"/>
-      <x:c r="E6" s="76"/>
+      <x:c r="A6" s="85"/>
+      <x:c r="B6" s="79"/>
+      <x:c r="C6" s="82"/>
+      <x:c r="D6" s="77"/>
+      <x:c r="E6" s="77"/>
       <x:c r="F6" s="37" t="s">
-        <x:v>57</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="G6" s="37"/>
       <x:c r="H6" s="37"/>
       <x:c r="I6" s="37"/>
     </x:row>
     <x:row r="7" spans="1:9">
-      <x:c r="A7" s="84"/>
-      <x:c r="B7" s="78"/>
-      <x:c r="C7" s="81"/>
-      <x:c r="D7" s="75" t="s">
-        <x:v>129</x:v>
+      <x:c r="A7" s="85"/>
+      <x:c r="B7" s="79"/>
+      <x:c r="C7" s="82"/>
+      <x:c r="D7" s="76" t="s">
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E7" s="37" t="s">
-        <x:v>172</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F7" s="37"/>
       <x:c r="G7" s="37"/>
@@ -3537,91 +3554,91 @@
       <x:c r="I7" s="37"/>
     </x:row>
     <x:row r="8" spans="1:9">
-      <x:c r="A8" s="84"/>
-      <x:c r="B8" s="78"/>
-      <x:c r="C8" s="81"/>
-      <x:c r="D8" s="81"/>
+      <x:c r="A8" s="85"/>
+      <x:c r="B8" s="79"/>
+      <x:c r="C8" s="82"/>
+      <x:c r="D8" s="82"/>
       <x:c r="E8" s="37" t="s">
-        <x:v>190</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="F8" s="37"/>
       <x:c r="G8" s="37"/>
       <x:c r="H8" s="37"/>
       <x:c r="I8" s="37" t="s">
-        <x:v>164</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:9">
-      <x:c r="A9" s="84"/>
-      <x:c r="B9" s="78"/>
-      <x:c r="C9" s="81"/>
-      <x:c r="D9" s="81"/>
+      <x:c r="A9" s="85"/>
+      <x:c r="B9" s="79"/>
+      <x:c r="C9" s="82"/>
+      <x:c r="D9" s="82"/>
       <x:c r="E9" s="37" t="s">
-        <x:v>188</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F9" s="37"/>
       <x:c r="G9" s="37"/>
       <x:c r="H9" s="37"/>
       <x:c r="I9" s="37" t="s">
-        <x:v>237</x:v>
+        <x:v>226</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
-      <x:c r="A10" s="84"/>
-      <x:c r="B10" s="78"/>
-      <x:c r="C10" s="81"/>
-      <x:c r="D10" s="81"/>
-      <x:c r="E10" s="75" t="s">
-        <x:v>140</x:v>
+      <x:c r="A10" s="85"/>
+      <x:c r="B10" s="79"/>
+      <x:c r="C10" s="82"/>
+      <x:c r="D10" s="82"/>
+      <x:c r="E10" s="76" t="s">
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F10" s="37" t="s">
-        <x:v>111</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G10" s="37"/>
       <x:c r="H10" s="37"/>
       <x:c r="I10" s="37"/>
     </x:row>
     <x:row r="11" spans="1:9">
-      <x:c r="A11" s="84"/>
-      <x:c r="B11" s="78"/>
-      <x:c r="C11" s="81"/>
-      <x:c r="D11" s="81"/>
-      <x:c r="E11" s="81"/>
+      <x:c r="A11" s="85"/>
+      <x:c r="B11" s="79"/>
+      <x:c r="C11" s="82"/>
+      <x:c r="D11" s="82"/>
+      <x:c r="E11" s="82"/>
       <x:c r="F11" s="37" t="s">
-        <x:v>116</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="G11" s="37"/>
       <x:c r="H11" s="37"/>
       <x:c r="I11" s="37" t="s">
-        <x:v>229</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
-      <x:c r="A12" s="84"/>
-      <x:c r="B12" s="78"/>
-      <x:c r="C12" s="81"/>
-      <x:c r="D12" s="81"/>
-      <x:c r="E12" s="81"/>
+      <x:c r="A12" s="85"/>
+      <x:c r="B12" s="79"/>
+      <x:c r="C12" s="82"/>
+      <x:c r="D12" s="82"/>
+      <x:c r="E12" s="82"/>
       <x:c r="F12" s="37" t="s">
-        <x:v>187</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="G12" s="37"/>
       <x:c r="H12" s="37"/>
       <x:c r="I12" s="37"/>
     </x:row>
     <x:row r="13" spans="1:28">
-      <x:c r="A13" s="84"/>
-      <x:c r="B13" s="78"/>
-      <x:c r="C13" s="76"/>
-      <x:c r="D13" s="76"/>
-      <x:c r="E13" s="76"/>
+      <x:c r="A13" s="85"/>
+      <x:c r="B13" s="79"/>
+      <x:c r="C13" s="77"/>
+      <x:c r="D13" s="77"/>
+      <x:c r="E13" s="77"/>
       <x:c r="F13" s="37" t="s">
-        <x:v>201</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="G13" s="37"/>
       <x:c r="H13" s="37"/>
       <x:c r="I13" s="37" t="s">
-        <x:v>242</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="J13" s="29"/>
       <x:c r="K13" s="29"/>
@@ -3644,22 +3661,22 @@
       <x:c r="AB13" s="29"/>
     </x:row>
     <x:row r="14" spans="1:28">
-      <x:c r="A14" s="84"/>
-      <x:c r="B14" s="78"/>
-      <x:c r="C14" s="75" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="D14" s="75" t="s">
-        <x:v>113</x:v>
+      <x:c r="A14" s="85"/>
+      <x:c r="B14" s="79"/>
+      <x:c r="C14" s="76" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="D14" s="76" t="s">
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E14" s="37" t="s">
-        <x:v>182</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F14" s="37"/>
       <x:c r="G14" s="37"/>
       <x:c r="H14" s="37"/>
       <x:c r="I14" s="37" t="s">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="J14" s="29"/>
       <x:c r="K14" s="29"/>
@@ -3682,18 +3699,18 @@
       <x:c r="AB14" s="29"/>
     </x:row>
     <x:row r="15" spans="1:28">
-      <x:c r="A15" s="84"/>
-      <x:c r="B15" s="78"/>
-      <x:c r="C15" s="81"/>
-      <x:c r="D15" s="81"/>
+      <x:c r="A15" s="85"/>
+      <x:c r="B15" s="79"/>
+      <x:c r="C15" s="82"/>
+      <x:c r="D15" s="82"/>
       <x:c r="E15" s="37" t="s">
-        <x:v>91</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="F15" s="37"/>
       <x:c r="G15" s="37"/>
       <x:c r="H15" s="37"/>
       <x:c r="I15" s="37" t="s">
-        <x:v>95</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="J15" s="29"/>
       <x:c r="K15" s="29"/>
@@ -3716,12 +3733,12 @@
       <x:c r="AB15" s="29"/>
     </x:row>
     <x:row r="16" spans="1:28">
-      <x:c r="A16" s="84"/>
-      <x:c r="B16" s="78"/>
-      <x:c r="C16" s="81"/>
-      <x:c r="D16" s="81"/>
+      <x:c r="A16" s="85"/>
+      <x:c r="B16" s="79"/>
+      <x:c r="C16" s="82"/>
+      <x:c r="D16" s="82"/>
       <x:c r="E16" s="37" t="s">
-        <x:v>92</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F16" s="37"/>
       <x:c r="G16" s="37"/>
@@ -3747,12 +3764,12 @@
       <x:c r="AB16" s="29"/>
     </x:row>
     <x:row r="17" spans="1:28">
-      <x:c r="A17" s="84"/>
-      <x:c r="B17" s="78"/>
-      <x:c r="C17" s="81"/>
-      <x:c r="D17" s="76"/>
+      <x:c r="A17" s="85"/>
+      <x:c r="B17" s="79"/>
+      <x:c r="C17" s="82"/>
+      <x:c r="D17" s="77"/>
       <x:c r="E17" s="37" t="s">
-        <x:v>103</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F17" s="37"/>
       <x:c r="G17" s="37"/>
@@ -3781,17 +3798,17 @@
       <x:c r="AB17" s="29"/>
     </x:row>
     <x:row r="18" spans="1:28">
-      <x:c r="A18" s="84"/>
-      <x:c r="B18" s="78"/>
-      <x:c r="C18" s="81"/>
+      <x:c r="A18" s="85"/>
+      <x:c r="B18" s="79"/>
+      <x:c r="C18" s="82"/>
       <x:c r="D18" s="37" t="s">
-        <x:v>81</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="E18" s="37" t="s">
-        <x:v>73</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F18" s="37" t="s">
-        <x:v>96</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="G18" s="37"/>
       <x:c r="H18" s="37"/>
@@ -3817,18 +3834,18 @@
       <x:c r="AB18" s="29"/>
     </x:row>
     <x:row r="19" spans="1:28">
-      <x:c r="A19" s="84"/>
-      <x:c r="B19" s="78"/>
-      <x:c r="C19" s="81"/>
+      <x:c r="A19" s="85"/>
+      <x:c r="B19" s="79"/>
+      <x:c r="C19" s="82"/>
       <x:c r="D19" s="37" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="E19" s="37"/>
       <x:c r="F19" s="37"/>
       <x:c r="G19" s="37"/>
       <x:c r="H19" s="37"/>
-      <x:c r="I19" s="75" t="s">
-        <x:v>52</x:v>
+      <x:c r="I19" s="76" t="s">
+        <x:v>145</x:v>
       </x:c>
       <x:c r="J19" s="29"/>
       <x:c r="K19" s="29"/>
@@ -3851,17 +3868,17 @@
       <x:c r="AB19" s="29"/>
     </x:row>
     <x:row r="20" spans="1:28">
-      <x:c r="A20" s="84"/>
-      <x:c r="B20" s="78"/>
-      <x:c r="C20" s="81"/>
+      <x:c r="A20" s="85"/>
+      <x:c r="B20" s="79"/>
+      <x:c r="C20" s="82"/>
       <x:c r="D20" s="37" t="s">
-        <x:v>103</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="E20" s="37"/>
       <x:c r="F20" s="37"/>
       <x:c r="G20" s="37"/>
       <x:c r="H20" s="37"/>
-      <x:c r="I20" s="81"/>
+      <x:c r="I20" s="82"/>
       <x:c r="J20" s="29"/>
       <x:c r="K20" s="29"/>
       <x:c r="L20" s="29"/>
@@ -3883,17 +3900,17 @@
       <x:c r="AB20" s="29"/>
     </x:row>
     <x:row r="21" spans="1:28">
-      <x:c r="A21" s="84"/>
-      <x:c r="B21" s="78"/>
-      <x:c r="C21" s="81"/>
+      <x:c r="A21" s="85"/>
+      <x:c r="B21" s="79"/>
+      <x:c r="C21" s="82"/>
       <x:c r="D21" s="37" t="s">
-        <x:v>92</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="E21" s="37"/>
       <x:c r="F21" s="37"/>
       <x:c r="G21" s="37"/>
       <x:c r="H21" s="37"/>
-      <x:c r="I21" s="76"/>
+      <x:c r="I21" s="77"/>
       <x:c r="J21" s="29"/>
       <x:c r="K21" s="29"/>
       <x:c r="L21" s="29"/>
@@ -3915,11 +3932,11 @@
       <x:c r="AB21" s="29"/>
     </x:row>
     <x:row r="22" spans="1:28">
-      <x:c r="A22" s="84"/>
-      <x:c r="B22" s="79"/>
-      <x:c r="C22" s="76"/>
+      <x:c r="A22" s="85"/>
+      <x:c r="B22" s="80"/>
+      <x:c r="C22" s="77"/>
       <x:c r="D22" s="37" t="s">
-        <x:v>54</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E22" s="37"/>
       <x:c r="F22" s="37"/>
@@ -3947,12 +3964,12 @@
       <x:c r="AB22" s="29"/>
     </x:row>
     <x:row r="23" spans="1:28">
-      <x:c r="A23" s="84"/>
-      <x:c r="B23" s="82" t="s">
-        <x:v>107</x:v>
+      <x:c r="A23" s="85"/>
+      <x:c r="B23" s="83" t="s">
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C23" s="37" t="s">
-        <x:v>72</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="D23" s="37"/>
       <x:c r="E23" s="37"/>
@@ -3981,10 +3998,10 @@
       <x:c r="AB23" s="29"/>
     </x:row>
     <x:row r="24" spans="1:28">
-      <x:c r="A24" s="84"/>
-      <x:c r="B24" s="78"/>
+      <x:c r="A24" s="85"/>
+      <x:c r="B24" s="79"/>
       <x:c r="C24" s="37" t="s">
-        <x:v>207</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="D24" s="37"/>
       <x:c r="E24" s="37"/>
@@ -4013,10 +4030,10 @@
       <x:c r="AB24" s="29"/>
     </x:row>
     <x:row r="25" spans="1:28">
-      <x:c r="A25" s="84"/>
-      <x:c r="B25" s="78"/>
+      <x:c r="A25" s="85"/>
+      <x:c r="B25" s="79"/>
       <x:c r="C25" s="37" t="s">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="D25" s="37"/>
       <x:c r="E25" s="37"/>
@@ -4045,16 +4062,16 @@
       <x:c r="AB25" s="29"/>
     </x:row>
     <x:row r="26" spans="1:87">
-      <x:c r="A26" s="84"/>
-      <x:c r="B26" s="78"/>
-      <x:c r="C26" s="75" t="s">
+      <x:c r="A26" s="85"/>
+      <x:c r="B26" s="79"/>
+      <x:c r="C26" s="76" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="D26" s="37" t="s">
         <x:v>107</x:v>
       </x:c>
-      <x:c r="D26" s="37" t="s">
-        <x:v>106</x:v>
-      </x:c>
       <x:c r="E26" s="37" t="s">
-        <x:v>53</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F26" s="37"/>
       <x:c r="G26" s="37"/>
@@ -4140,17 +4157,17 @@
       <x:c r="CI26" s="29"/>
     </x:row>
     <x:row r="27" spans="1:87" s="1" customFormat="1">
-      <x:c r="A27" s="83"/>
-      <x:c r="B27" s="82"/>
-      <x:c r="C27" s="81"/>
-      <x:c r="D27" s="75" t="s">
-        <x:v>209</x:v>
+      <x:c r="A27" s="84"/>
+      <x:c r="B27" s="83"/>
+      <x:c r="C27" s="82"/>
+      <x:c r="D27" s="76" t="s">
+        <x:v>199</x:v>
       </x:c>
       <x:c r="E27" s="37" t="s">
-        <x:v>150</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F27" s="37" t="s">
-        <x:v>67</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G27" s="37"/>
       <x:c r="H27" s="37"/>
@@ -4235,15 +4252,15 @@
       <x:c r="CI27" s="29"/>
     </x:row>
     <x:row r="28" spans="1:87">
-      <x:c r="A28" s="84"/>
-      <x:c r="B28" s="78"/>
-      <x:c r="C28" s="81"/>
-      <x:c r="D28" s="76"/>
+      <x:c r="A28" s="85"/>
+      <x:c r="B28" s="79"/>
+      <x:c r="C28" s="82"/>
+      <x:c r="D28" s="77"/>
       <x:c r="E28" s="37" t="s">
-        <x:v>156</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F28" s="37" t="s">
-        <x:v>67</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="G28" s="37"/>
       <x:c r="H28" s="37"/>
@@ -4328,14 +4345,14 @@
       <x:c r="CI28" s="29"/>
     </x:row>
     <x:row r="29" spans="1:87">
-      <x:c r="A29" s="84"/>
-      <x:c r="B29" s="78"/>
-      <x:c r="C29" s="81"/>
+      <x:c r="A29" s="85"/>
+      <x:c r="B29" s="79"/>
+      <x:c r="C29" s="82"/>
       <x:c r="D29" s="37" t="s">
-        <x:v>125</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E29" s="39" t="s">
-        <x:v>132</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F29" s="39"/>
       <x:c r="G29" s="37"/>
@@ -4421,14 +4438,14 @@
       <x:c r="CI29" s="29"/>
     </x:row>
     <x:row r="30" spans="1:87">
-      <x:c r="A30" s="84"/>
-      <x:c r="B30" s="78"/>
-      <x:c r="C30" s="81"/>
+      <x:c r="A30" s="85"/>
+      <x:c r="B30" s="79"/>
+      <x:c r="C30" s="82"/>
       <x:c r="D30" s="37" t="s">
-        <x:v>121</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="E30" s="37" t="s">
-        <x:v>183</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F30" s="37"/>
       <x:c r="G30" s="37"/>
@@ -4514,12 +4531,12 @@
       <x:c r="CI30" s="29"/>
     </x:row>
     <x:row r="31" spans="1:87" s="1" customFormat="1">
-      <x:c r="A31" s="83"/>
-      <x:c r="B31" s="82"/>
-      <x:c r="C31" s="81"/>
+      <x:c r="A31" s="84"/>
+      <x:c r="B31" s="83"/>
+      <x:c r="C31" s="82"/>
       <x:c r="D31" s="37"/>
       <x:c r="E31" s="37" t="s">
-        <x:v>130</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F31" s="37"/>
       <x:c r="G31" s="37"/>
@@ -4605,14 +4622,14 @@
       <x:c r="CI31" s="29"/>
     </x:row>
     <x:row r="32" spans="1:87">
-      <x:c r="A32" s="84"/>
-      <x:c r="B32" s="78"/>
-      <x:c r="C32" s="81"/>
+      <x:c r="A32" s="85"/>
+      <x:c r="B32" s="79"/>
+      <x:c r="C32" s="82"/>
       <x:c r="D32" s="37" t="s">
-        <x:v>104</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E32" s="37" t="s">
-        <x:v>115</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F32" s="37"/>
       <x:c r="G32" s="37"/>
@@ -4698,11 +4715,11 @@
       <x:c r="CI32" s="29"/>
     </x:row>
     <x:row r="33" spans="1:87">
-      <x:c r="A33" s="84"/>
-      <x:c r="B33" s="78"/>
-      <x:c r="C33" s="76"/>
+      <x:c r="A33" s="85"/>
+      <x:c r="B33" s="79"/>
+      <x:c r="C33" s="77"/>
       <x:c r="D33" s="37" t="s">
-        <x:v>108</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="E33" s="37"/>
       <x:c r="F33" s="37"/>
@@ -4789,13 +4806,13 @@
       <x:c r="CI33" s="29"/>
     </x:row>
     <x:row r="34" spans="1:87" s="1" customFormat="1">
-      <x:c r="A34" s="83"/>
-      <x:c r="B34" s="82"/>
-      <x:c r="C34" s="75" t="s">
-        <x:v>158</x:v>
+      <x:c r="A34" s="84"/>
+      <x:c r="B34" s="83"/>
+      <x:c r="C34" s="76" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="D34" s="37" t="s">
-        <x:v>155</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E34" s="37"/>
       <x:c r="F34" s="37"/>
@@ -4882,11 +4899,11 @@
       <x:c r="CI34" s="29"/>
     </x:row>
     <x:row r="35" spans="1:87" s="1" customFormat="1">
-      <x:c r="A35" s="84"/>
-      <x:c r="B35" s="78"/>
-      <x:c r="C35" s="81"/>
+      <x:c r="A35" s="85"/>
+      <x:c r="B35" s="79"/>
+      <x:c r="C35" s="82"/>
       <x:c r="D35" s="37" t="s">
-        <x:v>200</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="E35" s="37"/>
       <x:c r="F35" s="37"/>
@@ -4973,11 +4990,11 @@
       <x:c r="CI35" s="29"/>
     </x:row>
     <x:row r="36" spans="1:87" s="1" customFormat="1">
-      <x:c r="A36" s="84"/>
-      <x:c r="B36" s="78"/>
-      <x:c r="C36" s="81"/>
+      <x:c r="A36" s="85"/>
+      <x:c r="B36" s="79"/>
+      <x:c r="C36" s="82"/>
       <x:c r="D36" s="37" t="s">
-        <x:v>189</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="E36" s="37"/>
       <x:c r="F36" s="37"/>
@@ -5064,11 +5081,11 @@
       <x:c r="CI36" s="29"/>
     </x:row>
     <x:row r="37" spans="1:87" s="1" customFormat="1">
-      <x:c r="A37" s="84"/>
-      <x:c r="B37" s="78"/>
-      <x:c r="C37" s="81"/>
+      <x:c r="A37" s="85"/>
+      <x:c r="B37" s="79"/>
+      <x:c r="C37" s="82"/>
       <x:c r="D37" s="37" t="s">
-        <x:v>211</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="E37" s="37"/>
       <x:c r="F37" s="37"/>
@@ -5155,11 +5172,11 @@
       <x:c r="CI37" s="29"/>
     </x:row>
     <x:row r="38" spans="1:87" s="1" customFormat="1">
-      <x:c r="A38" s="84"/>
-      <x:c r="B38" s="78"/>
-      <x:c r="C38" s="81"/>
+      <x:c r="A38" s="85"/>
+      <x:c r="B38" s="79"/>
+      <x:c r="C38" s="82"/>
       <x:c r="D38" s="37" t="s">
-        <x:v>122</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="E38" s="37"/>
       <x:c r="F38" s="37"/>
@@ -5246,11 +5263,11 @@
       <x:c r="CI38" s="29"/>
     </x:row>
     <x:row r="39" spans="1:87" s="1" customFormat="1">
-      <x:c r="A39" s="83"/>
-      <x:c r="B39" s="82"/>
-      <x:c r="C39" s="76"/>
+      <x:c r="A39" s="84"/>
+      <x:c r="B39" s="83"/>
+      <x:c r="C39" s="77"/>
       <x:c r="D39" s="37" t="s">
-        <x:v>142</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E39" s="37"/>
       <x:c r="F39" s="37"/>
@@ -5337,12 +5354,12 @@
       <x:c r="CI39" s="29"/>
     </x:row>
     <x:row r="40" spans="1:87">
-      <x:c r="A40" s="84"/>
-      <x:c r="B40" s="82" t="s">
-        <x:v>208</x:v>
+      <x:c r="A40" s="85"/>
+      <x:c r="B40" s="83" t="s">
+        <x:v>216</x:v>
       </x:c>
       <x:c r="C40" s="37" t="s">
-        <x:v>202</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="D40" s="37"/>
       <x:c r="E40" s="37"/>
@@ -5430,10 +5447,10 @@
       <x:c r="CI40" s="29"/>
     </x:row>
     <x:row r="41" spans="1:87">
-      <x:c r="A41" s="84"/>
-      <x:c r="B41" s="78"/>
+      <x:c r="A41" s="85"/>
+      <x:c r="B41" s="79"/>
       <x:c r="C41" s="37" t="s">
-        <x:v>143</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D41" s="37"/>
       <x:c r="E41" s="37"/>
@@ -5521,10 +5538,10 @@
       <x:c r="CI41" s="29"/>
     </x:row>
     <x:row r="42" spans="1:87">
-      <x:c r="A42" s="84"/>
-      <x:c r="B42" s="78"/>
+      <x:c r="A42" s="85"/>
+      <x:c r="B42" s="79"/>
       <x:c r="C42" s="37" t="s">
-        <x:v>145</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D42" s="37"/>
       <x:c r="E42" s="37"/>
@@ -5612,10 +5629,10 @@
       <x:c r="CI42" s="29"/>
     </x:row>
     <x:row r="43" spans="1:87">
-      <x:c r="A43" s="84"/>
-      <x:c r="B43" s="78"/>
+      <x:c r="A43" s="85"/>
+      <x:c r="B43" s="79"/>
       <x:c r="C43" s="37" t="s">
-        <x:v>126</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="D43" s="37"/>
       <x:c r="E43" s="37"/>
@@ -5703,10 +5720,10 @@
       <x:c r="CI43" s="29"/>
     </x:row>
     <x:row r="44" spans="1:87">
-      <x:c r="A44" s="84"/>
-      <x:c r="B44" s="78"/>
+      <x:c r="A44" s="85"/>
+      <x:c r="B44" s="79"/>
       <x:c r="C44" s="37" t="s">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="D44" s="37"/>
       <x:c r="E44" s="37"/>
@@ -5794,10 +5811,10 @@
       <x:c r="CI44" s="29"/>
     </x:row>
     <x:row r="45" spans="1:87">
-      <x:c r="A45" s="84"/>
-      <x:c r="B45" s="79"/>
+      <x:c r="A45" s="85"/>
+      <x:c r="B45" s="80"/>
       <x:c r="C45" s="37" t="s">
-        <x:v>123</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D45" s="37"/>
       <x:c r="E45" s="37"/>
@@ -5885,12 +5902,12 @@
       <x:c r="CI45" s="29"/>
     </x:row>
     <x:row r="46" spans="1:87">
-      <x:c r="A46" s="84"/>
-      <x:c r="B46" s="82" t="s">
+      <x:c r="A46" s="85"/>
+      <x:c r="B46" s="83" t="s">
         <x:v>195</x:v>
       </x:c>
       <x:c r="C46" s="37" t="s">
-        <x:v>205</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="D46" s="37"/>
       <x:c r="E46" s="37"/>
@@ -5978,10 +5995,10 @@
       <x:c r="CI46" s="29"/>
     </x:row>
     <x:row r="47" spans="1:87">
-      <x:c r="A47" s="84"/>
-      <x:c r="B47" s="78"/>
+      <x:c r="A47" s="85"/>
+      <x:c r="B47" s="79"/>
       <x:c r="C47" s="37" t="s">
-        <x:v>169</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="D47" s="37"/>
       <x:c r="E47" s="37"/>
@@ -6069,10 +6086,10 @@
       <x:c r="CI47" s="29"/>
     </x:row>
     <x:row r="48" spans="1:87">
-      <x:c r="A48" s="84"/>
-      <x:c r="B48" s="78"/>
+      <x:c r="A48" s="85"/>
+      <x:c r="B48" s="79"/>
       <x:c r="C48" s="37" t="s">
-        <x:v>84</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D48" s="37"/>
       <x:c r="E48" s="37"/>
@@ -6160,10 +6177,10 @@
       <x:c r="CI48" s="29"/>
     </x:row>
     <x:row r="49" spans="1:87">
-      <x:c r="A49" s="84"/>
-      <x:c r="B49" s="79"/>
+      <x:c r="A49" s="85"/>
+      <x:c r="B49" s="80"/>
       <x:c r="C49" s="37" t="s">
-        <x:v>110</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D49" s="37"/>
       <x:c r="E49" s="37"/>
@@ -6251,15 +6268,15 @@
       <x:c r="CI49" s="29"/>
     </x:row>
     <x:row r="50" spans="1:87">
-      <x:c r="A50" s="84"/>
-      <x:c r="B50" s="82" t="s">
-        <x:v>152</x:v>
-      </x:c>
-      <x:c r="C50" s="75" t="s">
-        <x:v>72</x:v>
+      <x:c r="A50" s="85"/>
+      <x:c r="B50" s="83" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C50" s="76" t="s">
+        <x:v>154</x:v>
       </x:c>
       <x:c r="D50" s="37" t="s">
-        <x:v>133</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E50" s="37"/>
       <x:c r="F50" s="37"/>
@@ -6346,11 +6363,11 @@
       <x:c r="CI50" s="29"/>
     </x:row>
     <x:row r="51" spans="1:87">
-      <x:c r="A51" s="84"/>
-      <x:c r="B51" s="78"/>
-      <x:c r="C51" s="76"/>
+      <x:c r="A51" s="85"/>
+      <x:c r="B51" s="79"/>
+      <x:c r="C51" s="77"/>
       <x:c r="D51" s="37" t="s">
-        <x:v>112</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E51" s="37"/>
       <x:c r="F51" s="37"/>
@@ -6437,13 +6454,13 @@
       <x:c r="CI51" s="29"/>
     </x:row>
     <x:row r="52" spans="1:87">
-      <x:c r="A52" s="84"/>
-      <x:c r="B52" s="78"/>
-      <x:c r="C52" s="75" t="s">
-        <x:v>171</x:v>
+      <x:c r="A52" s="85"/>
+      <x:c r="B52" s="79"/>
+      <x:c r="C52" s="76" t="s">
+        <x:v>173</x:v>
       </x:c>
       <x:c r="D52" s="37" t="s">
-        <x:v>79</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="E52" s="37"/>
       <x:c r="F52" s="37"/>
@@ -6530,11 +6547,11 @@
       <x:c r="CI52" s="29"/>
     </x:row>
     <x:row r="53" spans="1:87">
-      <x:c r="A53" s="84"/>
-      <x:c r="B53" s="78"/>
-      <x:c r="C53" s="76"/>
+      <x:c r="A53" s="85"/>
+      <x:c r="B53" s="79"/>
+      <x:c r="C53" s="77"/>
       <x:c r="D53" s="37" t="s">
-        <x:v>76</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="E53" s="37"/>
       <x:c r="F53" s="37"/>
@@ -6621,13 +6638,13 @@
       <x:c r="CI53" s="29"/>
     </x:row>
     <x:row r="54" spans="1:87">
-      <x:c r="A54" s="84"/>
-      <x:c r="B54" s="78"/>
-      <x:c r="C54" s="75" t="s">
-        <x:v>59</x:v>
+      <x:c r="A54" s="85"/>
+      <x:c r="B54" s="79"/>
+      <x:c r="C54" s="76" t="s">
+        <x:v>128</x:v>
       </x:c>
       <x:c r="D54" s="37" t="s">
-        <x:v>70</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E54" s="37"/>
       <x:c r="F54" s="37"/>
@@ -6714,11 +6731,11 @@
       <x:c r="CI54" s="29"/>
     </x:row>
     <x:row r="55" spans="1:87">
-      <x:c r="A55" s="84"/>
-      <x:c r="B55" s="78"/>
-      <x:c r="C55" s="81"/>
+      <x:c r="A55" s="85"/>
+      <x:c r="B55" s="79"/>
+      <x:c r="C55" s="82"/>
       <x:c r="D55" s="37" t="s">
-        <x:v>61</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E55" s="37"/>
       <x:c r="F55" s="37"/>
@@ -6805,11 +6822,11 @@
       <x:c r="CI55" s="29"/>
     </x:row>
     <x:row r="56" spans="1:87">
-      <x:c r="A56" s="84"/>
-      <x:c r="B56" s="78"/>
-      <x:c r="C56" s="76"/>
+      <x:c r="A56" s="85"/>
+      <x:c r="B56" s="79"/>
+      <x:c r="C56" s="77"/>
       <x:c r="D56" s="37" t="s">
-        <x:v>235</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="E56" s="37"/>
       <x:c r="F56" s="37"/>
@@ -6896,13 +6913,13 @@
       <x:c r="CI56" s="29"/>
     </x:row>
     <x:row r="57" spans="1:87">
-      <x:c r="A57" s="84"/>
-      <x:c r="B57" s="78"/>
-      <x:c r="C57" s="75" t="s">
-        <x:v>141</x:v>
+      <x:c r="A57" s="85"/>
+      <x:c r="B57" s="79"/>
+      <x:c r="C57" s="76" t="s">
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D57" s="37" t="s">
-        <x:v>232</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="E57" s="37"/>
       <x:c r="F57" s="37"/>
@@ -6989,11 +7006,11 @@
       <x:c r="CI57" s="29"/>
     </x:row>
     <x:row r="58" spans="1:87">
-      <x:c r="A58" s="84"/>
-      <x:c r="B58" s="78"/>
-      <x:c r="C58" s="76"/>
+      <x:c r="A58" s="85"/>
+      <x:c r="B58" s="79"/>
+      <x:c r="C58" s="77"/>
       <x:c r="D58" s="37" t="s">
-        <x:v>82</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E58" s="37"/>
       <x:c r="F58" s="37"/>
@@ -7080,13 +7097,13 @@
       <x:c r="CI58" s="29"/>
     </x:row>
     <x:row r="59" spans="1:87">
-      <x:c r="A59" s="84"/>
-      <x:c r="B59" s="78"/>
-      <x:c r="C59" s="75" t="s">
-        <x:v>80</x:v>
+      <x:c r="A59" s="85"/>
+      <x:c r="B59" s="79"/>
+      <x:c r="C59" s="76" t="s">
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D59" s="37" t="s">
-        <x:v>233</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="E59" s="37"/>
       <x:c r="F59" s="37"/>
@@ -7173,11 +7190,11 @@
       <x:c r="CI59" s="29"/>
     </x:row>
     <x:row r="60" spans="1:87">
-      <x:c r="A60" s="84"/>
-      <x:c r="B60" s="78"/>
-      <x:c r="C60" s="76"/>
+      <x:c r="A60" s="85"/>
+      <x:c r="B60" s="79"/>
+      <x:c r="C60" s="77"/>
       <x:c r="D60" s="37" t="s">
-        <x:v>234</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="E60" s="37"/>
       <x:c r="F60" s="37"/>
@@ -7264,13 +7281,13 @@
       <x:c r="CI60" s="29"/>
     </x:row>
     <x:row r="61" spans="1:87">
-      <x:c r="A61" s="84"/>
-      <x:c r="B61" s="78"/>
-      <x:c r="C61" s="75" t="s">
-        <x:v>119</x:v>
+      <x:c r="A61" s="85"/>
+      <x:c r="B61" s="79"/>
+      <x:c r="C61" s="76" t="s">
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D61" s="37" t="s">
-        <x:v>170</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="E61" s="37"/>
       <x:c r="F61" s="37"/>
@@ -7357,11 +7374,11 @@
       <x:c r="CI61" s="29"/>
     </x:row>
     <x:row r="62" spans="1:87">
-      <x:c r="A62" s="85"/>
-      <x:c r="B62" s="79"/>
-      <x:c r="C62" s="76"/>
+      <x:c r="A62" s="86"/>
+      <x:c r="B62" s="80"/>
+      <x:c r="C62" s="77"/>
       <x:c r="D62" s="37" t="s">
-        <x:v>134</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E62" s="37"/>
       <x:c r="F62" s="37"/>
@@ -9387,7 +9404,7 @@
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31:D31"/>
+      <x:selection pane="bottomLeft" activeCell="G28" activeCellId="0" sqref="G28:G28"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
@@ -9403,288 +9420,288 @@
   <x:sheetData>
     <x:row r="1" spans="1:8" ht="17.149999999999999">
       <x:c r="A1" s="32" t="s">
-        <x:v>64</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>154</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="D1" s="34" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="E1" s="34" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="F1" s="34" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="D1" s="34" t="s">
-        <x:v>151</x:v>
-      </x:c>
-      <x:c r="E1" s="34" t="s">
-        <x:v>124</x:v>
-      </x:c>
-      <x:c r="F1" s="34" t="s">
-        <x:v>87</x:v>
-      </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>206</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="H1" s="35" t="s">
-        <x:v>197</x:v>
+        <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8" ht="16.75" customHeight="1">
-      <x:c r="A2" s="83" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="B2" s="77" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="C2" s="90" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="D2" s="88" t="s">
-        <x:v>113</x:v>
+      <x:c r="A2" s="84" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B2" s="78" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="C2" s="91" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="D2" s="89" t="s">
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E2" s="61" t="s">
-        <x:v>46</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F2" s="61"/>
       <x:c r="G2" s="61"/>
       <x:c r="H2" s="61" t="s">
-        <x:v>240</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
-      <x:c r="A3" s="84"/>
-      <x:c r="B3" s="78"/>
-      <x:c r="C3" s="91"/>
-      <x:c r="D3" s="89"/>
+      <x:c r="A3" s="85"/>
+      <x:c r="B3" s="79"/>
+      <x:c r="C3" s="92"/>
+      <x:c r="D3" s="90"/>
       <x:c r="E3" s="62" t="s">
-        <x:v>139</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F3" s="62"/>
       <x:c r="G3" s="62"/>
       <x:c r="H3" s="62" t="s">
-        <x:v>136</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
-      <x:c r="A4" s="84"/>
-      <x:c r="B4" s="78"/>
-      <x:c r="C4" s="91"/>
-      <x:c r="D4" s="87"/>
+      <x:c r="A4" s="85"/>
+      <x:c r="B4" s="79"/>
+      <x:c r="C4" s="92"/>
+      <x:c r="D4" s="88"/>
       <x:c r="E4" s="62" t="s">
-        <x:v>105</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F4" s="62"/>
       <x:c r="G4" s="62"/>
       <x:c r="H4" s="62" t="s">
-        <x:v>241</x:v>
+        <x:v>219</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
-      <x:c r="A5" s="84"/>
-      <x:c r="B5" s="78"/>
-      <x:c r="C5" s="91"/>
-      <x:c r="D5" s="86" t="s">
-        <x:v>129</x:v>
+      <x:c r="A5" s="85"/>
+      <x:c r="B5" s="79"/>
+      <x:c r="C5" s="92"/>
+      <x:c r="D5" s="87" t="s">
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E5" s="63" t="s">
-        <x:v>144</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F5" s="62"/>
       <x:c r="G5" s="62"/>
       <x:c r="H5" s="62" t="s">
-        <x:v>215</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
-      <x:c r="A6" s="84"/>
-      <x:c r="B6" s="78"/>
-      <x:c r="C6" s="92"/>
-      <x:c r="D6" s="87"/>
+      <x:c r="A6" s="85"/>
+      <x:c r="B6" s="79"/>
+      <x:c r="C6" s="93"/>
+      <x:c r="D6" s="88"/>
       <x:c r="E6" s="63" t="s">
-        <x:v>188</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F6" s="62"/>
       <x:c r="G6" s="62"/>
       <x:c r="H6" s="62" t="s">
-        <x:v>38</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
-      <x:c r="A7" s="84"/>
-      <x:c r="B7" s="78"/>
-      <x:c r="C7" s="94" t="s">
-        <x:v>153</x:v>
-      </x:c>
-      <x:c r="D7" s="86" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="E7" s="86" t="s">
-        <x:v>113</x:v>
+      <x:c r="A7" s="85"/>
+      <x:c r="B7" s="79"/>
+      <x:c r="C7" s="95" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D7" s="87" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E7" s="87" t="s">
+        <x:v>102</x:v>
       </x:c>
       <x:c r="F7" s="62" t="s">
-        <x:v>182</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="G7" s="62"/>
       <x:c r="H7" s="62"/>
     </x:row>
     <x:row r="8" spans="1:8">
-      <x:c r="A8" s="84"/>
-      <x:c r="B8" s="78"/>
-      <x:c r="C8" s="91"/>
-      <x:c r="D8" s="89"/>
-      <x:c r="E8" s="89"/>
+      <x:c r="A8" s="85"/>
+      <x:c r="B8" s="79"/>
+      <x:c r="C8" s="92"/>
+      <x:c r="D8" s="90"/>
+      <x:c r="E8" s="90"/>
       <x:c r="F8" s="62" t="s">
-        <x:v>49</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="G8" s="62"/>
       <x:c r="H8" s="62"/>
     </x:row>
     <x:row r="9" spans="1:8">
-      <x:c r="A9" s="84"/>
-      <x:c r="B9" s="78"/>
-      <x:c r="C9" s="91"/>
-      <x:c r="D9" s="89"/>
-      <x:c r="E9" s="89"/>
+      <x:c r="A9" s="85"/>
+      <x:c r="B9" s="79"/>
+      <x:c r="C9" s="92"/>
+      <x:c r="D9" s="90"/>
+      <x:c r="E9" s="90"/>
       <x:c r="F9" s="62" t="s">
-        <x:v>137</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G9" s="62"/>
       <x:c r="H9" s="62"/>
     </x:row>
     <x:row r="10" spans="1:8">
-      <x:c r="A10" s="84"/>
-      <x:c r="B10" s="78"/>
-      <x:c r="C10" s="91"/>
-      <x:c r="D10" s="89"/>
-      <x:c r="E10" s="89"/>
+      <x:c r="A10" s="85"/>
+      <x:c r="B10" s="79"/>
+      <x:c r="C10" s="92"/>
+      <x:c r="D10" s="90"/>
+      <x:c r="E10" s="90"/>
       <x:c r="F10" s="62" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G10" s="62"/>
       <x:c r="H10" s="62"/>
     </x:row>
     <x:row r="11" spans="1:8" ht="16.75">
-      <x:c r="A11" s="84"/>
-      <x:c r="B11" s="95"/>
-      <x:c r="C11" s="96"/>
-      <x:c r="D11" s="93"/>
-      <x:c r="E11" s="93"/>
+      <x:c r="A11" s="85"/>
+      <x:c r="B11" s="96"/>
+      <x:c r="C11" s="97"/>
+      <x:c r="D11" s="94"/>
+      <x:c r="E11" s="94"/>
       <x:c r="F11" s="65" t="s">
-        <x:v>128</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G11" s="65"/>
       <x:c r="H11" s="65"/>
     </x:row>
     <x:row r="12" spans="1:8">
-      <x:c r="A12" s="84"/>
-      <x:c r="B12" s="78" t="s">
-        <x:v>203</x:v>
-      </x:c>
-      <x:c r="C12" s="91" t="s">
-        <x:v>147</x:v>
+      <x:c r="A12" s="85"/>
+      <x:c r="B12" s="79" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="C12" s="92" t="s">
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D12" s="61" t="s">
-        <x:v>209</x:v>
-      </x:c>
-      <x:c r="E12" s="89" t="s">
-        <x:v>239</x:v>
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="E12" s="90" t="s">
+        <x:v>227</x:v>
       </x:c>
       <x:c r="F12" s="61"/>
       <x:c r="G12" s="61"/>
       <x:c r="H12" s="61"/>
     </x:row>
     <x:row r="13" spans="1:8">
-      <x:c r="A13" s="84"/>
-      <x:c r="B13" s="78"/>
-      <x:c r="C13" s="91"/>
+      <x:c r="A13" s="85"/>
+      <x:c r="B13" s="79"/>
+      <x:c r="C13" s="92"/>
       <x:c r="D13" s="63" t="s">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="E13" s="89"/>
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="E13" s="90"/>
       <x:c r="F13" s="62"/>
       <x:c r="G13" s="62"/>
       <x:c r="H13" s="62"/>
     </x:row>
     <x:row r="14" spans="1:8">
-      <x:c r="A14" s="84"/>
-      <x:c r="B14" s="78"/>
-      <x:c r="C14" s="91"/>
+      <x:c r="A14" s="85"/>
+      <x:c r="B14" s="79"/>
+      <x:c r="C14" s="92"/>
       <x:c r="D14" s="63" t="s">
-        <x:v>120</x:v>
-      </x:c>
-      <x:c r="E14" s="89"/>
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="E14" s="90"/>
       <x:c r="F14" s="62"/>
       <x:c r="G14" s="62"/>
       <x:c r="H14" s="62"/>
     </x:row>
     <x:row r="15" spans="1:8">
-      <x:c r="A15" s="84"/>
-      <x:c r="B15" s="78"/>
-      <x:c r="C15" s="92"/>
+      <x:c r="A15" s="85"/>
+      <x:c r="B15" s="79"/>
+      <x:c r="C15" s="93"/>
       <x:c r="D15" s="63" t="s">
-        <x:v>142</x:v>
-      </x:c>
-      <x:c r="E15" s="87"/>
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="E15" s="88"/>
       <x:c r="F15" s="62"/>
       <x:c r="G15" s="62"/>
       <x:c r="H15" s="62"/>
     </x:row>
     <x:row r="16" spans="1:8">
-      <x:c r="A16" s="84"/>
-      <x:c r="B16" s="78"/>
-      <x:c r="C16" s="94" t="s">
-        <x:v>89</x:v>
+      <x:c r="A16" s="85"/>
+      <x:c r="B16" s="79"/>
+      <x:c r="C16" s="95" t="s">
+        <x:v>111</x:v>
       </x:c>
       <x:c r="D16" s="63" t="s">
-        <x:v>159</x:v>
-      </x:c>
-      <x:c r="E16" s="86" t="s">
-        <x:v>72</x:v>
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="E16" s="87" t="s">
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F16" s="62" t="s">
-        <x:v>133</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G16" s="62"/>
-      <x:c r="H16" s="86" t="s">
-        <x:v>246</x:v>
+      <x:c r="H16" s="87" t="s">
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
-      <x:c r="A17" s="84"/>
-      <x:c r="B17" s="78"/>
-      <x:c r="C17" s="92"/>
+      <x:c r="A17" s="85"/>
+      <x:c r="B17" s="79"/>
+      <x:c r="C17" s="93"/>
       <x:c r="D17" s="62" t="s">
-        <x:v>194</x:v>
-      </x:c>
-      <x:c r="E17" s="87"/>
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="E17" s="88"/>
       <x:c r="F17" s="62" t="s">
-        <x:v>112</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="G17" s="62"/>
-      <x:c r="H17" s="87"/>
+      <x:c r="H17" s="88"/>
     </x:row>
     <x:row r="18" spans="1:8" ht="16.75">
-      <x:c r="A18" s="84"/>
-      <x:c r="B18" s="95"/>
+      <x:c r="A18" s="85"/>
+      <x:c r="B18" s="96"/>
       <x:c r="C18" s="66" t="s">
-        <x:v>99</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D18" s="65"/>
       <x:c r="E18" s="65"/>
       <x:c r="F18" s="65"/>
       <x:c r="G18" s="65"/>
       <x:c r="H18" s="65" t="s">
-        <x:v>236</x:v>
+        <x:v>223</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
-      <x:c r="A19" s="84"/>
-      <x:c r="B19" s="78" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="C19" s="91" t="s">
-        <x:v>208</x:v>
+      <x:c r="A19" s="85"/>
+      <x:c r="B19" s="79" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="C19" s="92" t="s">
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D19" s="61" t="s">
-        <x:v>202</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="E19" s="61"/>
       <x:c r="F19" s="61"/>
@@ -9692,11 +9709,11 @@
       <x:c r="H19" s="61"/>
     </x:row>
     <x:row r="20" spans="1:8">
-      <x:c r="A20" s="84"/>
-      <x:c r="B20" s="78"/>
-      <x:c r="C20" s="91"/>
+      <x:c r="A20" s="85"/>
+      <x:c r="B20" s="79"/>
+      <x:c r="C20" s="92"/>
       <x:c r="D20" s="62" t="s">
-        <x:v>213</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="E20" s="62"/>
       <x:c r="F20" s="62"/>
@@ -9704,11 +9721,11 @@
       <x:c r="H20" s="62"/>
     </x:row>
     <x:row r="21" spans="1:8">
-      <x:c r="A21" s="84"/>
-      <x:c r="B21" s="78"/>
-      <x:c r="C21" s="91"/>
+      <x:c r="A21" s="85"/>
+      <x:c r="B21" s="79"/>
+      <x:c r="C21" s="92"/>
       <x:c r="D21" s="62" t="s">
-        <x:v>145</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E21" s="62"/>
       <x:c r="F21" s="62"/>
@@ -9716,11 +9733,11 @@
       <x:c r="H21" s="62"/>
     </x:row>
     <x:row r="22" spans="1:8">
-      <x:c r="A22" s="84"/>
-      <x:c r="B22" s="78"/>
-      <x:c r="C22" s="91"/>
+      <x:c r="A22" s="85"/>
+      <x:c r="B22" s="79"/>
+      <x:c r="C22" s="92"/>
       <x:c r="D22" s="62" t="s">
-        <x:v>179</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="E22" s="62"/>
       <x:c r="F22" s="62"/>
@@ -9728,11 +9745,11 @@
       <x:c r="H22" s="62"/>
     </x:row>
     <x:row r="23" spans="1:8">
-      <x:c r="A23" s="84"/>
-      <x:c r="B23" s="78"/>
-      <x:c r="C23" s="92"/>
+      <x:c r="A23" s="85"/>
+      <x:c r="B23" s="79"/>
+      <x:c r="C23" s="93"/>
       <x:c r="D23" s="62" t="s">
-        <x:v>123</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E23" s="62"/>
       <x:c r="F23" s="62"/>
@@ -9740,90 +9757,90 @@
       <x:c r="H23" s="62"/>
     </x:row>
     <x:row r="24" spans="1:8">
-      <x:c r="A24" s="83"/>
-      <x:c r="B24" s="82"/>
-      <x:c r="C24" s="94" t="s">
-        <x:v>126</x:v>
-      </x:c>
-      <x:c r="D24" s="86" t="s">
-        <x:v>177</x:v>
+      <x:c r="A24" s="84"/>
+      <x:c r="B24" s="83"/>
+      <x:c r="C24" s="95" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="D24" s="87" t="s">
+        <x:v>184</x:v>
       </x:c>
       <x:c r="E24" s="62" t="s">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F24" s="62"/>
       <x:c r="G24" s="62"/>
       <x:c r="H24" s="62"/>
     </x:row>
     <x:row r="25" spans="1:8">
-      <x:c r="A25" s="84"/>
-      <x:c r="B25" s="78"/>
-      <x:c r="C25" s="91"/>
-      <x:c r="D25" s="87"/>
+      <x:c r="A25" s="85"/>
+      <x:c r="B25" s="79"/>
+      <x:c r="C25" s="92"/>
+      <x:c r="D25" s="88"/>
       <x:c r="E25" s="62" t="s">
-        <x:v>196</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F25" s="62"/>
       <x:c r="G25" s="62"/>
       <x:c r="H25" s="62"/>
     </x:row>
     <x:row r="26" spans="1:8">
-      <x:c r="A26" s="83"/>
-      <x:c r="B26" s="82"/>
-      <x:c r="C26" s="91"/>
-      <x:c r="D26" s="86" t="s">
-        <x:v>204</x:v>
+      <x:c r="A26" s="84"/>
+      <x:c r="B26" s="83"/>
+      <x:c r="C26" s="92"/>
+      <x:c r="D26" s="87" t="s">
+        <x:v>215</x:v>
       </x:c>
       <x:c r="E26" s="62" t="s">
-        <x:v>199</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F26" s="62"/>
       <x:c r="G26" s="62"/>
       <x:c r="H26" s="62"/>
     </x:row>
     <x:row r="27" spans="1:8">
-      <x:c r="A27" s="84"/>
-      <x:c r="B27" s="78"/>
-      <x:c r="C27" s="91"/>
-      <x:c r="D27" s="89"/>
+      <x:c r="A27" s="85"/>
+      <x:c r="B27" s="79"/>
+      <x:c r="C27" s="92"/>
+      <x:c r="D27" s="90"/>
       <x:c r="E27" s="62" t="s">
-        <x:v>175</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F27" s="62"/>
       <x:c r="G27" s="62"/>
       <x:c r="H27" s="62"/>
     </x:row>
     <x:row r="28" spans="1:8">
-      <x:c r="A28" s="84"/>
-      <x:c r="B28" s="78"/>
-      <x:c r="C28" s="91"/>
-      <x:c r="D28" s="89"/>
+      <x:c r="A28" s="85"/>
+      <x:c r="B28" s="79"/>
+      <x:c r="C28" s="92"/>
+      <x:c r="D28" s="90"/>
       <x:c r="E28" s="62" t="s">
-        <x:v>180</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F28" s="62"/>
       <x:c r="G28" s="62"/>
       <x:c r="H28" s="62"/>
     </x:row>
     <x:row r="29" spans="1:8" ht="16.75">
-      <x:c r="A29" s="84"/>
-      <x:c r="B29" s="95"/>
-      <x:c r="C29" s="96"/>
-      <x:c r="D29" s="93"/>
+      <x:c r="A29" s="85"/>
+      <x:c r="B29" s="96"/>
+      <x:c r="C29" s="97"/>
+      <x:c r="D29" s="94"/>
       <x:c r="E29" s="65" t="s">
-        <x:v>191</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F29" s="65"/>
       <x:c r="G29" s="65"/>
       <x:c r="H29" s="65"/>
     </x:row>
     <x:row r="30" spans="1:8">
-      <x:c r="A30" s="84"/>
-      <x:c r="B30" s="78" t="s">
+      <x:c r="A30" s="85"/>
+      <x:c r="B30" s="79" t="s">
         <x:v>195</x:v>
       </x:c>
       <x:c r="C30" s="67" t="s">
-        <x:v>205</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="D30" s="61"/>
       <x:c r="E30" s="61"/>
@@ -9832,10 +9849,10 @@
       <x:c r="H30" s="61"/>
     </x:row>
     <x:row r="31" spans="1:8">
-      <x:c r="A31" s="84"/>
-      <x:c r="B31" s="78"/>
+      <x:c r="A31" s="85"/>
+      <x:c r="B31" s="79"/>
       <x:c r="C31" s="58" t="s">
-        <x:v>169</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="D31" s="62"/>
       <x:c r="E31" s="62"/>
@@ -9844,10 +9861,10 @@
       <x:c r="H31" s="62"/>
     </x:row>
     <x:row r="32" spans="1:8">
-      <x:c r="A32" s="84"/>
-      <x:c r="B32" s="78"/>
+      <x:c r="A32" s="85"/>
+      <x:c r="B32" s="79"/>
       <x:c r="C32" s="58" t="s">
-        <x:v>84</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D32" s="62"/>
       <x:c r="E32" s="62"/>
@@ -9856,10 +9873,10 @@
       <x:c r="H32" s="62"/>
     </x:row>
     <x:row r="33" spans="1:8" ht="16.75">
-      <x:c r="A33" s="84"/>
-      <x:c r="B33" s="95"/>
+      <x:c r="A33" s="85"/>
+      <x:c r="B33" s="96"/>
       <x:c r="C33" s="68" t="s">
-        <x:v>110</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D33" s="65"/>
       <x:c r="E33" s="65"/>
@@ -9868,12 +9885,12 @@
       <x:c r="H33" s="65"/>
     </x:row>
     <x:row r="34" spans="1:8">
-      <x:c r="A34" s="84"/>
-      <x:c r="B34" s="78" t="s">
-        <x:v>114</x:v>
+      <x:c r="A34" s="85"/>
+      <x:c r="B34" s="79" t="s">
+        <x:v>103</x:v>
       </x:c>
       <x:c r="C34" s="67" t="s">
-        <x:v>45</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D34" s="61"/>
       <x:c r="E34" s="61"/>
@@ -9882,13 +9899,13 @@
       <x:c r="H34" s="61"/>
     </x:row>
     <x:row r="35" spans="1:8">
-      <x:c r="A35" s="84"/>
-      <x:c r="B35" s="78"/>
-      <x:c r="C35" s="94" t="s">
-        <x:v>119</x:v>
+      <x:c r="A35" s="85"/>
+      <x:c r="B35" s="79"/>
+      <x:c r="C35" s="95" t="s">
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D35" s="62" t="s">
-        <x:v>170</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="E35" s="62"/>
       <x:c r="F35" s="62"/>
@@ -9896,11 +9913,11 @@
       <x:c r="H35" s="62"/>
     </x:row>
     <x:row r="36" spans="1:8">
-      <x:c r="A36" s="84"/>
-      <x:c r="B36" s="78"/>
-      <x:c r="C36" s="91"/>
+      <x:c r="A36" s="85"/>
+      <x:c r="B36" s="79"/>
+      <x:c r="C36" s="92"/>
       <x:c r="D36" s="62" t="s">
-        <x:v>134</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E36" s="62"/>
       <x:c r="F36" s="62"/>
@@ -9908,11 +9925,11 @@
       <x:c r="H36" s="62"/>
     </x:row>
     <x:row r="37" spans="1:8" ht="16.75">
-      <x:c r="A37" s="84"/>
-      <x:c r="B37" s="95"/>
-      <x:c r="C37" s="96"/>
+      <x:c r="A37" s="85"/>
+      <x:c r="B37" s="96"/>
+      <x:c r="C37" s="97"/>
       <x:c r="D37" s="65" t="s">
-        <x:v>50</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="E37" s="65"/>
       <x:c r="F37" s="65"/>
@@ -9920,7 +9937,7 @@
       <x:c r="H37" s="65"/>
     </x:row>
     <x:row r="38" spans="1:8">
-      <x:c r="A38" s="84"/>
+      <x:c r="A38" s="85"/>
       <x:c r="B38" s="64"/>
       <x:c r="C38" s="67"/>
       <x:c r="D38" s="61"/>
@@ -9930,7 +9947,7 @@
       <x:c r="H38" s="61"/>
     </x:row>
     <x:row r="39" spans="1:8">
-      <x:c r="A39" s="84"/>
+      <x:c r="A39" s="85"/>
       <x:c r="B39" s="59"/>
       <x:c r="C39" s="60"/>
       <x:c r="D39" s="62"/>
@@ -9940,7 +9957,7 @@
       <x:c r="H39" s="62"/>
     </x:row>
     <x:row r="40" spans="1:8" ht="16.75">
-      <x:c r="A40" s="97"/>
+      <x:c r="A40" s="98"/>
       <x:c r="B40" s="47"/>
       <x:c r="C40" s="48"/>
       <x:c r="D40" s="48"/>
@@ -9992,7 +10009,7 @@
     <x:row r="45" spans="1:8">
       <x:c r="A45" s="44"/>
       <x:c r="B45" s="44"/>
-      <x:c r="C45" s="98"/>
+      <x:c r="C45" s="99"/>
       <x:c r="D45" s="57"/>
       <x:c r="E45" s="46"/>
       <x:c r="F45" s="46"/>
@@ -10002,7 +10019,7 @@
     <x:row r="46" spans="1:8">
       <x:c r="A46" s="44"/>
       <x:c r="B46" s="44"/>
-      <x:c r="C46" s="98"/>
+      <x:c r="C46" s="99"/>
       <x:c r="D46" s="57"/>
       <x:c r="E46" s="46"/>
       <x:c r="F46" s="46"/>
@@ -10012,7 +10029,7 @@
     <x:row r="47" spans="1:8">
       <x:c r="A47" s="44"/>
       <x:c r="B47" s="44"/>
-      <x:c r="C47" s="98"/>
+      <x:c r="C47" s="99"/>
       <x:c r="D47" s="57"/>
       <x:c r="E47" s="46"/>
       <x:c r="F47" s="46"/>
@@ -10022,7 +10039,7 @@
     <x:row r="48" spans="1:8">
       <x:c r="A48" s="44"/>
       <x:c r="B48" s="44"/>
-      <x:c r="C48" s="98"/>
+      <x:c r="C48" s="99"/>
       <x:c r="D48" s="57"/>
       <x:c r="E48" s="46"/>
       <x:c r="F48" s="46"/>
@@ -10032,7 +10049,7 @@
     <x:row r="49" spans="1:8">
       <x:c r="A49" s="44"/>
       <x:c r="B49" s="44"/>
-      <x:c r="C49" s="98"/>
+      <x:c r="C49" s="99"/>
       <x:c r="D49" s="57"/>
       <x:c r="E49" s="46"/>
       <x:c r="F49" s="46"/>
@@ -10042,7 +10059,7 @@
     <x:row r="50" spans="1:8">
       <x:c r="A50" s="44"/>
       <x:c r="B50" s="44"/>
-      <x:c r="C50" s="98"/>
+      <x:c r="C50" s="99"/>
       <x:c r="D50" s="57"/>
       <x:c r="E50" s="46"/>
       <x:c r="F50" s="46"/>
@@ -10052,7 +10069,7 @@
     <x:row r="51" spans="1:8">
       <x:c r="A51" s="44"/>
       <x:c r="B51" s="44"/>
-      <x:c r="C51" s="98"/>
+      <x:c r="C51" s="99"/>
       <x:c r="D51" s="57"/>
       <x:c r="E51" s="46"/>
       <x:c r="F51" s="46"/>
@@ -10062,7 +10079,7 @@
     <x:row r="52" spans="1:8">
       <x:c r="A52" s="44"/>
       <x:c r="B52" s="44"/>
-      <x:c r="C52" s="98"/>
+      <x:c r="C52" s="99"/>
       <x:c r="D52" s="57"/>
       <x:c r="E52" s="46"/>
       <x:c r="F52" s="46"/>
@@ -10072,7 +10089,7 @@
     <x:row r="53" spans="1:8">
       <x:c r="A53" s="44"/>
       <x:c r="B53" s="44"/>
-      <x:c r="C53" s="98"/>
+      <x:c r="C53" s="99"/>
       <x:c r="D53" s="57"/>
       <x:c r="E53" s="46"/>
       <x:c r="F53" s="46"/>
@@ -10082,7 +10099,7 @@
     <x:row r="54" spans="1:8">
       <x:c r="A54" s="44"/>
       <x:c r="B54" s="44"/>
-      <x:c r="C54" s="98"/>
+      <x:c r="C54" s="99"/>
       <x:c r="D54" s="57"/>
       <x:c r="E54" s="46"/>
       <x:c r="F54" s="46"/>
@@ -10092,7 +10109,7 @@
     <x:row r="55" spans="1:8">
       <x:c r="A55" s="44"/>
       <x:c r="B55" s="44"/>
-      <x:c r="C55" s="98"/>
+      <x:c r="C55" s="99"/>
       <x:c r="D55" s="57"/>
       <x:c r="E55" s="46"/>
       <x:c r="F55" s="46"/>
@@ -10102,7 +10119,7 @@
     <x:row r="56" spans="1:8">
       <x:c r="A56" s="44"/>
       <x:c r="B56" s="44"/>
-      <x:c r="C56" s="98"/>
+      <x:c r="C56" s="99"/>
       <x:c r="D56" s="57"/>
       <x:c r="E56" s="46"/>
       <x:c r="F56" s="46"/>
@@ -10112,7 +10129,7 @@
     <x:row r="57" spans="1:8">
       <x:c r="A57" s="44"/>
       <x:c r="B57" s="44"/>
-      <x:c r="C57" s="98"/>
+      <x:c r="C57" s="99"/>
       <x:c r="D57" s="57"/>
       <x:c r="E57" s="46"/>
       <x:c r="F57" s="46"/>
@@ -10236,388 +10253,388 @@
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="49"/>
       <x:c r="B2" s="36" t="s">
-        <x:v>168</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="C2" s="36" t="s">
-        <x:v>66</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D2" s="36" t="s">
-        <x:v>83</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="E2" s="36" t="s">
         <x:v>109</x:v>
       </x:c>
       <x:c r="F2" s="36" t="s">
-        <x:v>197</x:v>
+        <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" ht="16.75">
       <x:c r="A3" s="49"/>
-      <x:c r="B3" s="77" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="C3" s="80" t="s">
-        <x:v>135</x:v>
-      </x:c>
-      <x:c r="D3" s="80" t="s">
-        <x:v>138</x:v>
+      <x:c r="B3" s="78" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C3" s="81" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D3" s="81" t="s">
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E3" s="50" t="s">
-        <x:v>26</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F3" s="69"/>
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="A4" s="49"/>
-      <x:c r="B4" s="78"/>
-      <x:c r="C4" s="81"/>
-      <x:c r="D4" s="81"/>
+      <x:c r="B4" s="79"/>
+      <x:c r="C4" s="82"/>
+      <x:c r="D4" s="82"/>
       <x:c r="E4" s="51" t="s">
-        <x:v>244</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F4" s="70"/>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="49"/>
-      <x:c r="B5" s="78"/>
-      <x:c r="C5" s="81"/>
-      <x:c r="D5" s="81"/>
+      <x:c r="B5" s="79"/>
+      <x:c r="C5" s="82"/>
+      <x:c r="D5" s="82"/>
       <x:c r="E5" s="51" t="s">
-        <x:v>29</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="F5" s="70"/>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="49"/>
-      <x:c r="B6" s="78"/>
-      <x:c r="C6" s="81"/>
-      <x:c r="D6" s="81"/>
+      <x:c r="B6" s="79"/>
+      <x:c r="C6" s="82"/>
+      <x:c r="D6" s="82"/>
       <x:c r="E6" s="51" t="s">
-        <x:v>5</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F6" s="70"/>
     </x:row>
     <x:row r="7" spans="1:6" ht="32.75">
       <x:c r="A7" s="49"/>
-      <x:c r="B7" s="78"/>
-      <x:c r="C7" s="81"/>
-      <x:c r="D7" s="76"/>
+      <x:c r="B7" s="79"/>
+      <x:c r="C7" s="82"/>
+      <x:c r="D7" s="77"/>
       <x:c r="E7" s="52" t="s">
-        <x:v>34</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F7" s="70"/>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="49"/>
-      <x:c r="B8" s="78"/>
-      <x:c r="C8" s="81"/>
-      <x:c r="D8" s="75" t="s">
-        <x:v>210</x:v>
+      <x:c r="B8" s="79"/>
+      <x:c r="C8" s="82"/>
+      <x:c r="D8" s="76" t="s">
+        <x:v>187</x:v>
       </x:c>
       <x:c r="E8" s="53" t="s">
-        <x:v>24</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F8" s="70"/>
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="A9" s="49"/>
-      <x:c r="B9" s="78"/>
-      <x:c r="C9" s="81"/>
-      <x:c r="D9" s="81"/>
+      <x:c r="B9" s="79"/>
+      <x:c r="C9" s="82"/>
+      <x:c r="D9" s="82"/>
       <x:c r="E9" s="51" t="s">
-        <x:v>228</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="F9" s="70"/>
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="A10" s="49"/>
-      <x:c r="B10" s="78"/>
-      <x:c r="C10" s="81"/>
-      <x:c r="D10" s="76"/>
+      <x:c r="B10" s="79"/>
+      <x:c r="C10" s="82"/>
+      <x:c r="D10" s="77"/>
       <x:c r="E10" s="54" t="s">
-        <x:v>231</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="F10" s="70"/>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="49"/>
-      <x:c r="B11" s="78"/>
-      <x:c r="C11" s="81"/>
-      <x:c r="D11" s="75" t="s">
-        <x:v>193</x:v>
+      <x:c r="B11" s="79"/>
+      <x:c r="C11" s="82"/>
+      <x:c r="D11" s="76" t="s">
+        <x:v>189</x:v>
       </x:c>
       <x:c r="E11" s="53" t="s">
-        <x:v>166</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F11" s="70"/>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="49"/>
-      <x:c r="B12" s="78"/>
-      <x:c r="C12" s="76"/>
-      <x:c r="D12" s="76"/>
+      <x:c r="B12" s="79"/>
+      <x:c r="C12" s="77"/>
+      <x:c r="D12" s="77"/>
       <x:c r="E12" s="54" t="s">
-        <x:v>6</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F12" s="70"/>
     </x:row>
     <x:row r="13" spans="1:6">
       <x:c r="A13" s="49"/>
-      <x:c r="B13" s="78"/>
-      <x:c r="C13" s="75" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="D13" s="75" t="s">
-        <x:v>208</x:v>
+      <x:c r="B13" s="79"/>
+      <x:c r="C13" s="76" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="D13" s="76" t="s">
+        <x:v>216</x:v>
       </x:c>
       <x:c r="E13" s="53" t="s">
-        <x:v>219</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F13" s="70"/>
     </x:row>
     <x:row r="14" spans="1:6">
       <x:c r="A14" s="49"/>
-      <x:c r="B14" s="78"/>
-      <x:c r="C14" s="81"/>
-      <x:c r="D14" s="81"/>
+      <x:c r="B14" s="79"/>
+      <x:c r="C14" s="82"/>
+      <x:c r="D14" s="82"/>
       <x:c r="E14" s="51" t="s">
-        <x:v>25</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F14" s="70"/>
     </x:row>
     <x:row r="15" spans="1:6">
       <x:c r="A15" s="49"/>
-      <x:c r="B15" s="78"/>
-      <x:c r="C15" s="81"/>
-      <x:c r="D15" s="81"/>
+      <x:c r="B15" s="79"/>
+      <x:c r="C15" s="82"/>
+      <x:c r="D15" s="82"/>
       <x:c r="E15" s="51" t="s">
-        <x:v>226</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="F15" s="70"/>
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="A16" s="49"/>
-      <x:c r="B16" s="78"/>
-      <x:c r="C16" s="81"/>
-      <x:c r="D16" s="76"/>
+      <x:c r="B16" s="79"/>
+      <x:c r="C16" s="82"/>
+      <x:c r="D16" s="77"/>
       <x:c r="E16" s="54" t="s">
-        <x:v>160</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F16" s="70"/>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="A17" s="49"/>
-      <x:c r="B17" s="78"/>
-      <x:c r="C17" s="81"/>
-      <x:c r="D17" s="75" t="s">
-        <x:v>181</x:v>
+      <x:c r="B17" s="79"/>
+      <x:c r="C17" s="82"/>
+      <x:c r="D17" s="76" t="s">
+        <x:v>193</x:v>
       </x:c>
       <x:c r="E17" s="53" t="s">
-        <x:v>221</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="F17" s="70"/>
     </x:row>
     <x:row r="18" spans="1:6" ht="32.75">
       <x:c r="A18" s="49"/>
-      <x:c r="B18" s="78"/>
-      <x:c r="C18" s="76"/>
-      <x:c r="D18" s="76"/>
+      <x:c r="B18" s="79"/>
+      <x:c r="C18" s="77"/>
+      <x:c r="D18" s="77"/>
       <x:c r="E18" s="52" t="s">
-        <x:v>33</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F18" s="70"/>
     </x:row>
     <x:row r="19" spans="1:6">
       <x:c r="A19" s="49"/>
-      <x:c r="B19" s="78"/>
-      <x:c r="C19" s="75" t="s">
-        <x:v>185</x:v>
-      </x:c>
-      <x:c r="D19" s="75" t="s">
-        <x:v>40</x:v>
+      <x:c r="B19" s="79"/>
+      <x:c r="C19" s="76" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="D19" s="76" t="s">
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E19" s="53" t="s">
-        <x:v>220</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="F19" s="70"/>
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="A20" s="49"/>
-      <x:c r="B20" s="78"/>
-      <x:c r="C20" s="81"/>
-      <x:c r="D20" s="76"/>
+      <x:c r="B20" s="79"/>
+      <x:c r="C20" s="82"/>
+      <x:c r="D20" s="77"/>
       <x:c r="E20" s="54" t="s">
-        <x:v>7</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F20" s="70"/>
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="A21" s="49"/>
-      <x:c r="B21" s="78"/>
-      <x:c r="C21" s="81"/>
-      <x:c r="D21" s="75" t="s">
-        <x:v>68</x:v>
+      <x:c r="B21" s="79"/>
+      <x:c r="C21" s="82"/>
+      <x:c r="D21" s="76" t="s">
+        <x:v>130</x:v>
       </x:c>
       <x:c r="E21" s="53" t="s">
-        <x:v>245</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="F21" s="70"/>
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="A22" s="49"/>
-      <x:c r="B22" s="78"/>
-      <x:c r="C22" s="81"/>
-      <x:c r="D22" s="76"/>
+      <x:c r="B22" s="79"/>
+      <x:c r="C22" s="82"/>
+      <x:c r="D22" s="77"/>
       <x:c r="E22" s="54" t="s">
-        <x:v>167</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F22" s="70"/>
     </x:row>
     <x:row r="23" spans="1:6">
       <x:c r="A23" s="49"/>
-      <x:c r="B23" s="78"/>
-      <x:c r="C23" s="81"/>
+      <x:c r="B23" s="79"/>
+      <x:c r="C23" s="82"/>
       <x:c r="D23" s="37" t="s">
-        <x:v>194</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="E23" s="55" t="s">
-        <x:v>162</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F23" s="70"/>
     </x:row>
     <x:row r="24" spans="1:6">
       <x:c r="A24" s="49"/>
-      <x:c r="B24" s="78"/>
-      <x:c r="C24" s="81"/>
-      <x:c r="D24" s="75" t="s">
-        <x:v>55</x:v>
+      <x:c r="B24" s="79"/>
+      <x:c r="C24" s="82"/>
+      <x:c r="D24" s="76" t="s">
+        <x:v>153</x:v>
       </x:c>
       <x:c r="E24" s="53" t="s">
-        <x:v>39</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F24" s="70"/>
     </x:row>
     <x:row r="25" spans="1:6">
       <x:c r="A25" s="49"/>
-      <x:c r="B25" s="78"/>
-      <x:c r="C25" s="81"/>
-      <x:c r="D25" s="81"/>
+      <x:c r="B25" s="79"/>
+      <x:c r="C25" s="82"/>
+      <x:c r="D25" s="82"/>
       <x:c r="E25" s="51" t="s">
-        <x:v>161</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F25" s="70"/>
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="A26" s="49"/>
-      <x:c r="B26" s="78"/>
-      <x:c r="C26" s="81"/>
-      <x:c r="D26" s="81"/>
+      <x:c r="B26" s="79"/>
+      <x:c r="C26" s="82"/>
+      <x:c r="D26" s="82"/>
       <x:c r="E26" s="51" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F26" s="70"/>
     </x:row>
     <x:row r="27" spans="1:6" ht="16.75">
       <x:c r="A27" s="49"/>
-      <x:c r="B27" s="95"/>
-      <x:c r="C27" s="99"/>
-      <x:c r="D27" s="99"/>
+      <x:c r="B27" s="96"/>
+      <x:c r="C27" s="100"/>
+      <x:c r="D27" s="100"/>
       <x:c r="E27" s="56" t="s">
-        <x:v>227</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F27" s="71"/>
     </x:row>
     <x:row r="28" spans="1:6" ht="16.75">
       <x:c r="A28" s="49"/>
-      <x:c r="B28" s="77" t="s">
-        <x:v>94</x:v>
+      <x:c r="B28" s="78" t="s">
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C28" s="72" t="s">
-        <x:v>148</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D28" s="72" t="s">
-        <x:v>173</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="E28" s="73" t="s">
-        <x:v>225</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F28" s="69"/>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="A29" s="49"/>
-      <x:c r="B29" s="78"/>
-      <x:c r="C29" s="75" t="s">
-        <x:v>149</x:v>
+      <x:c r="B29" s="79"/>
+      <x:c r="C29" s="76" t="s">
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D29" s="37" t="s">
-        <x:v>186</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="E29" s="55" t="s">
-        <x:v>163</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F29" s="70"/>
     </x:row>
     <x:row r="30" spans="1:6">
       <x:c r="A30" s="49"/>
-      <x:c r="B30" s="78"/>
-      <x:c r="C30" s="81"/>
-      <x:c r="D30" s="75" t="s">
-        <x:v>192</x:v>
+      <x:c r="B30" s="79"/>
+      <x:c r="C30" s="82"/>
+      <x:c r="D30" s="76" t="s">
+        <x:v>217</x:v>
       </x:c>
       <x:c r="E30" s="53" t="s">
-        <x:v>218</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F30" s="70"/>
     </x:row>
     <x:row r="31" spans="1:6">
       <x:c r="A31" s="49"/>
-      <x:c r="B31" s="78"/>
-      <x:c r="C31" s="81"/>
-      <x:c r="D31" s="81"/>
+      <x:c r="B31" s="79"/>
+      <x:c r="C31" s="82"/>
+      <x:c r="D31" s="82"/>
       <x:c r="E31" s="51" t="s">
-        <x:v>165</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F31" s="70"/>
     </x:row>
     <x:row r="32" spans="1:6">
       <x:c r="A32" s="49"/>
-      <x:c r="B32" s="78"/>
-      <x:c r="C32" s="81"/>
-      <x:c r="D32" s="81"/>
+      <x:c r="B32" s="79"/>
+      <x:c r="C32" s="82"/>
+      <x:c r="D32" s="82"/>
       <x:c r="E32" s="51" t="s">
-        <x:v>27</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F32" s="70"/>
     </x:row>
     <x:row r="33" spans="1:6" ht="16.75">
       <x:c r="A33" s="49"/>
-      <x:c r="B33" s="95"/>
-      <x:c r="C33" s="99"/>
-      <x:c r="D33" s="99"/>
+      <x:c r="B33" s="96"/>
+      <x:c r="C33" s="100"/>
+      <x:c r="D33" s="100"/>
       <x:c r="E33" s="56" t="s">
-        <x:v>214</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="F33" s="71"/>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="49"/>
-      <x:c r="B34" s="78" t="s">
-        <x:v>157</x:v>
-      </x:c>
-      <x:c r="C34" s="81"/>
-      <x:c r="D34" s="81"/>
+      <x:c r="B34" s="79" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C34" s="82"/>
+      <x:c r="D34" s="82"/>
       <x:c r="E34" s="51" t="s">
-        <x:v>10</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F34" s="70"/>
     </x:row>
     <x:row r="35" spans="1:6" ht="16.75">
       <x:c r="A35" s="49"/>
-      <x:c r="B35" s="95"/>
-      <x:c r="C35" s="99"/>
-      <x:c r="D35" s="99"/>
+      <x:c r="B35" s="96"/>
+      <x:c r="C35" s="100"/>
+      <x:c r="D35" s="100"/>
       <x:c r="E35" s="56" t="s">
-        <x:v>217</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="F35" s="71"/>
     </x:row>

</xml_diff>

<commit_message>
add 0716 comment, 0719 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="252">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="254">
   <x:si>
     <x:t>1. 요구사항 분석 (실현성 확인)
 2. 데이터 흐름도 수정
@@ -33,79 +33,10 @@
  -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 필요 자료 추가 조사
 2. 한계점 및 필요기술 추가
  - 차량 블루투스와 어플 연결 어떻게?
  - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 경쟁 어플 메뉴트리 수정
-2. 요구사항, 기능정의 순서 수정
-3. 한계점 수정
-블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
- - 컴퓨터 견적 추천 앱
- - 주차시 사고발생 알림 앱
-2. 주제 아이디어 최종 선정
- - 차량 관리 어플
-3. 개발 계획서 및 요구사항 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 진행사항 체크 및 2주차 목표 설정
-2. 06.28 회의록 작성
-3. 상용화 된 타 앱 기능 분석
-4. 요구사항 정의
- - 회원가입, DB, 무결성 (미완)
-5. vi사용법 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 07.02 회의록 작성
-2. Git 업로드 한 것 중 중복된 것들 삭제
-3. 어플 흐름 구상도 작성
-4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -119,12 +50,13 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>1-1. Datebook Comment 부분 요약
-1-2. GIT 보고서 다시 작성
-1-3. PPT 머릿글 요약 작성
-1-4. 파일명 수정
-1-5 최종 아이디어 선정 이유 작성
-2. 요구사항 수집 및 분석</x:t>
+    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
+2. 요구사항 추가 및 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 플로우 차트 작성
+2. 설계 계획서 작성
+3. Menu_Tree 도식화 수정</x:t>
   </x:si>
   <x:si>
     <x:t>1. 현장실습 OT
@@ -137,29 +69,101 @@
  - 개발 설계</x:t>
   </x:si>
   <x:si>
-    <x:t>1. Git 목록 삭제
+    <x:t>1. 아이디어 도출
+ - 컴퓨터 견적 추천 앱
+ - 주차시 사고발생 알림 앱
+2. 주제 아이디어 최종 선정
+ - 차량 관리 어플
+3. 개발 계획서 및 요구사항 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 경쟁 어플 메뉴트리 수정
+2. 요구사항, 기능정의 순서 수정
+3. 한계점 수정
+블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1-1. Datebook Comment 부분 요약
+1-2. GIT 보고서 다시 작성
+1-3. PPT 머릿글 요약 작성
+1-4. 파일명 수정
+1-5 최종 아이디어 선정 이유 작성
+2. 요구사항 수집 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
+2. 블루투스 관련 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
+로그인 버튼이 나와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성
+ - 화면별 세부기능 설계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
+  </x:si>
+  <x:si>
+    <x:t>각 버튼 및 창 기능 설명 + 기능 플로우 + 설계 기획 추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
 2. 요구사항 분석
-3. 인터페이스 구상도 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성 (미완)
-2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 추가 자료조사(관련 코드)
-2. FlowChart 수정 및 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
   </x:si>
   <x:si>
     <x:t>1. (2-2) 수익적 요소 추가
@@ -168,434 +172,79 @@
  - 비슷한 어플(마이클) 화면 구성 조사</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
-2. 요구사항 추가 및 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 플로우 차트 작성
-2. 설계 계획서 작성
-3. Menu_Tree 도식화 수정</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 앱 화면별 Sequence 작성
 2. 앱 화면별 어떻게 구성할 것인지 구상
 3. 추가 자료조사</x:t>
   </x:si>
   <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
-로그인 버튼이 나와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
-2. 블루투스 관련 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검내역서(정비소 제공 문서)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리별 check list</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보(오너들의 평균 정보)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
     <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
 비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
   </x:si>
   <x:si>
-    <x:t>경기/인천</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오너들의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수리견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 메뉴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>견적 요청</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고객상담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>최신 글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록 및 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오늘 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연차, 보험료</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공유게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>더 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>글 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 방문 장소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Menu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 검사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자차 게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>함수의 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALL*</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공식 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 주변 검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수익적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험사 선택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메모 입력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 시기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결함/리콜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균 연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>첫예약할인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>카카오톡 문의</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>setting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 후기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모두의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>엔진오일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 시세</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필요 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차 정보 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Home</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연비 랭킹</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용 가이드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨 필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>디테일링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어샵</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 장착점 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 추천 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소 지도 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:25
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 정보 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:22
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>진행 방향 ---&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:40
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스 (메뉴)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 기본 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재</x:t>
-  </x:si>
-  <x:si>
-    <x:t>community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고장사례(리콜사례)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 판매견적 받기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자주 하는 질문</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유사 모델 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 교체 예상 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약/견적 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험료 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰 보유 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성</x:t>
+    <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 인터페이스 구상도 작성
+2. 요구사항 분류하여 수정
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사
+2. 요구사항 추가 조사
+3. 경쟁 어플 기능 비교 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성(설명,컨테이너등 정보 채우기)
+2. 기능플로우 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성 (미완)
+2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사(관련 코드)
+2. FlowChart 수정 및 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
+2. 추가 자료 조사</x:t>
   </x:si>
   <x:si>
     <x:t>1. vi 명령어 설명서 작성 완료
@@ -604,45 +253,184 @@
  - 비기능적 요구사항</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 메뉴시퀀스 작성(설명,컨테이너등 정보 채우기)
-2. 기능플로우 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 인터페이스 구상도 작성
-2. 요구사항 분류하여 수정
-3. 추가 자료조사</x:t>
-  </x:si>
-  <x:si>
     <x:t>1. 요구사항 수집 및 정의
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 추가 자료조사
-2. 요구사항 추가 조사
-3. 경쟁 어플 기능 비교 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 진행사항 체크 및 2주차 목표 설정
+2. 06.28 회의록 작성
+3. 상용화 된 타 앱 기능 분석
+4. 요구사항 정의
+ - 회원가입, DB, 무결성 (미완)
+5. vi사용법 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 07.02 회의록 작성
+2. Git 업로드 한 것 중 중복된 것들 삭제
+3. 어플 흐름 구상도 작성
+4. 요구사항/기능 정의/기능 설계 3가지 부분으로 나누어 요구사항 수정(미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보(오너들의 평균 정보)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검내역서(정비소 제공 문서)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리별 check list</x:t>
   </x:si>
   <x:si>
     <x:t>데이터 연동 설정</x:t>
   </x:si>
   <x:si>
     <x:t>친구 초대 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험료 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰 보유 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 교체 예상 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유사 모델 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약/견적 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 선호도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인 쿠폰 등록</x:t>
   </x:si>
   <x:si>
     <x:t>08:32
 18:03</x:t>
   </x:si>
   <x:si>
-    <x:t>자동차 보험 선호도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인 쿠폰 등록</x:t>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 추천 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소 지도 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 장착점 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고장사례(리콜사례)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 판매견적 받기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자주 하는 질문</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 기본 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>진행 방향 ---&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:40
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스 (메뉴)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 형태로 존재</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:22
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 정보 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>장마철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q&amp;A</x:t>
   </x:si>
   <x:si>
     <x:t>쿠폰함</x:t>
@@ -651,129 +439,117 @@
     <x:t>가을</x:t>
   </x:si>
   <x:si>
-    <x:t>이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>장마철</x:t>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>여름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클</x:t>
   </x:si>
   <x:si>
     <x:t>만족도</x:t>
   </x:si>
   <x:si>
-    <x:t>기록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>여름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Q&amp;A</x:t>
+    <x:t>겨울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>편집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보안성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>봄</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>계절별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>광고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폭설철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평점</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소</x:t>
   </x:si>
   <x:si>
     <x:t>상황별</x:t>
   </x:si>
   <x:si>
+    <x:t>DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인기글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>홈</x:t>
+  </x:si>
+  <x:si>
+    <x:t>손세차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검</x:t>
+  </x:si>
+  <x:si>
     <x:t>검색</x:t>
   </x:si>
   <x:si>
-    <x:t>평점</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폭설철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>광고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰</x:t>
-  </x:si>
-  <x:si>
-    <x:t>채팅창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>홈</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비</x:t>
-  </x:si>
-  <x:si>
     <x:t>달력</x:t>
   </x:si>
   <x:si>
-    <x:t>봄</x:t>
-  </x:si>
-  <x:si>
-    <x:t>편집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보안성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인기글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>손세차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
     <x:t>리뷰</x:t>
   </x:si>
   <x:si>
-    <x:t>겨울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>계절별</x:t>
-  </x:si>
-  <x:si>
     <x:t>게시판</x:t>
   </x:si>
   <x:si>
@@ -783,71 +559,331 @@
     <x:t>최신글</x:t>
   </x:si>
   <x:si>
+    <x:t>경기/인천</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수리견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오너들의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 메뉴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>견적 요청</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고객상담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자차 게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>함수의 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메모 입력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>최신 글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>글 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 방문 장소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Menu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tips</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공식 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연차, 보험료</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록 및 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공유게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 검사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오늘 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>더 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 주변 검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수익적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험사 선택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALL*</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>setting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 후기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 시세</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연비 랭킹</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용 가이드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>디테일링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨 필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어샵</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 시기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필요 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>엔진오일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균 연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카카오톡 문의</x:t>
+  </x:si>
+  <x:si>
+    <x:t>첫예약할인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모두의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차 정보 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결함/리콜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 무료 판매 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 별 남은 수명 보여줌</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소 포인트 적립 연동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이달의 정비/세차 혜택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험료 확인 및 갱신일 알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차종, 차번호, 연식 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 찾아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기아 커넥티드카 연동하기</x:t>
+  </x:si>
+  <x:si>
     <x:t>방문 정비소 기록, 메모</x:t>
   </x:si>
   <x:si>
-    <x:t>차종, 차번호, 연식 등</x:t>
-  </x:si>
-  <x:si>
     <x:t>항목 및 정비 주기 추가</x:t>
   </x:si>
   <x:si>
-    <x:t>이달의 정비/세차 혜택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 별 남은 수명 보여줌</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소 포인트 적립 연동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 무료 판매 견적</x:t>
-  </x:si>
-  <x:si>
     <x:t>점검 스케쥴 및 일정 관리</x:t>
   </x:si>
   <x:si>
-    <x:t>가까운 정비소 찾아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험료 확인 및 갱신일 알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기아 커넥티드카 연동하기</x:t>
+    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 시퀀스 작성
+2. 추가 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 계약서 작성
+2. 현장실습 오리엔테이션</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 보완
+2. 기능정의 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
   </x:si>
   <x:si>
     <x:t>1. Menu_Tree 수정(완료)
 2. 추가 자료 조사</x:t>
   </x:si>
   <x:si>
-    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 보완
-2. 기능정의 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:02</x:t>
+    <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
   </x:si>
   <x:si>
     <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
@@ -857,35 +893,6 @@
   </x:si>
   <x:si>
     <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 화면 시퀀스 작성
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 계약서 작성
-2. 현장실습 오리엔테이션</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2946,7 +2953,7 @@
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="2" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21:D21"/>
+      <x:selection pane="bottomLeft" activeCell="E22" activeCellId="0" sqref="E22:E22"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -2962,16 +2969,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="5" t="s">
-        <x:v>122</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C2" s="6" t="s">
-        <x:v>105</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="D2" s="6" t="s">
-        <x:v>74</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="E2" s="7" t="s">
-        <x:v>117</x:v>
+        <x:v>193</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -2979,13 +2986,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="15" t="s">
-        <x:v>159</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D3" s="9" t="s">
-        <x:v>251</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="E3" s="9" t="s">
-        <x:v>17</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -2993,13 +3000,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="14" t="s">
-        <x:v>159</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D4" s="12" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="E4" s="12" t="s">
         <x:v>2</x:v>
-      </x:c>
-      <x:c r="E4" s="12" t="s">
-        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -3007,13 +3014,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="16" t="s">
-        <x:v>156</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D5" s="12" t="s">
-        <x:v>39</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E5" s="12" t="s">
-        <x:v>12</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -3021,13 +3028,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="18" t="s">
-        <x:v>156</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D6" s="12" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="17" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -3035,13 +3042,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="14" t="s">
-        <x:v>129</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D7" s="12" t="s">
-        <x:v>232</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="E7" s="12" t="s">
-        <x:v>13</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -3049,13 +3056,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="14" t="s">
-        <x:v>131</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="D8" s="12" t="s">
-        <x:v>29</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E8" s="12" t="s">
-        <x:v>161</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -3063,13 +3070,13 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="19" t="s">
-        <x:v>126</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D9" s="12" t="s">
-        <x:v>1</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E9" s="12" t="s">
-        <x:v>40</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -3077,13 +3084,13 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="20" t="s">
-        <x:v>170</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D10" s="12" t="s">
-        <x:v>164</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E10" s="12" t="s">
-        <x:v>3</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
@@ -3091,13 +3098,13 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="22" t="s">
-        <x:v>132</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="D11" s="12" t="s">
-        <x:v>18</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E11" s="12" t="s">
-        <x:v>14</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:5" ht="105.40000000000001">
@@ -3105,10 +3112,10 @@
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="21" t="s">
-        <x:v>134</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="D12" s="12" t="s">
-        <x:v>163</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E12" s="12" t="s">
         <x:v>0</x:v>
@@ -3119,13 +3126,13 @@
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="23" t="s">
-        <x:v>170</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D13" s="12" t="s">
-        <x:v>20</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E13" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5" ht="52.700000000000003">
@@ -3133,13 +3140,13 @@
         <x:v>44384</x:v>
       </x:c>
       <x:c r="C14" s="24" t="s">
-        <x:v>137</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D14" s="12" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E14" s="12" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="E14" s="12" t="s">
-        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:5" ht="52.700000000000003">
@@ -3147,13 +3154,13 @@
         <x:v>44385</x:v>
       </x:c>
       <x:c r="C15" s="30" t="s">
-        <x:v>157</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D15" s="12" t="s">
-        <x:v>165</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>11</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="2:5" ht="26.350000000000001">
@@ -3161,13 +3168,13 @@
         <x:v>44386</x:v>
       </x:c>
       <x:c r="C16" s="31" t="s">
-        <x:v>139</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="D16" s="12" t="s">
-        <x:v>233</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="E16" s="12" t="s">
-        <x:v>26</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="2:5" ht="39.549999999999997">
@@ -3175,13 +3182,13 @@
         <x:v>44389</x:v>
       </x:c>
       <x:c r="C17" s="74" t="s">
-        <x:v>142</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="D17" s="12" t="s">
-        <x:v>27</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>230</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:5" ht="26.350000000000001">
@@ -3189,13 +3196,13 @@
         <x:v>44390</x:v>
       </x:c>
       <x:c r="C18" s="75" t="s">
-        <x:v>141</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D18" s="12" t="s">
-        <x:v>248</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="E18" s="12" t="s">
-        <x:v>42</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="2:5" ht="26.350000000000001">
@@ -3203,13 +3210,13 @@
         <x:v>44391</x:v>
       </x:c>
       <x:c r="C19" s="75" t="s">
-        <x:v>170</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D19" s="12" t="s">
-        <x:v>248</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="E19" s="12" t="s">
-        <x:v>19</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="2:5" ht="26.350000000000001">
@@ -3217,13 +3224,13 @@
         <x:v>44392</x:v>
       </x:c>
       <x:c r="C20" s="14" t="s">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="D20" s="12" t="s">
-        <x:v>5</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="E20" s="11" t="s">
-        <x:v>160</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="2:5" ht="26.350000000000001">
@@ -3232,16 +3239,20 @@
       </x:c>
       <x:c r="C21" s="10"/>
       <x:c r="D21" s="12" t="s">
-        <x:v>162</x:v>
-      </x:c>
-      <x:c r="E21" s="11"/>
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E21" s="12" t="s">
+        <x:v>14</x:v>
+      </x:c>
     </x:row>
     <x:row r="22" spans="2:5">
       <x:c r="B22" s="13">
         <x:v>44396</x:v>
       </x:c>
       <x:c r="C22" s="10"/>
-      <x:c r="D22" s="11"/>
+      <x:c r="D22" s="11" t="s">
+        <x:v>25</x:v>
+      </x:c>
       <x:c r="E22" s="11"/>
     </x:row>
     <x:row r="23" spans="2:5">
@@ -3432,54 +3443,54 @@
   <x:sheetData>
     <x:row r="1" spans="1:9" ht="17.149999999999999">
       <x:c r="A1" s="26" t="s">
-        <x:v>138</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>72</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
-        <x:v>87</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D1" s="34" t="s">
-        <x:v>66</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="E1" s="34" t="s">
-        <x:v>51</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F1" s="34" t="s">
-        <x:v>98</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>113</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="H1" s="34" t="s">
-        <x:v>198</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="I1" s="35" t="s">
-        <x:v>188</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:9">
       <x:c r="A2" s="84" t="s">
-        <x:v>182</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="B2" s="78" t="s">
-        <x:v>197</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="C2" s="81" t="s">
-        <x:v>88</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D2" s="81" t="s">
-        <x:v>112</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="E2" s="38" t="s">
-        <x:v>108</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F2" s="38"/>
       <x:c r="G2" s="38"/>
       <x:c r="H2" s="38"/>
       <x:c r="I2" s="38" t="s">
-        <x:v>148</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9">
@@ -3488,13 +3499,13 @@
       <x:c r="C3" s="82"/>
       <x:c r="D3" s="82"/>
       <x:c r="E3" s="37" t="s">
-        <x:v>152</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="F3" s="37"/>
       <x:c r="G3" s="37"/>
       <x:c r="H3" s="37"/>
       <x:c r="I3" s="37" t="s">
-        <x:v>228</x:v>
+        <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
@@ -3503,7 +3514,7 @@
       <x:c r="C4" s="82"/>
       <x:c r="D4" s="82"/>
       <x:c r="E4" s="37" t="s">
-        <x:v>89</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F4" s="37"/>
       <x:c r="G4" s="37"/>
@@ -3516,10 +3527,10 @@
       <x:c r="C5" s="82"/>
       <x:c r="D5" s="82"/>
       <x:c r="E5" s="76" t="s">
-        <x:v>94</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F5" s="37" t="s">
-        <x:v>70</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="G5" s="37"/>
       <x:c r="H5" s="37"/>
@@ -3532,7 +3543,7 @@
       <x:c r="D6" s="77"/>
       <x:c r="E6" s="77"/>
       <x:c r="F6" s="37" t="s">
-        <x:v>135</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G6" s="37"/>
       <x:c r="H6" s="37"/>
@@ -3543,10 +3554,10 @@
       <x:c r="B7" s="79"/>
       <x:c r="C7" s="82"/>
       <x:c r="D7" s="76" t="s">
-        <x:v>52</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="E7" s="37" t="s">
-        <x:v>178</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F7" s="37"/>
       <x:c r="G7" s="37"/>
@@ -3559,13 +3570,13 @@
       <x:c r="C8" s="82"/>
       <x:c r="D8" s="82"/>
       <x:c r="E8" s="37" t="s">
-        <x:v>202</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="F8" s="37"/>
       <x:c r="G8" s="37"/>
       <x:c r="H8" s="37"/>
       <x:c r="I8" s="37" t="s">
-        <x:v>34</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:9">
@@ -3574,13 +3585,13 @@
       <x:c r="C9" s="82"/>
       <x:c r="D9" s="82"/>
       <x:c r="E9" s="37" t="s">
-        <x:v>201</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F9" s="37"/>
       <x:c r="G9" s="37"/>
       <x:c r="H9" s="37"/>
       <x:c r="I9" s="37" t="s">
-        <x:v>226</x:v>
+        <x:v>231</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
@@ -3589,10 +3600,10 @@
       <x:c r="C10" s="82"/>
       <x:c r="D10" s="82"/>
       <x:c r="E10" s="76" t="s">
-        <x:v>71</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F10" s="37" t="s">
-        <x:v>100</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="G10" s="37"/>
       <x:c r="H10" s="37"/>
@@ -3605,12 +3616,12 @@
       <x:c r="D11" s="82"/>
       <x:c r="E11" s="82"/>
       <x:c r="F11" s="37" t="s">
-        <x:v>123</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="G11" s="37"/>
       <x:c r="H11" s="37"/>
       <x:c r="I11" s="37" t="s">
-        <x:v>236</x:v>
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
@@ -3620,7 +3631,7 @@
       <x:c r="D12" s="82"/>
       <x:c r="E12" s="82"/>
       <x:c r="F12" s="37" t="s">
-        <x:v>207</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="G12" s="37"/>
       <x:c r="H12" s="37"/>
@@ -3633,12 +3644,12 @@
       <x:c r="D13" s="77"/>
       <x:c r="E13" s="77"/>
       <x:c r="F13" s="37" t="s">
-        <x:v>194</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="G13" s="37"/>
       <x:c r="H13" s="37"/>
       <x:c r="I13" s="37" t="s">
-        <x:v>221</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="J13" s="29"/>
       <x:c r="K13" s="29"/>
@@ -3664,19 +3675,19 @@
       <x:c r="A14" s="85"/>
       <x:c r="B14" s="79"/>
       <x:c r="C14" s="76" t="s">
-        <x:v>106</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="D14" s="76" t="s">
-        <x:v>102</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="E14" s="37" t="s">
-        <x:v>186</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F14" s="37"/>
       <x:c r="G14" s="37"/>
       <x:c r="H14" s="37"/>
       <x:c r="I14" s="37" t="s">
-        <x:v>177</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="J14" s="29"/>
       <x:c r="K14" s="29"/>
@@ -3704,13 +3715,13 @@
       <x:c r="C15" s="82"/>
       <x:c r="D15" s="82"/>
       <x:c r="E15" s="37" t="s">
-        <x:v>95</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="F15" s="37"/>
       <x:c r="G15" s="37"/>
       <x:c r="H15" s="37"/>
       <x:c r="I15" s="37" t="s">
-        <x:v>115</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="J15" s="29"/>
       <x:c r="K15" s="29"/>
@@ -3738,7 +3749,7 @@
       <x:c r="C16" s="82"/>
       <x:c r="D16" s="82"/>
       <x:c r="E16" s="37" t="s">
-        <x:v>104</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="F16" s="37"/>
       <x:c r="G16" s="37"/>
@@ -3769,13 +3780,13 @@
       <x:c r="C17" s="82"/>
       <x:c r="D17" s="77"/>
       <x:c r="E17" s="37" t="s">
-        <x:v>91</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F17" s="37"/>
       <x:c r="G17" s="37"/>
       <x:c r="H17" s="37"/>
       <x:c r="I17" s="37" t="s">
-        <x:v>243</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="J17" s="29"/>
       <x:c r="K17" s="29"/>
@@ -3802,13 +3813,13 @@
       <x:c r="B18" s="79"/>
       <x:c r="C18" s="82"/>
       <x:c r="D18" s="37" t="s">
-        <x:v>171</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E18" s="37" t="s">
-        <x:v>155</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F18" s="37" t="s">
-        <x:v>85</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="G18" s="37"/>
       <x:c r="H18" s="37"/>
@@ -3838,14 +3849,14 @@
       <x:c r="B19" s="79"/>
       <x:c r="C19" s="82"/>
       <x:c r="D19" s="37" t="s">
-        <x:v>213</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="E19" s="37"/>
       <x:c r="F19" s="37"/>
       <x:c r="G19" s="37"/>
       <x:c r="H19" s="37"/>
       <x:c r="I19" s="76" t="s">
-        <x:v>145</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="J19" s="29"/>
       <x:c r="K19" s="29"/>
@@ -3872,7 +3883,7 @@
       <x:c r="B20" s="79"/>
       <x:c r="C20" s="82"/>
       <x:c r="D20" s="37" t="s">
-        <x:v>91</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="E20" s="37"/>
       <x:c r="F20" s="37"/>
@@ -3904,7 +3915,7 @@
       <x:c r="B21" s="79"/>
       <x:c r="C21" s="82"/>
       <x:c r="D21" s="37" t="s">
-        <x:v>104</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="E21" s="37"/>
       <x:c r="F21" s="37"/>
@@ -3936,7 +3947,7 @@
       <x:c r="B22" s="80"/>
       <x:c r="C22" s="77"/>
       <x:c r="D22" s="37" t="s">
-        <x:v>151</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E22" s="37"/>
       <x:c r="F22" s="37"/>
@@ -3966,10 +3977,10 @@
     <x:row r="23" spans="1:28">
       <x:c r="A23" s="85"/>
       <x:c r="B23" s="83" t="s">
-        <x:v>96</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="C23" s="37" t="s">
-        <x:v>154</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="D23" s="37"/>
       <x:c r="E23" s="37"/>
@@ -4001,7 +4012,7 @@
       <x:c r="A24" s="85"/>
       <x:c r="B24" s="79"/>
       <x:c r="C24" s="37" t="s">
-        <x:v>192</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="D24" s="37"/>
       <x:c r="E24" s="37"/>
@@ -4033,7 +4044,7 @@
       <x:c r="A25" s="85"/>
       <x:c r="B25" s="79"/>
       <x:c r="C25" s="37" t="s">
-        <x:v>185</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="D25" s="37"/>
       <x:c r="E25" s="37"/>
@@ -4065,13 +4076,13 @@
       <x:c r="A26" s="85"/>
       <x:c r="B26" s="79"/>
       <x:c r="C26" s="76" t="s">
-        <x:v>96</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="D26" s="37" t="s">
-        <x:v>107</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="E26" s="37" t="s">
-        <x:v>150</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F26" s="37"/>
       <x:c r="G26" s="37"/>
@@ -4161,13 +4172,13 @@
       <x:c r="B27" s="83"/>
       <x:c r="C27" s="82"/>
       <x:c r="D27" s="76" t="s">
-        <x:v>199</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E27" s="37" t="s">
-        <x:v>60</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F27" s="37" t="s">
-        <x:v>127</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G27" s="37"/>
       <x:c r="H27" s="37"/>
@@ -4257,10 +4268,10 @@
       <x:c r="C28" s="82"/>
       <x:c r="D28" s="77"/>
       <x:c r="E28" s="37" t="s">
-        <x:v>84</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F28" s="37" t="s">
-        <x:v>127</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="G28" s="37"/>
       <x:c r="H28" s="37"/>
@@ -4349,10 +4360,10 @@
       <x:c r="B29" s="79"/>
       <x:c r="C29" s="82"/>
       <x:c r="D29" s="37" t="s">
-        <x:v>50</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="E29" s="39" t="s">
-        <x:v>53</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F29" s="39"/>
       <x:c r="G29" s="37"/>
@@ -4442,10 +4453,10 @@
       <x:c r="B30" s="79"/>
       <x:c r="C30" s="82"/>
       <x:c r="D30" s="37" t="s">
-        <x:v>120</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="E30" s="37" t="s">
-        <x:v>200</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F30" s="37"/>
       <x:c r="G30" s="37"/>
@@ -4536,7 +4547,7 @@
       <x:c r="C31" s="82"/>
       <x:c r="D31" s="37"/>
       <x:c r="E31" s="37" t="s">
-        <x:v>48</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F31" s="37"/>
       <x:c r="G31" s="37"/>
@@ -4626,10 +4637,10 @@
       <x:c r="B32" s="79"/>
       <x:c r="C32" s="82"/>
       <x:c r="D32" s="37" t="s">
-        <x:v>93</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="E32" s="37" t="s">
-        <x:v>124</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F32" s="37"/>
       <x:c r="G32" s="37"/>
@@ -4719,7 +4730,7 @@
       <x:c r="B33" s="79"/>
       <x:c r="C33" s="77"/>
       <x:c r="D33" s="37" t="s">
-        <x:v>97</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="E33" s="37"/>
       <x:c r="F33" s="37"/>
@@ -4809,10 +4820,10 @@
       <x:c r="A34" s="84"/>
       <x:c r="B34" s="83"/>
       <x:c r="C34" s="76" t="s">
-        <x:v>82</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D34" s="37" t="s">
-        <x:v>80</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E34" s="37"/>
       <x:c r="F34" s="37"/>
@@ -4903,7 +4914,7 @@
       <x:c r="B35" s="79"/>
       <x:c r="C35" s="82"/>
       <x:c r="D35" s="37" t="s">
-        <x:v>203</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="E35" s="37"/>
       <x:c r="F35" s="37"/>
@@ -4994,7 +5005,7 @@
       <x:c r="B36" s="79"/>
       <x:c r="C36" s="82"/>
       <x:c r="D36" s="37" t="s">
-        <x:v>196</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="E36" s="37"/>
       <x:c r="F36" s="37"/>
@@ -5085,7 +5096,7 @@
       <x:c r="B37" s="79"/>
       <x:c r="C37" s="82"/>
       <x:c r="D37" s="37" t="s">
-        <x:v>210</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E37" s="37"/>
       <x:c r="F37" s="37"/>
@@ -5176,7 +5187,7 @@
       <x:c r="B38" s="79"/>
       <x:c r="C38" s="82"/>
       <x:c r="D38" s="37" t="s">
-        <x:v>121</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="E38" s="37"/>
       <x:c r="F38" s="37"/>
@@ -5267,7 +5278,7 @@
       <x:c r="B39" s="83"/>
       <x:c r="C39" s="77"/>
       <x:c r="D39" s="37" t="s">
-        <x:v>73</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="E39" s="37"/>
       <x:c r="F39" s="37"/>
@@ -5356,10 +5367,10 @@
     <x:row r="40" spans="1:87">
       <x:c r="A40" s="85"/>
       <x:c r="B40" s="83" t="s">
-        <x:v>216</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C40" s="37" t="s">
-        <x:v>209</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="D40" s="37"/>
       <x:c r="E40" s="37"/>
@@ -5450,7 +5461,7 @@
       <x:c r="A41" s="85"/>
       <x:c r="B41" s="79"/>
       <x:c r="C41" s="37" t="s">
-        <x:v>58</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D41" s="37"/>
       <x:c r="E41" s="37"/>
@@ -5541,7 +5552,7 @@
       <x:c r="A42" s="85"/>
       <x:c r="B42" s="79"/>
       <x:c r="C42" s="37" t="s">
-        <x:v>75</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="D42" s="37"/>
       <x:c r="E42" s="37"/>
@@ -5632,7 +5643,7 @@
       <x:c r="A43" s="85"/>
       <x:c r="B43" s="79"/>
       <x:c r="C43" s="37" t="s">
-        <x:v>64</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D43" s="37"/>
       <x:c r="E43" s="37"/>
@@ -5723,7 +5734,7 @@
       <x:c r="A44" s="85"/>
       <x:c r="B44" s="79"/>
       <x:c r="C44" s="37" t="s">
-        <x:v>185</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="D44" s="37"/>
       <x:c r="E44" s="37"/>
@@ -5814,7 +5825,7 @@
       <x:c r="A45" s="85"/>
       <x:c r="B45" s="80"/>
       <x:c r="C45" s="37" t="s">
-        <x:v>69</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="D45" s="37"/>
       <x:c r="E45" s="37"/>
@@ -5904,10 +5915,10 @@
     <x:row r="46" spans="1:87">
       <x:c r="A46" s="85"/>
       <x:c r="B46" s="83" t="s">
-        <x:v>195</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C46" s="37" t="s">
-        <x:v>191</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D46" s="37"/>
       <x:c r="E46" s="37"/>
@@ -5998,7 +6009,7 @@
       <x:c r="A47" s="85"/>
       <x:c r="B47" s="79"/>
       <x:c r="C47" s="37" t="s">
-        <x:v>175</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D47" s="37"/>
       <x:c r="E47" s="37"/>
@@ -6089,7 +6100,7 @@
       <x:c r="A48" s="85"/>
       <x:c r="B48" s="79"/>
       <x:c r="C48" s="37" t="s">
-        <x:v>90</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D48" s="37"/>
       <x:c r="E48" s="37"/>
@@ -6180,7 +6191,7 @@
       <x:c r="A49" s="85"/>
       <x:c r="B49" s="80"/>
       <x:c r="C49" s="37" t="s">
-        <x:v>99</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="D49" s="37"/>
       <x:c r="E49" s="37"/>
@@ -6270,13 +6281,13 @@
     <x:row r="50" spans="1:87">
       <x:c r="A50" s="85"/>
       <x:c r="B50" s="83" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="C50" s="76" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="C50" s="76" t="s">
-        <x:v>154</x:v>
-      </x:c>
       <x:c r="D50" s="37" t="s">
-        <x:v>56</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E50" s="37"/>
       <x:c r="F50" s="37"/>
@@ -6367,7 +6378,7 @@
       <x:c r="B51" s="79"/>
       <x:c r="C51" s="77"/>
       <x:c r="D51" s="37" t="s">
-        <x:v>101</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="E51" s="37"/>
       <x:c r="F51" s="37"/>
@@ -6457,10 +6468,10 @@
       <x:c r="A52" s="85"/>
       <x:c r="B52" s="79"/>
       <x:c r="C52" s="76" t="s">
-        <x:v>173</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D52" s="37" t="s">
-        <x:v>172</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E52" s="37"/>
       <x:c r="F52" s="37"/>
@@ -6551,7 +6562,7 @@
       <x:c r="B53" s="79"/>
       <x:c r="C53" s="77"/>
       <x:c r="D53" s="37" t="s">
-        <x:v>158</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="E53" s="37"/>
       <x:c r="F53" s="37"/>
@@ -6641,10 +6652,10 @@
       <x:c r="A54" s="85"/>
       <x:c r="B54" s="79"/>
       <x:c r="C54" s="76" t="s">
-        <x:v>128</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D54" s="37" t="s">
-        <x:v>133</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E54" s="37"/>
       <x:c r="F54" s="37"/>
@@ -6735,7 +6746,7 @@
       <x:c r="B55" s="79"/>
       <x:c r="C55" s="82"/>
       <x:c r="D55" s="37" t="s">
-        <x:v>136</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E55" s="37"/>
       <x:c r="F55" s="37"/>
@@ -6826,7 +6837,7 @@
       <x:c r="B56" s="79"/>
       <x:c r="C56" s="77"/>
       <x:c r="D56" s="37" t="s">
-        <x:v>225</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="E56" s="37"/>
       <x:c r="F56" s="37"/>
@@ -6916,10 +6927,10 @@
       <x:c r="A57" s="85"/>
       <x:c r="B57" s="79"/>
       <x:c r="C57" s="76" t="s">
-        <x:v>57</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D57" s="37" t="s">
-        <x:v>222</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="E57" s="37"/>
       <x:c r="F57" s="37"/>
@@ -7010,7 +7021,7 @@
       <x:c r="B58" s="79"/>
       <x:c r="C58" s="77"/>
       <x:c r="D58" s="37" t="s">
-        <x:v>169</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E58" s="37"/>
       <x:c r="F58" s="37"/>
@@ -7100,10 +7111,10 @@
       <x:c r="A59" s="85"/>
       <x:c r="B59" s="79"/>
       <x:c r="C59" s="76" t="s">
-        <x:v>168</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D59" s="37" t="s">
-        <x:v>229</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="E59" s="37"/>
       <x:c r="F59" s="37"/>
@@ -7194,7 +7205,7 @@
       <x:c r="B60" s="79"/>
       <x:c r="C60" s="77"/>
       <x:c r="D60" s="37" t="s">
-        <x:v>224</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="E60" s="37"/>
       <x:c r="F60" s="37"/>
@@ -7284,10 +7295,10 @@
       <x:c r="A61" s="85"/>
       <x:c r="B61" s="79"/>
       <x:c r="C61" s="76" t="s">
-        <x:v>118</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="D61" s="37" t="s">
-        <x:v>183</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E61" s="37"/>
       <x:c r="F61" s="37"/>
@@ -7378,7 +7389,7 @@
       <x:c r="B62" s="80"/>
       <x:c r="C62" s="77"/>
       <x:c r="D62" s="37" t="s">
-        <x:v>54</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="E62" s="37"/>
       <x:c r="F62" s="37"/>
@@ -9420,50 +9431,50 @@
   <x:sheetData>
     <x:row r="1" spans="1:8" ht="17.149999999999999">
       <x:c r="A1" s="32" t="s">
-        <x:v>138</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>72</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
-        <x:v>87</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D1" s="34" t="s">
-        <x:v>66</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="E1" s="34" t="s">
-        <x:v>51</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F1" s="34" t="s">
-        <x:v>98</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>198</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="H1" s="35" t="s">
-        <x:v>212</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8" ht="16.75" customHeight="1">
       <x:c r="A2" s="84" t="s">
-        <x:v>92</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="B2" s="78" t="s">
-        <x:v>114</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="C2" s="91" t="s">
-        <x:v>88</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D2" s="89" t="s">
-        <x:v>102</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="E2" s="61" t="s">
-        <x:v>144</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F2" s="61"/>
       <x:c r="G2" s="61"/>
       <x:c r="H2" s="61" t="s">
-        <x:v>220</x:v>
+        <x:v>226</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -9472,12 +9483,12 @@
       <x:c r="C3" s="92"/>
       <x:c r="D3" s="90"/>
       <x:c r="E3" s="62" t="s">
-        <x:v>77</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F3" s="62"/>
       <x:c r="G3" s="62"/>
       <x:c r="H3" s="62" t="s">
-        <x:v>63</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -9486,12 +9497,12 @@
       <x:c r="C4" s="92"/>
       <x:c r="D4" s="88"/>
       <x:c r="E4" s="62" t="s">
-        <x:v>94</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F4" s="62"/>
       <x:c r="G4" s="62"/>
       <x:c r="H4" s="62" t="s">
-        <x:v>219</x:v>
+        <x:v>229</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -9499,15 +9510,15 @@
       <x:c r="B5" s="79"/>
       <x:c r="C5" s="92"/>
       <x:c r="D5" s="87" t="s">
-        <x:v>52</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="E5" s="63" t="s">
-        <x:v>59</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="F5" s="62"/>
       <x:c r="G5" s="62"/>
       <x:c r="H5" s="62" t="s">
-        <x:v>244</x:v>
+        <x:v>234</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -9516,28 +9527,28 @@
       <x:c r="C6" s="93"/>
       <x:c r="D6" s="88"/>
       <x:c r="E6" s="63" t="s">
-        <x:v>201</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F6" s="62"/>
       <x:c r="G6" s="62"/>
       <x:c r="H6" s="62" t="s">
-        <x:v>43</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="85"/>
       <x:c r="B7" s="79"/>
       <x:c r="C7" s="95" t="s">
-        <x:v>49</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D7" s="87" t="s">
-        <x:v>45</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E7" s="87" t="s">
-        <x:v>102</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F7" s="62" t="s">
-        <x:v>186</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="G7" s="62"/>
       <x:c r="H7" s="62"/>
@@ -9549,7 +9560,7 @@
       <x:c r="D8" s="90"/>
       <x:c r="E8" s="90"/>
       <x:c r="F8" s="62" t="s">
-        <x:v>147</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="G8" s="62"/>
       <x:c r="H8" s="62"/>
@@ -9561,7 +9572,7 @@
       <x:c r="D9" s="90"/>
       <x:c r="E9" s="90"/>
       <x:c r="F9" s="62" t="s">
-        <x:v>62</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G9" s="62"/>
       <x:c r="H9" s="62"/>
@@ -9573,7 +9584,7 @@
       <x:c r="D10" s="90"/>
       <x:c r="E10" s="90"/>
       <x:c r="F10" s="62" t="s">
-        <x:v>213</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="G10" s="62"/>
       <x:c r="H10" s="62"/>
@@ -9585,7 +9596,7 @@
       <x:c r="D11" s="94"/>
       <x:c r="E11" s="94"/>
       <x:c r="F11" s="65" t="s">
-        <x:v>65</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="G11" s="65"/>
       <x:c r="H11" s="65"/>
@@ -9593,13 +9604,13 @@
     <x:row r="12" spans="1:8">
       <x:c r="A12" s="85"/>
       <x:c r="B12" s="79" t="s">
-        <x:v>204</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C12" s="92" t="s">
-        <x:v>68</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="D12" s="61" t="s">
-        <x:v>199</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E12" s="90" t="s">
         <x:v>227</x:v>
@@ -9613,7 +9624,7 @@
       <x:c r="B13" s="79"/>
       <x:c r="C13" s="92"/>
       <x:c r="D13" s="63" t="s">
-        <x:v>107</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="E13" s="90"/>
       <x:c r="F13" s="62"/>
@@ -9625,7 +9636,7 @@
       <x:c r="B14" s="79"/>
       <x:c r="C14" s="92"/>
       <x:c r="D14" s="63" t="s">
-        <x:v>119</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="E14" s="90"/>
       <x:c r="F14" s="62"/>
@@ -9637,7 +9648,7 @@
       <x:c r="B15" s="79"/>
       <x:c r="C15" s="93"/>
       <x:c r="D15" s="63" t="s">
-        <x:v>73</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="E15" s="88"/>
       <x:c r="F15" s="62"/>
@@ -9648,20 +9659,20 @@
       <x:c r="A16" s="85"/>
       <x:c r="B16" s="79"/>
       <x:c r="C16" s="95" t="s">
-        <x:v>111</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="D16" s="63" t="s">
-        <x:v>81</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="E16" s="87" t="s">
-        <x:v>154</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F16" s="62" t="s">
-        <x:v>56</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="G16" s="62"/>
       <x:c r="H16" s="87" t="s">
-        <x:v>241</x:v>
+        <x:v>252</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:8">
@@ -9669,11 +9680,11 @@
       <x:c r="B17" s="79"/>
       <x:c r="C17" s="93"/>
       <x:c r="D17" s="62" t="s">
-        <x:v>205</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="E17" s="88"/>
       <x:c r="F17" s="62" t="s">
-        <x:v>101</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="G17" s="62"/>
       <x:c r="H17" s="88"/>
@@ -9682,26 +9693,26 @@
       <x:c r="A18" s="85"/>
       <x:c r="B18" s="96"/>
       <x:c r="C18" s="66" t="s">
-        <x:v>116</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="D18" s="65"/>
       <x:c r="E18" s="65"/>
       <x:c r="F18" s="65"/>
       <x:c r="G18" s="65"/>
       <x:c r="H18" s="65" t="s">
-        <x:v>223</x:v>
+        <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
       <x:c r="A19" s="85"/>
       <x:c r="B19" s="79" t="s">
-        <x:v>146</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C19" s="92" t="s">
-        <x:v>216</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D19" s="61" t="s">
-        <x:v>209</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="E19" s="61"/>
       <x:c r="F19" s="61"/>
@@ -9713,7 +9724,7 @@
       <x:c r="B20" s="79"/>
       <x:c r="C20" s="92"/>
       <x:c r="D20" s="62" t="s">
-        <x:v>218</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E20" s="62"/>
       <x:c r="F20" s="62"/>
@@ -9725,7 +9736,7 @@
       <x:c r="B21" s="79"/>
       <x:c r="C21" s="92"/>
       <x:c r="D21" s="62" t="s">
-        <x:v>75</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="E21" s="62"/>
       <x:c r="F21" s="62"/>
@@ -9737,7 +9748,7 @@
       <x:c r="B22" s="79"/>
       <x:c r="C22" s="92"/>
       <x:c r="D22" s="62" t="s">
-        <x:v>185</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="E22" s="62"/>
       <x:c r="F22" s="62"/>
@@ -9749,7 +9760,7 @@
       <x:c r="B23" s="79"/>
       <x:c r="C23" s="93"/>
       <x:c r="D23" s="62" t="s">
-        <x:v>69</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="E23" s="62"/>
       <x:c r="F23" s="62"/>
@@ -9760,13 +9771,13 @@
       <x:c r="A24" s="84"/>
       <x:c r="B24" s="83"/>
       <x:c r="C24" s="95" t="s">
-        <x:v>64</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D24" s="87" t="s">
-        <x:v>184</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="E24" s="62" t="s">
-        <x:v>176</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F24" s="62"/>
       <x:c r="G24" s="62"/>
@@ -9778,7 +9789,7 @@
       <x:c r="C25" s="92"/>
       <x:c r="D25" s="88"/>
       <x:c r="E25" s="62" t="s">
-        <x:v>190</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F25" s="62"/>
       <x:c r="G25" s="62"/>
@@ -9789,10 +9800,10 @@
       <x:c r="B26" s="83"/>
       <x:c r="C26" s="92"/>
       <x:c r="D26" s="87" t="s">
-        <x:v>215</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="E26" s="62" t="s">
-        <x:v>206</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F26" s="62"/>
       <x:c r="G26" s="62"/>
@@ -9804,7 +9815,7 @@
       <x:c r="C27" s="92"/>
       <x:c r="D27" s="90"/>
       <x:c r="E27" s="62" t="s">
-        <x:v>180</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F27" s="62"/>
       <x:c r="G27" s="62"/>
@@ -9816,7 +9827,7 @@
       <x:c r="C28" s="92"/>
       <x:c r="D28" s="90"/>
       <x:c r="E28" s="62" t="s">
-        <x:v>174</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="F28" s="62"/>
       <x:c r="G28" s="62"/>
@@ -9828,7 +9839,7 @@
       <x:c r="C29" s="97"/>
       <x:c r="D29" s="94"/>
       <x:c r="E29" s="65" t="s">
-        <x:v>214</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F29" s="65"/>
       <x:c r="G29" s="65"/>
@@ -9837,10 +9848,10 @@
     <x:row r="30" spans="1:8">
       <x:c r="A30" s="85"/>
       <x:c r="B30" s="79" t="s">
-        <x:v>195</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C30" s="67" t="s">
-        <x:v>191</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D30" s="61"/>
       <x:c r="E30" s="61"/>
@@ -9852,7 +9863,7 @@
       <x:c r="A31" s="85"/>
       <x:c r="B31" s="79"/>
       <x:c r="C31" s="58" t="s">
-        <x:v>175</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D31" s="62"/>
       <x:c r="E31" s="62"/>
@@ -9864,7 +9875,7 @@
       <x:c r="A32" s="85"/>
       <x:c r="B32" s="79"/>
       <x:c r="C32" s="58" t="s">
-        <x:v>90</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D32" s="62"/>
       <x:c r="E32" s="62"/>
@@ -9876,7 +9887,7 @@
       <x:c r="A33" s="85"/>
       <x:c r="B33" s="96"/>
       <x:c r="C33" s="68" t="s">
-        <x:v>99</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="D33" s="65"/>
       <x:c r="E33" s="65"/>
@@ -9887,10 +9898,10 @@
     <x:row r="34" spans="1:8">
       <x:c r="A34" s="85"/>
       <x:c r="B34" s="79" t="s">
-        <x:v>103</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="C34" s="67" t="s">
-        <x:v>143</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="D34" s="61"/>
       <x:c r="E34" s="61"/>
@@ -9902,10 +9913,10 @@
       <x:c r="A35" s="85"/>
       <x:c r="B35" s="79"/>
       <x:c r="C35" s="95" t="s">
-        <x:v>118</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="D35" s="62" t="s">
-        <x:v>183</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E35" s="62"/>
       <x:c r="F35" s="62"/>
@@ -9917,7 +9928,7 @@
       <x:c r="B36" s="79"/>
       <x:c r="C36" s="92"/>
       <x:c r="D36" s="62" t="s">
-        <x:v>54</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="E36" s="62"/>
       <x:c r="F36" s="62"/>
@@ -9929,7 +9940,7 @@
       <x:c r="B37" s="96"/>
       <x:c r="C37" s="97"/>
       <x:c r="D37" s="65" t="s">
-        <x:v>149</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="E37" s="65"/>
       <x:c r="F37" s="65"/>
@@ -10253,34 +10264,34 @@
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="49"/>
       <x:c r="B2" s="36" t="s">
-        <x:v>181</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C2" s="36" t="s">
-        <x:v>140</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="D2" s="36" t="s">
-        <x:v>110</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="E2" s="36" t="s">
-        <x:v>109</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F2" s="36" t="s">
-        <x:v>212</x:v>
+        <x:v>114</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" ht="16.75">
       <x:c r="A3" s="49"/>
       <x:c r="B3" s="78" t="s">
-        <x:v>61</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="C3" s="81" t="s">
-        <x:v>76</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="D3" s="81" t="s">
-        <x:v>55</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="E3" s="50" t="s">
-        <x:v>9</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F3" s="69"/>
     </x:row>
@@ -10290,7 +10301,7 @@
       <x:c r="C4" s="82"/>
       <x:c r="D4" s="82"/>
       <x:c r="E4" s="51" t="s">
-        <x:v>240</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="F4" s="70"/>
     </x:row>
@@ -10300,7 +10311,7 @@
       <x:c r="C5" s="82"/>
       <x:c r="D5" s="82"/>
       <x:c r="E5" s="51" t="s">
-        <x:v>166</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F5" s="70"/>
     </x:row>
@@ -10310,7 +10321,7 @@
       <x:c r="C6" s="82"/>
       <x:c r="D6" s="82"/>
       <x:c r="E6" s="51" t="s">
-        <x:v>22</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F6" s="70"/>
     </x:row>
@@ -10320,7 +10331,7 @@
       <x:c r="C7" s="82"/>
       <x:c r="D7" s="77"/>
       <x:c r="E7" s="52" t="s">
-        <x:v>47</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F7" s="70"/>
     </x:row>
@@ -10329,10 +10340,10 @@
       <x:c r="B8" s="79"/>
       <x:c r="C8" s="82"/>
       <x:c r="D8" s="76" t="s">
-        <x:v>187</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E8" s="53" t="s">
-        <x:v>7</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F8" s="70"/>
     </x:row>
@@ -10342,7 +10353,7 @@
       <x:c r="C9" s="82"/>
       <x:c r="D9" s="82"/>
       <x:c r="E9" s="51" t="s">
-        <x:v>234</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="F9" s="70"/>
     </x:row>
@@ -10352,7 +10363,7 @@
       <x:c r="C10" s="82"/>
       <x:c r="D10" s="77"/>
       <x:c r="E10" s="54" t="s">
-        <x:v>167</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F10" s="70"/>
     </x:row>
@@ -10361,10 +10372,10 @@
       <x:c r="B11" s="79"/>
       <x:c r="C11" s="82"/>
       <x:c r="D11" s="76" t="s">
-        <x:v>189</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="E11" s="53" t="s">
-        <x:v>38</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F11" s="70"/>
     </x:row>
@@ -10374,7 +10385,7 @@
       <x:c r="C12" s="77"/>
       <x:c r="D12" s="77"/>
       <x:c r="E12" s="54" t="s">
-        <x:v>24</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F12" s="70"/>
     </x:row>
@@ -10382,13 +10393,13 @@
       <x:c r="A13" s="49"/>
       <x:c r="B13" s="79"/>
       <x:c r="C13" s="76" t="s">
-        <x:v>125</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D13" s="76" t="s">
-        <x:v>216</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="E13" s="53" t="s">
-        <x:v>246</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F13" s="70"/>
     </x:row>
@@ -10398,7 +10409,7 @@
       <x:c r="C14" s="82"/>
       <x:c r="D14" s="82"/>
       <x:c r="E14" s="51" t="s">
-        <x:v>8</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F14" s="70"/>
     </x:row>
@@ -10408,7 +10419,7 @@
       <x:c r="C15" s="82"/>
       <x:c r="D15" s="82"/>
       <x:c r="E15" s="51" t="s">
-        <x:v>237</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="F15" s="70"/>
     </x:row>
@@ -10418,7 +10429,7 @@
       <x:c r="C16" s="82"/>
       <x:c r="D16" s="77"/>
       <x:c r="E16" s="54" t="s">
-        <x:v>35</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F16" s="70"/>
     </x:row>
@@ -10427,10 +10438,10 @@
       <x:c r="B17" s="79"/>
       <x:c r="C17" s="82"/>
       <x:c r="D17" s="76" t="s">
-        <x:v>193</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="E17" s="53" t="s">
-        <x:v>231</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F17" s="70"/>
     </x:row>
@@ -10440,7 +10451,7 @@
       <x:c r="C18" s="77"/>
       <x:c r="D18" s="77"/>
       <x:c r="E18" s="52" t="s">
-        <x:v>41</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F18" s="70"/>
     </x:row>
@@ -10448,13 +10459,13 @@
       <x:c r="A19" s="49"/>
       <x:c r="B19" s="79"/>
       <x:c r="C19" s="76" t="s">
-        <x:v>211</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D19" s="76" t="s">
-        <x:v>44</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E19" s="53" t="s">
-        <x:v>247</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F19" s="70"/>
     </x:row>
@@ -10464,7 +10475,7 @@
       <x:c r="C20" s="82"/>
       <x:c r="D20" s="77"/>
       <x:c r="E20" s="54" t="s">
-        <x:v>23</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="F20" s="70"/>
     </x:row>
@@ -10473,10 +10484,10 @@
       <x:c r="B21" s="79"/>
       <x:c r="C21" s="82"/>
       <x:c r="D21" s="76" t="s">
-        <x:v>130</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E21" s="53" t="s">
-        <x:v>242</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="F21" s="70"/>
     </x:row>
@@ -10486,7 +10497,7 @@
       <x:c r="C22" s="82"/>
       <x:c r="D22" s="77"/>
       <x:c r="E22" s="54" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F22" s="70"/>
     </x:row>
@@ -10495,10 +10506,10 @@
       <x:c r="B23" s="79"/>
       <x:c r="C23" s="82"/>
       <x:c r="D23" s="37" t="s">
-        <x:v>205</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="E23" s="55" t="s">
-        <x:v>30</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F23" s="70"/>
     </x:row>
@@ -10507,10 +10518,10 @@
       <x:c r="B24" s="79"/>
       <x:c r="C24" s="82"/>
       <x:c r="D24" s="76" t="s">
-        <x:v>153</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E24" s="53" t="s">
-        <x:v>46</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F24" s="70"/>
     </x:row>
@@ -10520,7 +10531,7 @@
       <x:c r="C25" s="82"/>
       <x:c r="D25" s="82"/>
       <x:c r="E25" s="51" t="s">
-        <x:v>37</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F25" s="70"/>
     </x:row>
@@ -10530,7 +10541,7 @@
       <x:c r="C26" s="82"/>
       <x:c r="D26" s="82"/>
       <x:c r="E26" s="51" t="s">
-        <x:v>32</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F26" s="70"/>
     </x:row>
@@ -10540,23 +10551,23 @@
       <x:c r="C27" s="100"/>
       <x:c r="D27" s="100"/>
       <x:c r="E27" s="56" t="s">
-        <x:v>238</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="F27" s="71"/>
     </x:row>
     <x:row r="28" spans="1:6" ht="16.75">
       <x:c r="A28" s="49"/>
       <x:c r="B28" s="78" t="s">
-        <x:v>86</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C28" s="72" t="s">
-        <x:v>78</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="D28" s="72" t="s">
-        <x:v>179</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="E28" s="73" t="s">
-        <x:v>235</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="F28" s="69"/>
     </x:row>
@@ -10564,13 +10575,13 @@
       <x:c r="A29" s="49"/>
       <x:c r="B29" s="79"/>
       <x:c r="C29" s="76" t="s">
-        <x:v>79</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="D29" s="37" t="s">
-        <x:v>208</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="E29" s="55" t="s">
-        <x:v>31</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F29" s="70"/>
     </x:row>
@@ -10579,10 +10590,10 @@
       <x:c r="B30" s="79"/>
       <x:c r="C30" s="82"/>
       <x:c r="D30" s="76" t="s">
-        <x:v>217</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="E30" s="53" t="s">
-        <x:v>250</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F30" s="70"/>
     </x:row>
@@ -10592,7 +10603,7 @@
       <x:c r="C31" s="82"/>
       <x:c r="D31" s="82"/>
       <x:c r="E31" s="51" t="s">
-        <x:v>33</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F31" s="70"/>
     </x:row>
@@ -10602,7 +10613,7 @@
       <x:c r="C32" s="82"/>
       <x:c r="D32" s="82"/>
       <x:c r="E32" s="51" t="s">
-        <x:v>6</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F32" s="70"/>
     </x:row>
@@ -10612,19 +10623,19 @@
       <x:c r="C33" s="100"/>
       <x:c r="D33" s="100"/>
       <x:c r="E33" s="56" t="s">
-        <x:v>249</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="F33" s="71"/>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="49"/>
       <x:c r="B34" s="79" t="s">
-        <x:v>83</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="C34" s="82"/>
       <x:c r="D34" s="82"/>
       <x:c r="E34" s="51" t="s">
-        <x:v>21</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F34" s="70"/>
     </x:row>
@@ -10634,7 +10645,7 @@
       <x:c r="C35" s="100"/>
       <x:c r="D35" s="100"/>
       <x:c r="E35" s="56" t="s">
-        <x:v>245</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F35" s="71"/>
     </x:row>

</xml_diff>

<commit_message>
add 0721 comment, 0722 goal
</commit_message>
<xml_diff>
--- a/2021_Summer/jp.hong/Datebook_jph.xlsx
+++ b/2021_Summer/jp.hong/Datebook_jph.xlsx
@@ -22,26 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="264">
-  <x:si>
-    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성
-2. 요구사항 정의 및 분석</x:t>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="266">
+  <x:si>
+    <x:t>1. 요구사항 분석 (실현성 확인)
+2. 데이터 흐름도 수정
+ - 차량 관련 새소식 창 삭제 및 다른 사항 수정
+3. Menu_Tree 작성
+4. Flow_Chart 작성
+5. 필요 자료 추가 조사
+ -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성 완료
+2. 요구사항 정의 및 분류
+ - 기능적 요구사항
+ - 비기능적 요구사항</x:t>
   </x:si>
   <x:si>
     <x:t>1. 실습 환경 설정 및 설명
@@ -55,19 +50,63 @@
  - 차량 관리 어플</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 요구사항 분석 (실현성 확인)
-2. 데이터 흐름도 수정
- - 차량 관련 새소식 창 삭제 및 다른 사항 수정
-3. Menu_Tree 작성
-4. Flow_Chart 작성
-5. 필요 자료 추가 조사
- -&gt; 주유, 부품들의 수명정보(?) 어떻게 자동으로 받아올지 알아봐야함 -&gt; 블루투스 =&gt; 블루투스 연동 어떻게?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 필요 자료 추가 조사
-2. 한계점 및 필요기술 추가
- - 차량 블루투스와 어플 연결 어떻게?
- - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
+    <x:t>1. 메뉴시퀀스 작성 (미완)
+2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. Git 목록 삭제
+2. 요구사항 분석
+3. 인터페이스 구상도 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사(관련 코드)
+2. FlowChart 수정 및 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
+2. 요구사항 추가 및 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 플로우 차트 작성
+2. 설계 계획서 작성
+3. Menu_Tree 도식화 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성(각 화면 기능 설명 채우기)
+2. 각 화면 플로우 차트 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 경쟁 어플 메뉴트리 수정
+2. 요구사항, 기능정의 순서 수정
+3. 한계점 수정
+블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. DateBook_Comment 부분 수정
+2. GIT보고서 수정
+ - 설치 과정 추가
+ - 명령어 부분 내용 추가
+3. PPT 머릿글 요약 작성 - (미완)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+ - 컴퓨터 견적 추천 앱
+ - 주차시 사고발생 알림 앱
+2. 주제 아이디어 최종 선정
+ - 차량 관리 어플
+3. 개발 계획서 및 요구사항 작성</x:t>
   </x:si>
   <x:si>
     <x:t>1. 현장실습 OT
@@ -80,6 +119,18 @@
  - 개발 설계</x:t>
   </x:si>
   <x:si>
+    <x:t>1. 06.22, 06.23 회의록 작성
+2. Git 환경 설정
+3. Git 설정 화면 캡처 및 보고서 작성
+4. 캡스톤 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 정의 및 분석 - 체계화
+ - 기능 / 비기능적 요구사항 분류 및 수정
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
     <x:t>1-1. Datebook Comment 부분 요약
 1-2. GIT 보고서 다시 작성
 1-3. PPT 머릿글 요약 작성
@@ -88,333 +139,532 @@
 2. 요구사항 수집 및 분석</x:t>
   </x:si>
   <x:si>
-    <x:t>차량 정보(오너들의 평균 정보)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리별 check list</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검내역서(정비소 제공 문서)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성(각 화면 기능 설명 채우기)
-2. 각 화면 플로우 차트 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 계획하고 있는 어플의 메뉴트리 작성 및 ppt 수정
-2. 요구사항 추가 및 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 플로우 차트 작성
-2. 설계 계획서 작성
-3. Menu_Tree 도식화 수정</x:t>
+    <x:t>내 차 정보 삭제</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:40
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 판매견적 받기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 형태로 존재</x:t>
+  </x:si>
+  <x:si>
+    <x:t>community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 기본 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:34
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보 수정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:22
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>진행 방향 ---&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자주 하는 질문</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서비스 (메뉴)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유사 모델 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 추천 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>09:00
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>친구 초대 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>운전자 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:33
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:43
+18:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험료 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약/견적 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 교체 예상 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰 보유 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 장착점 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 보험 선호도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소 지도 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Community</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:25
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:36
+18:02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인 쿠폰 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:32
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고장사례(리콜사례)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>데이터 연동 설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:23
+15:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 보험료 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:27
+18:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:30
+18:04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 플로우 마무리
+2. Setting창 화면 추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+ - 파일 헥사코드 분석 툴
+ - 헤더와 푸터를 이용한 카빙 툴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리에 메모한 사항 달력에 날짜 표시</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 플로우 작업
+2. 정비예약화면 아이콘 추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성(설명,컨테이너등 정보 채우기)
+2. 기능플로우 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 추가 자료조사
+2. 요구사항 추가 조사
+3. 경쟁 어플 기능 비교 보완</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 인터페이스 구상도 작성
+2. 요구사항 분류하여 수정
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+2. 요구사항 분석
+3. 구현 가능 여부 확인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 앱 화면별 Sequence 작성
+2. 앱 화면별 어떻게 구성할 것인지 구상
+3. 추가 자료조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약을 하는 과정에서 사용자가 선택한 지점과 선택된 지점의 정보가 일치해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 가입시 아이디, 비밀번호, 이름, 전화번호, 생년월일, 차종의 정보를 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알맞은 ID값과 패스워드 값이 입력 될 경우 그에 맞는 회원 정보가 로그인 되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 화면 시퀀스 작성 (설명, 커뮤니티, 알림, 설정화면 추가)
+2. 추가 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판의 글을 삭제하거나 올리기 위한 '글쓰기'버튼과 '글 삭제' 버튼이 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. vi 명령어 설명서 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰 등록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차 정보 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 목록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>경기/인천</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>어플 설정</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수리견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자차 게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 방문 장소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입</x:t>
+  </x:si>
+  <x:si>
+    <x:t>결함/리콜</x:t>
+  </x:si>
+  <x:si>
+    <x:t>모두의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공유게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 메뉴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>최신 글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>함수의 계산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록 및 통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공식 서비스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연비 랭킹</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 시세</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 예약</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨 필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 시기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클 이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tips</x:t>
+  </x:si>
+  <x:si>
+    <x:t>고객상담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메모 입력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비기능적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연차, 보험료</x:t>
+  </x:si>
+  <x:si>
+    <x:t>견적 요청</x:t>
+  </x:si>
+  <x:si>
+    <x:t>필요 기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Menu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오너들의 차고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>글 작성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>예약하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오늘 교체</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALL*</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>엔진오일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 후기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 주변 검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험사 선택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평균 연비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>디테일링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>setting</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Depth 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능 설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 항목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비 내역</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원 정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카카오톡 문의</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에어컨필터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>다이어리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>첫예약할인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수익적 요소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어샵</x:t>
+  </x:si>
+  <x:si>
+    <x:t>자동차 검사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용 가이드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>더 보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
+비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06_30 회의록 작성
+2. 요구사항 수정 및 관련 필요 자료 조사
+3. 15:00 ~ 지도교수 면담</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
+로그인 버튼이 나와야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출
+2. 최종 아이디어 선정
+3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
+2. 블루투스 관련 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 요구사항 수집 및 정의
+ - 관련 필요 자료 조사
+ - 기능적/ 비기능적 요구사항 내용 추가
+2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
   </x:si>
   <x:si>
     <x:t>1. (2-2) 수익적 요소 추가
 2. (4-1) 기능정의 추가
 3. 추가 자료 조사
  - 비슷한 어플(마이클) 화면 구성 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입을 위해 시도한 비밀번호가 7자리 이하이거나 13자리 이상일 경우
-비밀번호 입력 오류 메세지가 출력되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 화면 플로우 마무리
-2. Setting창 화면 추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. DateBook_Comment 부분 수정
-2. GIT보고서 수정
- - 설치 과정 추가
- - 명령어 부분 내용 추가
-3. PPT 머릿글 요약 작성 - (미완)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
- - 컴퓨터 견적 추천 앱
- - 주차시 사고발생 알림 앱
-2. 주제 아이디어 최종 선정
- - 차량 관리 어플
-3. 개발 계획서 및 요구사항 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 경쟁 어플 메뉴트리 수정
-2. 요구사항, 기능정의 순서 수정
-3. 한계점 수정
-블루투스 -&gt; 사진 촬영 ====&gt; 대체하게 되면 글자 인식하는 코드 필요</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Git 목록 삭제
-2. 요구사항 분석
-3. 인터페이스 구상도 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06.22, 06.23 회의록 작성
-2. Git 환경 설정
-3. Git 설정 화면 캡처 및 보고서 작성
-4. 캡스톤 아이디어 도출</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 정의 및 분석 - 체계화
- - 기능 / 비기능적 요구사항 분류 및 수정
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플 설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 화면 플로우 마무리
-2. 정비예약화면 아이콘 추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>선택 된 부품은 값의 변조 없이 알맞은 값이 저장되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입시 필요한 정보 및 소유한 차량의 정보를 포함해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유, 연비, 운행거리, 정비 및 기타비용 총액/월별 지출액</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품의 종류를 다르게 하여 여러가지를 선택 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사라지거나 위치가 바뀐 정보를 수시로 업데이트 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 날짜를 기록할 수 있도록 다이어리 형식으로 제공해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>등록된 사용자만이 자신이 등록한 차량의 정보를 확인해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수정 기능을 통해 작성했던 글을 수정 할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>외부에서 받아오는 정보(지도, 가격 등)에 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
- - 관련 필요 자료 조사
- - 기능적/ 비기능적 요구사항 내용 추가
-2. 개발에 필요한 요구사항 분석 (실현성 확인)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 앱 화면별 Sequence 작성
-2. 앱 화면별 어떻게 구성할 것인지 구상
-3. 추가 자료조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:34
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서비스 (메뉴)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:22
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 정보 삭제</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:40
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보 수정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재</x:t>
-  </x:si>
-  <x:si>
-    <x:t>진행 방향 ---&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자주 하는 질문</x:t>
-  </x:si>
-  <x:si>
-    <x:t>community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 판매견적 받기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 기본 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약/견적 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험료 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>09:00
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유사 모델 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:33
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 교체 예상 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:43
-18:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰 보유 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>친구 초대 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>운전자 추천 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 장착점 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 보험 선호도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:23
-15:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:25
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Community</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:32
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고장사례(리콜사례)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>데이터 연동 설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 보험료 확인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소 지도 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인 쿠폰 등록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:27
-18:05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:36
-18:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>08:30
-18:04</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출
-2. 최종 아이디어 선정
-3. 최종 아이디어 관련 자료, 필요 기술 정리, 문서화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 화면을 들어가게 되면 아이디와 비밀번호의 입력 창, 회원가입 버튼과
-로그인 버튼이 나와야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 06_30 회의록 작성
-2. 요구사항 수정 및 관련 필요 자료 조사
-3. 15:00 ~ 지도교수 면담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성(login, join, 내 차고, 차량 정보) 미완
-2. 블루투스 관련 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. vi 명령어 설명서 작성 완료
-2. 요구사항 정의 및 분류
- - 기능적 요구사항
- - 비기능적 요구사항</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인에 성공했다면 로그인 버튼이 아닌 로그 아웃 버튼을 보여주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성(설명,컨테이너등 정보 채우기)
-2. 기능플로우 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 추가 자료조사
-2. 요구사항 추가 조사
-3. 경쟁 어플 기능 비교 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디로 가입시도시 아이디 입력 오류 메세지가 출력되어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 인터페이스 구상도 작성
-2. 요구사항 분류하여 수정
-3. 추가 자료조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 요구사항 수집 및 정의
-2. 요구사항 분석
-3. 구현 가능 여부 확인</x:t>
   </x:si>
   <x:si>
     <x:t>1. 07.02 회의록 작성
@@ -431,504 +681,263 @@
 5. vi사용법 설명</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 추가 자료조사(관련 코드)
-2. FlowChart 수정 및 보완</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주행 거리 정보를 받아 계산하여 남은 수명에 대해 알려 주어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 메뉴시퀀스 작성 (미완)
-2. 스피너 및 캘린더 뷰 다이어리 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>소유한 차량이 여러 대일 경우 차량의 정보를 추가할 수 있어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비밀번호는 특수문자 포함 8자리 이상 12자리 이하 이어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>어플의 예약기능을 통해 예약한 경우 업체로부터 일정 수수료를 받는다.</x:t>
+    <x:t>주행 거리별 check list</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검내역서(정비소 제공 문서)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>교체할 부품을 선택 받아야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차량 정보(오너들의 평균 정보)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 필요 자료 추가 조사
+2. 한계점 및 필요기술 추가
+ - 차량 블루투스와 어플 연결 어떻게?
+ - 연결이 된다면 원하는 정보만 어떻게 가져 올건지?</x:t>
   </x:si>
   <x:si>
     <x:t>1. 각 버튼 및 창 기능 설명, 기능 플로우 추가</x:t>
   </x:si>
   <x:si>
-    <x:t>차 정보 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수리견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Goal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 목록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>경기/인천</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 방문 장소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원가입</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모두의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>모아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>결함/리콜</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자차 게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공식 서비스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연비 랭킹</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 시세</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Home</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 메뉴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>최신 글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>함수의 계산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨 필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공유게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 예약</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록 및 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클 이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 시기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>필요 기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>고객상담</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비기능적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메모 입력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연차, 보험료</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오너들의 차고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Menu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>견적 요청</x:t>
-  </x:si>
-  <x:si>
-    <x:t>글 작성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>예약하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능 설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용 가이드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALL*</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 주변 검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>첫예약할인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오늘 교체</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>카카오톡 문의</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평균 연비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 항목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>회원 정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>더 보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>엔진오일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>디테일링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>setting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차량 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에어컨필터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비 후기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Depth 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험사 선택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수익적 요소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>자동차 검사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어샵</x:t>
-  </x:si>
-  <x:si>
-    <x:t>서울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검</x:t>
-  </x:si>
-  <x:si>
-    <x:t>무결성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폭설철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>최신글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>달력</x:t>
-  </x:si>
-  <x:si>
-    <x:t>리뷰</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>비고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>손세차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가을</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기록</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상황별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>만족도</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Q&amp;A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보안성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>평점</x:t>
-  </x:si>
-  <x:si>
-    <x:t>설명</x:t>
-  </x:si>
-  <x:si>
-    <x:t>겨울</x:t>
-  </x:si>
-  <x:si>
-    <x:t>편집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>봄</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정보</x:t>
-  </x:si>
-  <x:si>
-    <x:t>검색</x:t>
-  </x:si>
-  <x:si>
-    <x:t>광고</x:t>
-  </x:si>
-  <x:si>
-    <x:t>타이어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>장마철</x:t>
-  </x:si>
-  <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기능</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인기글</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>홈</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정비</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쿠폰함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>채팅창</x:t>
-  </x:si>
-  <x:si>
-    <x:t>계절별</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>여름</x:t>
-  </x:si>
-  <x:si>
-    <x:t>연산</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이벤트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마이클</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유소 포인트 적립 연동</x:t>
-  </x:si>
-  <x:si>
-    <x:t>차종, 차번호, 연식 등</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이달의 정비/세차 혜택</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기아 커넥티드카 연동하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험료 확인 및 갱신일 알림</x:t>
-  </x:si>
-  <x:si>
-    <x:t>방문 정비소 기록, 메모</x:t>
-  </x:si>
-  <x:si>
-    <x:t>점검 스케쥴 및 일정 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>내 차 무료 판매 견적</x:t>
-  </x:si>
-  <x:si>
-    <x:t>항목 및 정비 주기 추가</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품 별 남은 수명 보여줌</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가까운 정비소 찾아보기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>다이어리에 메모한 사항 달력에 날짜 표시</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중복되는 아이디는 가입이 되어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판 형태로 존재, 결함/리콜 내역</x:t>
-  </x:si>
-  <x:si>
-    <x:t>정확한 위치의 지도 정보를 받아와야 한다.</x:t>
+    <x:t>1. Menu_Tree 수정(완료)
+2. 추가 자료 조사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 06.28 회의록 작성
+2. 요구사항 정의 및 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
   </x:si>
   <x:si>
     <x:t>게시판의 글들은 페이지당 20개씩 보여주어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
   </x:si>
   <x:si>
     <x:t>1. 요구사항 정의 및 분석 보완
 2. 기능정의 보완</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 06.28 회의록 작성
-2. 요구사항 정의 및 분석</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로그인 실패시 로그인 오류 메세지를 출력해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. Menu_Tree 수정(완료)
-2. 추가 자료 조사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>할인률, 총액의 계산 과정에 오류가 있어선 안된다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>채팅방 및 게시판에 들어가기 위해서는 로그인을 해야한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>보험, 범칙금, 주차요금, 톨게이트 비용, 차량용품 등</x:t>
-  </x:si>
-  <x:si>
-    <x:t>부품들의 시세변동을 지속적으로 업데이트 해야 한다.</x:t>
+    <x:t>만족도</x:t>
+  </x:si>
+  <x:si>
+    <x:t>평점</x:t>
+  </x:si>
+  <x:si>
+    <x:t>봄</x:t>
+  </x:si>
+  <x:si>
+    <x:t>설명</x:t>
+  </x:si>
+  <x:si>
+    <x:t>리뷰</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정보</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>겨울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인기글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>채팅창</x:t>
+  </x:si>
+  <x:si>
+    <x:t>손세차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>타이어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>홈</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비</x:t>
+  </x:si>
+  <x:si>
+    <x:t>정비소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보안성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q&amp;A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>광고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>장마철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>검색</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기능</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기록</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상황별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>편집</x:t>
+  </x:si>
+  <x:si>
+    <x:t>계절별</x:t>
+  </x:si>
+  <x:si>
+    <x:t>비고</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로그인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가을</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마이클</x:t>
+  </x:si>
+  <x:si>
+    <x:t>연산</x:t>
+  </x:si>
+  <x:si>
+    <x:t>여름</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이벤트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판</x:t>
+  </x:si>
+  <x:si>
+    <x:t>통계</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폭설철</x:t>
+  </x:si>
+  <x:si>
+    <x:t>최신글</x:t>
+  </x:si>
+  <x:si>
+    <x:t>서울</x:t>
+  </x:si>
+  <x:si>
+    <x:t>달력</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쿠폰</x:t>
+  </x:si>
+  <x:si>
+    <x:t>무결성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>부품 별 남은 수명 보여줌</x:t>
+  </x:si>
+  <x:si>
+    <x:t>점검 스케쥴 및 일정 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>방문 정비소 기록, 메모</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기아 커넥티드카 연동하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>차종, 차번호, 연식 등</x:t>
+  </x:si>
+  <x:si>
+    <x:t>보험료 확인 및 갱신일 알림</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가까운 정비소 찾아보기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유소 포인트 적립 연동</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이달의 정비/세차 혜택</x:t>
+  </x:si>
+  <x:si>
+    <x:t>항목 및 정비 주기 추가</x:t>
+  </x:si>
+  <x:si>
+    <x:t>내 차 무료 판매 견적</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 아이디어 도출</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1. 메뉴시퀀스 작성
+ - 화면별 세부기능 설계</x:t>
   </x:si>
   <x:si>
     <x:t>1. 화면 시퀀스 작성
 2. 추가 자료 조사</x:t>
   </x:si>
   <x:si>
-    <x:t>1. 메뉴시퀀스 작성
- - 화면별 세부기능 설계</x:t>
-  </x:si>
-  <x:si>
     <x:t>DB에 저장된 내용들은 변조가 없어야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
-  </x:si>
-  <x:si>
-    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
   </x:si>
   <x:si>
     <x:t>1. 계약서 작성
 2. 현장실습 오리엔테이션</x:t>
   </x:si>
   <x:si>
+    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주유량, 연비, 운행 거리 및 기타 비용 통계</x:t>
+  </x:si>
+  <x:si>
     <x:t>어플 내 광고를 통해 일정 수입료를 받는다.</x:t>
   </x:si>
   <x:si>
-    <x:t>아이콘을 활용하여 한 눈에 확인하기 쉬워야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>게시판을 이용하기 위해서는 로그인을 해야 한다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1. 아이디어 도출</x:t>
+    <x:t>APP종료시 입력된 데이터는 변조가 없어야 한다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>08:35
+18:03</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1493,7 +1502,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="100">
+  <x:cellXfs count="101">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -2004,6 +2013,19 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
@@ -2988,7 +3010,7 @@
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <x:pane xSplit="0" ySplit="2" topLeftCell="C18" activePane="bottomLeft" state="frozen"/>
-      <x:selection pane="bottomLeft" activeCell="E31" activeCellId="0" sqref="E31:E31"/>
+      <x:selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24:E24"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.199999999999999"/>
@@ -3004,16 +3026,16 @@
     <x:row r="1" ht="6.5999999999999996" customHeight="1"/>
     <x:row r="2" spans="2:5" ht="31.199999999999999" customHeight="1">
       <x:c r="B2" s="5" t="s">
-        <x:v>113</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C2" s="6" t="s">
-        <x:v>169</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D2" s="6" t="s">
-        <x:v>109</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="E2" s="7" t="s">
-        <x:v>140</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:5" ht="105.75">
@@ -3021,13 +3043,13 @@
         <x:v>44369</x:v>
       </x:c>
       <x:c r="C3" s="15" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D3" s="9" t="s">
         <x:v>259</x:v>
       </x:c>
       <x:c r="E3" s="9" t="s">
-        <x:v>9</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:5" ht="118.55">
@@ -3035,13 +3057,13 @@
         <x:v>44370</x:v>
       </x:c>
       <x:c r="C4" s="14" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="D4" s="12" t="s">
-        <x:v>26</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E4" s="12" t="s">
-        <x:v>6</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:5" ht="79.049999999999997">
@@ -3049,13 +3071,13 @@
         <x:v>44371</x:v>
       </x:c>
       <x:c r="C5" s="16" t="s">
-        <x:v>77</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D5" s="12" t="s">
-        <x:v>87</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="E5" s="12" t="s">
-        <x:v>22</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:5" ht="79.049999999999997">
@@ -3063,13 +3085,13 @@
         <x:v>44372</x:v>
       </x:c>
       <x:c r="C6" s="18" t="s">
-        <x:v>77</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D6" s="12" t="s">
-        <x:v>10</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E6" s="17" t="s">
-        <x:v>21</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5" ht="79.049999999999997">
@@ -3077,13 +3099,13 @@
         <x:v>44375</x:v>
       </x:c>
       <x:c r="C7" s="14" t="s">
-        <x:v>84</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D7" s="12" t="s">
-        <x:v>247</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="E7" s="12" t="s">
-        <x:v>99</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5" ht="52.700000000000003">
@@ -3091,13 +3113,13 @@
         <x:v>44376</x:v>
       </x:c>
       <x:c r="C8" s="14" t="s">
-        <x:v>81</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D8" s="12" t="s">
-        <x:v>5</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E8" s="12" t="s">
-        <x:v>91</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:5" ht="52.700000000000003">
@@ -3105,13 +3127,13 @@
         <x:v>44377</x:v>
       </x:c>
       <x:c r="C9" s="19" t="s">
-        <x:v>72</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D9" s="12" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E9" s="12" t="s">
-        <x:v>89</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:5" ht="52.700000000000003">
@@ -3119,13 +3141,13 @@
         <x:v>44378</x:v>
       </x:c>
       <x:c r="C10" s="20" t="s">
-        <x:v>75</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D10" s="12" t="s">
-        <x:v>97</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="E10" s="12" t="s">
-        <x:v>40</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:5" ht="65.849999999999994">
@@ -3133,13 +3155,13 @@
         <x:v>44379</x:v>
       </x:c>
       <x:c r="C11" s="22" t="s">
-        <x:v>80</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D11" s="12" t="s">
-        <x:v>24</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E11" s="12" t="s">
-        <x:v>98</x:v>
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:5" ht="105.40000000000001">
@@ -3147,13 +3169,13 @@
         <x:v>44382</x:v>
       </x:c>
       <x:c r="C12" s="21" t="s">
-        <x:v>73</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D12" s="12" t="s">
-        <x:v>96</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E12" s="12" t="s">
-        <x:v>7</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="2:5" ht="52.700000000000003">
@@ -3161,13 +3183,13 @@
         <x:v>44383</x:v>
       </x:c>
       <x:c r="C13" s="23" t="s">
-        <x:v>75</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D13" s="12" t="s">
-        <x:v>100</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="E13" s="12" t="s">
-        <x:v>8</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="2:5" ht="52.700000000000003">
@@ -3175,13 +3197,13 @@
         <x:v>44384</x:v>
       </x:c>
       <x:c r="C14" s="24" t="s">
-        <x:v>44</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D14" s="12" t="s">
-        <x:v>41</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E14" s="12" t="s">
-        <x:v>18</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="2:5" ht="52.700000000000003">
@@ -3189,13 +3211,13 @@
         <x:v>44385</x:v>
       </x:c>
       <x:c r="C15" s="30" t="s">
-        <x:v>55</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D15" s="12" t="s">
-        <x:v>94</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>23</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="2:5" ht="26.350000000000001">
@@ -3203,13 +3225,13 @@
         <x:v>44386</x:v>
       </x:c>
       <x:c r="C16" s="31" t="s">
-        <x:v>46</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D16" s="12" t="s">
-        <x:v>246</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="E16" s="12" t="s">
-        <x:v>16</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="2:5" ht="39.549999999999997">
@@ -3217,13 +3239,13 @@
         <x:v>44389</x:v>
       </x:c>
       <x:c r="C17" s="70" t="s">
-        <x:v>68</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D17" s="12" t="s">
-        <x:v>17</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>249</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="2:5" ht="26.350000000000001">
@@ -3231,13 +3253,13 @@
         <x:v>44390</x:v>
       </x:c>
       <x:c r="C18" s="71" t="s">
-        <x:v>63</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D18" s="12" t="s">
-        <x:v>254</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E18" s="12" t="s">
-        <x:v>90</x:v>
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="2:5" ht="26.350000000000001">
@@ -3245,13 +3267,13 @@
         <x:v>44391</x:v>
       </x:c>
       <x:c r="C19" s="71" t="s">
-        <x:v>75</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D19" s="12" t="s">
-        <x:v>254</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="E19" s="12" t="s">
-        <x:v>102</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="2:5" ht="26.350000000000001">
@@ -3259,13 +3281,13 @@
         <x:v>44392</x:v>
       </x:c>
       <x:c r="C20" s="14" t="s">
-        <x:v>85</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D20" s="12" t="s">
-        <x:v>4</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="E20" s="11" t="s">
-        <x:v>65</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="2:5" ht="26.350000000000001">
@@ -3273,13 +3295,13 @@
         <x:v>44393</x:v>
       </x:c>
       <x:c r="C21" s="72" t="s">
-        <x:v>60</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D21" s="12" t="s">
-        <x:v>93</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E21" s="12" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="2:5" ht="26.350000000000001">
@@ -3287,45 +3309,51 @@
         <x:v>44396</x:v>
       </x:c>
       <x:c r="C22" s="73" t="s">
-        <x:v>86</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="D22" s="11" t="s">
-        <x:v>106</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="E22" s="12" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="2:5" ht="26.350000000000001">
       <x:c r="B23" s="13">
         <x:v>44397</x:v>
       </x:c>
-      <x:c r="C23" s="99" t="s">
-        <x:v>42</x:v>
+      <x:c r="C23" s="74" t="s">
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D23" s="12" t="s">
-        <x:v>20</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E23" s="12" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="2:5">
+        <x:v>71</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="2:5" ht="39.549999999999997">
       <x:c r="B24" s="13">
         <x:v>44398</x:v>
       </x:c>
-      <x:c r="C24" s="10"/>
+      <x:c r="C24" s="100" t="s">
+        <x:v>265</x:v>
+      </x:c>
       <x:c r="D24" s="11" t="s">
-        <x:v>263</x:v>
-      </x:c>
-      <x:c r="E24" s="11"/>
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="E24" s="12" t="s">
+        <x:v>66</x:v>
+      </x:c>
     </x:row>
     <x:row r="25" spans="2:5">
       <x:c r="B25" s="13">
         <x:v>44399</x:v>
       </x:c>
       <x:c r="C25" s="10"/>
-      <x:c r="D25" s="11"/>
+      <x:c r="D25" s="11" t="s">
+        <x:v>255</x:v>
+      </x:c>
       <x:c r="E25" s="11"/>
     </x:row>
     <x:row r="26" spans="2:5">
@@ -3492,78 +3520,78 @@
   <x:sheetData>
     <x:row r="1" spans="1:9" ht="17.149999999999999">
       <x:c r="A1" s="26" t="s">
-        <x:v>49</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>153</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
-        <x:v>150</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D1" s="34" t="s">
-        <x:v>179</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="E1" s="34" t="s">
-        <x:v>135</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F1" s="34" t="s">
-        <x:v>124</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="G1" s="34" t="s">
-        <x:v>110</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="H1" s="34" t="s">
-        <x:v>217</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="I1" s="35" t="s">
-        <x:v>207</x:v>
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:9">
-      <x:c r="A2" s="82" t="s">
-        <x:v>229</x:v>
-      </x:c>
-      <x:c r="B2" s="76" t="s">
-        <x:v>220</x:v>
-      </x:c>
-      <x:c r="C2" s="79" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="D2" s="79" t="s">
-        <x:v>107</x:v>
+      <x:c r="A2" s="83" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B2" s="77" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="C2" s="80" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="D2" s="80" t="s">
+        <x:v>97</x:v>
       </x:c>
       <x:c r="E2" s="38" t="s">
-        <x:v>129</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F2" s="38"/>
       <x:c r="G2" s="38"/>
       <x:c r="H2" s="38"/>
       <x:c r="I2" s="38" t="s">
-        <x:v>52</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9">
-      <x:c r="A3" s="83"/>
-      <x:c r="B3" s="77"/>
-      <x:c r="C3" s="80"/>
-      <x:c r="D3" s="80"/>
+      <x:c r="A3" s="84"/>
+      <x:c r="B3" s="78"/>
+      <x:c r="C3" s="81"/>
+      <x:c r="D3" s="81"/>
       <x:c r="E3" s="37" t="s">
-        <x:v>67</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F3" s="37"/>
       <x:c r="G3" s="37"/>
       <x:c r="H3" s="37"/>
       <x:c r="I3" s="37" t="s">
-        <x:v>234</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
-      <x:c r="A4" s="83"/>
-      <x:c r="B4" s="77"/>
-      <x:c r="C4" s="80"/>
-      <x:c r="D4" s="80"/>
+      <x:c r="A4" s="84"/>
+      <x:c r="B4" s="78"/>
+      <x:c r="C4" s="81"/>
+      <x:c r="D4" s="81"/>
       <x:c r="E4" s="37" t="s">
-        <x:v>149</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="F4" s="37"/>
       <x:c r="G4" s="37"/>
@@ -3571,42 +3599,42 @@
       <x:c r="I4" s="37"/>
     </x:row>
     <x:row r="5" spans="1:9">
-      <x:c r="A5" s="83"/>
-      <x:c r="B5" s="77"/>
-      <x:c r="C5" s="80"/>
-      <x:c r="D5" s="80"/>
-      <x:c r="E5" s="74" t="s">
-        <x:v>122</x:v>
+      <x:c r="A5" s="84"/>
+      <x:c r="B5" s="78"/>
+      <x:c r="C5" s="81"/>
+      <x:c r="D5" s="81"/>
+      <x:c r="E5" s="75" t="s">
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F5" s="37" t="s">
-        <x:v>116</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G5" s="37"/>
       <x:c r="H5" s="37"/>
       <x:c r="I5" s="37"/>
     </x:row>
     <x:row r="6" spans="1:9">
-      <x:c r="A6" s="83"/>
-      <x:c r="B6" s="77"/>
-      <x:c r="C6" s="80"/>
-      <x:c r="D6" s="75"/>
-      <x:c r="E6" s="75"/>
+      <x:c r="A6" s="84"/>
+      <x:c r="B6" s="78"/>
+      <x:c r="C6" s="81"/>
+      <x:c r="D6" s="76"/>
+      <x:c r="E6" s="76"/>
       <x:c r="F6" s="37" t="s">
-        <x:v>45</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G6" s="37"/>
       <x:c r="H6" s="37"/>
       <x:c r="I6" s="37"/>
     </x:row>
     <x:row r="7" spans="1:9">
-      <x:c r="A7" s="83"/>
-      <x:c r="B7" s="77"/>
-      <x:c r="C7" s="80"/>
-      <x:c r="D7" s="74" t="s">
-        <x:v>131</x:v>
+      <x:c r="A7" s="84"/>
+      <x:c r="B7" s="78"/>
+      <x:c r="C7" s="81"/>
+      <x:c r="D7" s="75" t="s">
+        <x:v>118</x:v>
       </x:c>
       <x:c r="E7" s="37" t="s">
-        <x:v>200</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="F7" s="37"/>
       <x:c r="G7" s="37"/>
@@ -3614,91 +3642,91 @@
       <x:c r="I7" s="37"/>
     </x:row>
     <x:row r="8" spans="1:9">
-      <x:c r="A8" s="83"/>
-      <x:c r="B8" s="77"/>
-      <x:c r="C8" s="80"/>
-      <x:c r="D8" s="80"/>
+      <x:c r="A8" s="84"/>
+      <x:c r="B8" s="78"/>
+      <x:c r="C8" s="81"/>
+      <x:c r="D8" s="81"/>
       <x:c r="E8" s="37" t="s">
-        <x:v>192</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="F8" s="37"/>
       <x:c r="G8" s="37"/>
       <x:c r="H8" s="37"/>
       <x:c r="I8" s="37" t="s">
-        <x:v>33</x:v>
+        <x:v>86</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:9">
-      <x:c r="A9" s="83"/>
-      <x:c r="B9" s="77"/>
-      <x:c r="C9" s="80"/>
-      <x:c r="D9" s="80"/>
+      <x:c r="A9" s="84"/>
+      <x:c r="B9" s="78"/>
+      <x:c r="C9" s="81"/>
+      <x:c r="D9" s="81"/>
       <x:c r="E9" s="37" t="s">
-        <x:v>186</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="F9" s="37"/>
       <x:c r="G9" s="37"/>
       <x:c r="H9" s="37"/>
       <x:c r="I9" s="37" t="s">
-        <x:v>236</x:v>
+        <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
-      <x:c r="A10" s="83"/>
-      <x:c r="B10" s="77"/>
-      <x:c r="C10" s="80"/>
-      <x:c r="D10" s="80"/>
-      <x:c r="E10" s="74" t="s">
-        <x:v>112</x:v>
+      <x:c r="A10" s="84"/>
+      <x:c r="B10" s="78"/>
+      <x:c r="C10" s="81"/>
+      <x:c r="D10" s="81"/>
+      <x:c r="E10" s="75" t="s">
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F10" s="37" t="s">
-        <x:v>168</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="G10" s="37"/>
       <x:c r="H10" s="37"/>
       <x:c r="I10" s="37"/>
     </x:row>
     <x:row r="11" spans="1:9">
-      <x:c r="A11" s="83"/>
-      <x:c r="B11" s="77"/>
-      <x:c r="C11" s="80"/>
-      <x:c r="D11" s="80"/>
-      <x:c r="E11" s="80"/>
+      <x:c r="A11" s="84"/>
+      <x:c r="B11" s="78"/>
+      <x:c r="C11" s="81"/>
+      <x:c r="D11" s="81"/>
+      <x:c r="E11" s="81"/>
       <x:c r="F11" s="37" t="s">
-        <x:v>119</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="G11" s="37"/>
       <x:c r="H11" s="37"/>
       <x:c r="I11" s="37" t="s">
-        <x:v>252</x:v>
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
-      <x:c r="A12" s="83"/>
-      <x:c r="B12" s="77"/>
-      <x:c r="C12" s="80"/>
-      <x:c r="D12" s="80"/>
-      <x:c r="E12" s="80"/>
+      <x:c r="A12" s="84"/>
+      <x:c r="B12" s="78"/>
+      <x:c r="C12" s="81"/>
+      <x:c r="D12" s="81"/>
+      <x:c r="E12" s="81"/>
       <x:c r="F12" s="37" t="s">
-        <x:v>209</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="G12" s="37"/>
       <x:c r="H12" s="37"/>
       <x:c r="I12" s="37"/>
     </x:row>
     <x:row r="13" spans="1:28">
-      <x:c r="A13" s="83"/>
-      <x:c r="B13" s="77"/>
-      <x:c r="C13" s="75"/>
-      <x:c r="D13" s="75"/>
-      <x:c r="E13" s="75"/>
+      <x:c r="A13" s="84"/>
+      <x:c r="B13" s="78"/>
+      <x:c r="C13" s="76"/>
+      <x:c r="D13" s="76"/>
+      <x:c r="E13" s="76"/>
       <x:c r="F13" s="37" t="s">
-        <x:v>225</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="G13" s="37"/>
       <x:c r="H13" s="37"/>
       <x:c r="I13" s="37" t="s">
-        <x:v>238</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="J13" s="29"/>
       <x:c r="K13" s="29"/>
@@ -3721,22 +3749,22 @@
       <x:c r="AB13" s="29"/>
     </x:row>
     <x:row r="14" spans="1:28">
-      <x:c r="A14" s="83"/>
-      <x:c r="B14" s="77"/>
-      <x:c r="C14" s="74" t="s">
-        <x:v>120</x:v>
-      </x:c>
-      <x:c r="D14" s="74" t="s">
-        <x:v>115</x:v>
+      <x:c r="A14" s="84"/>
+      <x:c r="B14" s="78"/>
+      <x:c r="C14" s="75" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="D14" s="75" t="s">
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E14" s="37" t="s">
-        <x:v>206</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F14" s="37"/>
       <x:c r="G14" s="37"/>
       <x:c r="H14" s="37"/>
       <x:c r="I14" s="37" t="s">
-        <x:v>203</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="J14" s="29"/>
       <x:c r="K14" s="29"/>
@@ -3759,18 +3787,18 @@
       <x:c r="AB14" s="29"/>
     </x:row>
     <x:row r="15" spans="1:28">
-      <x:c r="A15" s="83"/>
-      <x:c r="B15" s="77"/>
-      <x:c r="C15" s="80"/>
-      <x:c r="D15" s="80"/>
+      <x:c r="A15" s="84"/>
+      <x:c r="B15" s="78"/>
+      <x:c r="C15" s="81"/>
+      <x:c r="D15" s="81"/>
       <x:c r="E15" s="37" t="s">
-        <x:v>167</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="F15" s="37"/>
       <x:c r="G15" s="37"/>
       <x:c r="H15" s="37"/>
       <x:c r="I15" s="37" t="s">
-        <x:v>128</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="J15" s="29"/>
       <x:c r="K15" s="29"/>
@@ -3793,12 +3821,12 @@
       <x:c r="AB15" s="29"/>
     </x:row>
     <x:row r="16" spans="1:28">
-      <x:c r="A16" s="83"/>
-      <x:c r="B16" s="77"/>
-      <x:c r="C16" s="80"/>
-      <x:c r="D16" s="80"/>
+      <x:c r="A16" s="84"/>
+      <x:c r="B16" s="78"/>
+      <x:c r="C16" s="81"/>
+      <x:c r="D16" s="81"/>
       <x:c r="E16" s="37" t="s">
-        <x:v>178</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="F16" s="37"/>
       <x:c r="G16" s="37"/>
@@ -3824,18 +3852,18 @@
       <x:c r="AB16" s="29"/>
     </x:row>
     <x:row r="17" spans="1:28">
-      <x:c r="A17" s="83"/>
-      <x:c r="B17" s="77"/>
-      <x:c r="C17" s="80"/>
-      <x:c r="D17" s="75"/>
+      <x:c r="A17" s="84"/>
+      <x:c r="B17" s="78"/>
+      <x:c r="C17" s="81"/>
+      <x:c r="D17" s="76"/>
       <x:c r="E17" s="37" t="s">
-        <x:v>123</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F17" s="37"/>
       <x:c r="G17" s="37"/>
       <x:c r="H17" s="37"/>
       <x:c r="I17" s="37" t="s">
-        <x:v>243</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="J17" s="29"/>
       <x:c r="K17" s="29"/>
@@ -3858,17 +3886,17 @@
       <x:c r="AB17" s="29"/>
     </x:row>
     <x:row r="18" spans="1:28">
-      <x:c r="A18" s="83"/>
-      <x:c r="B18" s="77"/>
-      <x:c r="C18" s="80"/>
+      <x:c r="A18" s="84"/>
+      <x:c r="B18" s="78"/>
+      <x:c r="C18" s="81"/>
       <x:c r="D18" s="37" t="s">
-        <x:v>71</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E18" s="37" t="s">
-        <x:v>57</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F18" s="37" t="s">
-        <x:v>180</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="G18" s="37"/>
       <x:c r="H18" s="37"/>
@@ -3894,18 +3922,18 @@
       <x:c r="AB18" s="29"/>
     </x:row>
     <x:row r="19" spans="1:28">
-      <x:c r="A19" s="83"/>
-      <x:c r="B19" s="77"/>
-      <x:c r="C19" s="80"/>
+      <x:c r="A19" s="84"/>
+      <x:c r="B19" s="78"/>
+      <x:c r="C19" s="81"/>
       <x:c r="D19" s="37" t="s">
-        <x:v>194</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="E19" s="37"/>
       <x:c r="F19" s="37"/>
       <x:c r="G19" s="37"/>
       <x:c r="H19" s="37"/>
-      <x:c r="I19" s="74" t="s">
-        <x:v>48</x:v>
+      <x:c r="I19" s="75" t="s">
+        <x:v>23</x:v>
       </x:c>
       <x:c r="J19" s="29"/>
       <x:c r="K19" s="29"/>
@@ -3928,17 +3956,17 @@
       <x:c r="AB19" s="29"/>
     </x:row>
     <x:row r="20" spans="1:28">
-      <x:c r="A20" s="83"/>
-      <x:c r="B20" s="77"/>
-      <x:c r="C20" s="80"/>
+      <x:c r="A20" s="84"/>
+      <x:c r="B20" s="78"/>
+      <x:c r="C20" s="81"/>
       <x:c r="D20" s="37" t="s">
-        <x:v>123</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="E20" s="37"/>
       <x:c r="F20" s="37"/>
       <x:c r="G20" s="37"/>
       <x:c r="H20" s="37"/>
-      <x:c r="I20" s="80"/>
+      <x:c r="I20" s="81"/>
       <x:c r="J20" s="29"/>
       <x:c r="K20" s="29"/>
       <x:c r="L20" s="29"/>
@@ -3960,17 +3988,17 @@
       <x:c r="AB20" s="29"/>
     </x:row>
     <x:row r="21" spans="1:28">
-      <x:c r="A21" s="83"/>
-      <x:c r="B21" s="77"/>
-      <x:c r="C21" s="80"/>
+      <x:c r="A21" s="84"/>
+      <x:c r="B21" s="78"/>
+      <x:c r="C21" s="81"/>
       <x:c r="D21" s="37" t="s">
-        <x:v>178</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="E21" s="37"/>
       <x:c r="F21" s="37"/>
       <x:c r="G21" s="37"/>
       <x:c r="H21" s="37"/>
-      <x:c r="I21" s="75"/>
+      <x:c r="I21" s="76"/>
       <x:c r="J21" s="29"/>
       <x:c r="K21" s="29"/>
       <x:c r="L21" s="29"/>
@@ -3992,11 +4020,11 @@
       <x:c r="AB21" s="29"/>
     </x:row>
     <x:row r="22" spans="1:28">
-      <x:c r="A22" s="83"/>
-      <x:c r="B22" s="78"/>
-      <x:c r="C22" s="75"/>
+      <x:c r="A22" s="84"/>
+      <x:c r="B22" s="79"/>
+      <x:c r="C22" s="76"/>
       <x:c r="D22" s="37" t="s">
-        <x:v>59</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E22" s="37"/>
       <x:c r="F22" s="37"/>
@@ -4024,12 +4052,12 @@
       <x:c r="AB22" s="29"/>
     </x:row>
     <x:row r="23" spans="1:28">
-      <x:c r="A23" s="83"/>
-      <x:c r="B23" s="81" t="s">
-        <x:v>139</x:v>
+      <x:c r="A23" s="84"/>
+      <x:c r="B23" s="82" t="s">
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C23" s="37" t="s">
-        <x:v>54</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D23" s="37"/>
       <x:c r="E23" s="37"/>
@@ -4058,10 +4086,10 @@
       <x:c r="AB23" s="29"/>
     </x:row>
     <x:row r="24" spans="1:28">
-      <x:c r="A24" s="83"/>
-      <x:c r="B24" s="77"/>
+      <x:c r="A24" s="84"/>
+      <x:c r="B24" s="78"/>
       <x:c r="C24" s="37" t="s">
-        <x:v>185</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="D24" s="37"/>
       <x:c r="E24" s="37"/>
@@ -4090,10 +4118,10 @@
       <x:c r="AB24" s="29"/>
     </x:row>
     <x:row r="25" spans="1:28">
-      <x:c r="A25" s="83"/>
-      <x:c r="B25" s="77"/>
+      <x:c r="A25" s="84"/>
+      <x:c r="B25" s="78"/>
       <x:c r="C25" s="37" t="s">
-        <x:v>212</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="D25" s="37"/>
       <x:c r="E25" s="37"/>
@@ -4122,16 +4150,16 @@
       <x:c r="AB25" s="29"/>
     </x:row>
     <x:row r="26" spans="1:87">
-      <x:c r="A26" s="83"/>
-      <x:c r="B26" s="77"/>
-      <x:c r="C26" s="74" t="s">
-        <x:v>139</x:v>
+      <x:c r="A26" s="84"/>
+      <x:c r="B26" s="78"/>
+      <x:c r="C26" s="75" t="s">
+        <x:v>129</x:v>
       </x:c>
       <x:c r="D26" s="37" t="s">
-        <x:v>172</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="E26" s="37" t="s">
-        <x:v>56</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F26" s="37"/>
       <x:c r="G26" s="37"/>
@@ -4217,17 +4245,17 @@
       <x:c r="CI26" s="29"/>
     </x:row>
     <x:row r="27" spans="1:87" s="1" customFormat="1">
-      <x:c r="A27" s="82"/>
-      <x:c r="B27" s="81"/>
-      <x:c r="C27" s="80"/>
-      <x:c r="D27" s="74" t="s">
-        <x:v>214</x:v>
+      <x:c r="A27" s="83"/>
+      <x:c r="B27" s="82"/>
+      <x:c r="C27" s="81"/>
+      <x:c r="D27" s="75" t="s">
+        <x:v>209</x:v>
       </x:c>
       <x:c r="E27" s="37" t="s">
-        <x:v>163</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F27" s="37" t="s">
-        <x:v>70</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G27" s="37"/>
       <x:c r="H27" s="37"/>
@@ -4312,15 +4340,15 @@
       <x:c r="CI27" s="29"/>
     </x:row>
     <x:row r="28" spans="1:87">
-      <x:c r="A28" s="83"/>
-      <x:c r="B28" s="77"/>
-      <x:c r="C28" s="80"/>
-      <x:c r="D28" s="75"/>
+      <x:c r="A28" s="84"/>
+      <x:c r="B28" s="78"/>
+      <x:c r="C28" s="81"/>
+      <x:c r="D28" s="76"/>
       <x:c r="E28" s="37" t="s">
-        <x:v>138</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F28" s="37" t="s">
-        <x:v>70</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="G28" s="37"/>
       <x:c r="H28" s="37"/>
@@ -4405,14 +4433,14 @@
       <x:c r="CI28" s="29"/>
     </x:row>
     <x:row r="29" spans="1:87">
-      <x:c r="A29" s="83"/>
-      <x:c r="B29" s="77"/>
-      <x:c r="C29" s="80"/>
+      <x:c r="A29" s="84"/>
+      <x:c r="B29" s="78"/>
+      <x:c r="C29" s="81"/>
       <x:c r="D29" s="37" t="s">
-        <x:v>108</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="E29" s="39" t="s">
-        <x:v>154</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F29" s="39"/>
       <x:c r="G29" s="37"/>
@@ -4498,14 +4526,14 @@
       <x:c r="CI29" s="29"/>
     </x:row>
     <x:row r="30" spans="1:87">
-      <x:c r="A30" s="83"/>
-      <x:c r="B30" s="77"/>
-      <x:c r="C30" s="80"/>
+      <x:c r="A30" s="84"/>
+      <x:c r="B30" s="78"/>
+      <x:c r="C30" s="81"/>
       <x:c r="D30" s="37" t="s">
-        <x:v>173</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="E30" s="37" t="s">
-        <x:v>184</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="F30" s="37"/>
       <x:c r="G30" s="37"/>
@@ -4591,12 +4619,12 @@
       <x:c r="CI30" s="29"/>
     </x:row>
     <x:row r="31" spans="1:87" s="1" customFormat="1">
-      <x:c r="A31" s="82"/>
-      <x:c r="B31" s="81"/>
-      <x:c r="C31" s="80"/>
+      <x:c r="A31" s="83"/>
+      <x:c r="B31" s="82"/>
+      <x:c r="C31" s="81"/>
       <x:c r="D31" s="37"/>
       <x:c r="E31" s="37" t="s">
-        <x:v>114</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F31" s="37"/>
       <x:c r="G31" s="37"/>
@@ -4682,14 +4710,14 @@
       <x:c r="CI31" s="29"/>
     </x:row>
     <x:row r="32" spans="1:87">
-      <x:c r="A32" s="83"/>
-      <x:c r="B32" s="77"/>
-      <x:c r="C32" s="80"/>
+      <x:c r="A32" s="84"/>
+      <x:c r="B32" s="78"/>
+      <x:c r="C32" s="81"/>
       <x:c r="D32" s="37" t="s">
-        <x:v>176</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="E32" s="37" t="s">
-        <x:v>117</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F32" s="37"/>
       <x:c r="G32" s="37"/>
@@ -4775,11 +4803,11 @@
       <x:c r="CI32" s="29"/>
     </x:row>
     <x:row r="33" spans="1:87">
-      <x:c r="A33" s="83"/>
-      <x:c r="B33" s="77"/>
-      <x:c r="C33" s="75"/>
+      <x:c r="A33" s="84"/>
+      <x:c r="B33" s="78"/>
+      <x:c r="C33" s="76"/>
       <x:c r="D33" s="37" t="s">
-        <x:v>162</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="E33" s="37"/>
       <x:c r="F33" s="37"/>
@@ -4866,13 +4894,13 @@
       <x:c r="CI33" s="29"/>
     </x:row>
     <x:row r="34" spans="1:87" s="1" customFormat="1">
-      <x:c r="A34" s="82"/>
-      <x:c r="B34" s="81"/>
-      <x:c r="C34" s="74" t="s">
-        <x:v>161</x:v>
+      <x:c r="A34" s="83"/>
+      <x:c r="B34" s="82"/>
+      <x:c r="C34" s="75" t="s">
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D34" s="37" t="s">
-        <x:v>127</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="E34" s="37"/>
       <x:c r="F34" s="37"/>
@@ -4959,11 +4987,11 @@
       <x:c r="CI34" s="29"/>
     </x:row>
     <x:row r="35" spans="1:87" s="1" customFormat="1">
-      <x:c r="A35" s="83"/>
-      <x:c r="B35" s="77"/>
-      <x:c r="C35" s="80"/>
+      <x:c r="A35" s="84"/>
+      <x:c r="B35" s="78"/>
+      <x:c r="C35" s="81"/>
       <x:c r="D35" s="37" t="s">
-        <x:v>196</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="E35" s="37"/>
       <x:c r="F35" s="37"/>
@@ -5050,11 +5078,11 @@
       <x:c r="CI35" s="29"/>
     </x:row>
     <x:row r="36" spans="1:87" s="1" customFormat="1">
-      <x:c r="A36" s="83"/>
-      <x:c r="B36" s="77"/>
-      <x:c r="C36" s="80"/>
+      <x:c r="A36" s="84"/>
+      <x:c r="B36" s="78"/>
+      <x:c r="C36" s="81"/>
       <x:c r="D36" s="37" t="s">
-        <x:v>201</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="E36" s="37"/>
       <x:c r="F36" s="37"/>
@@ -5141,11 +5169,11 @@
       <x:c r="CI36" s="29"/>
     </x:row>
     <x:row r="37" spans="1:87" s="1" customFormat="1">
-      <x:c r="A37" s="83"/>
-      <x:c r="B37" s="77"/>
-      <x:c r="C37" s="80"/>
+      <x:c r="A37" s="84"/>
+      <x:c r="B37" s="78"/>
+      <x:c r="C37" s="81"/>
       <x:c r="D37" s="37" t="s">
-        <x:v>198</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="E37" s="37"/>
       <x:c r="F37" s="37"/>
@@ -5232,11 +5260,11 @@
       <x:c r="CI37" s="29"/>
     </x:row>
     <x:row r="38" spans="1:87" s="1" customFormat="1">
-      <x:c r="A38" s="83"/>
-      <x:c r="B38" s="77"/>
-      <x:c r="C38" s="80"/>
+      <x:c r="A38" s="84"/>
+      <x:c r="B38" s="78"/>
+      <x:c r="C38" s="81"/>
       <x:c r="D38" s="37" t="s">
-        <x:v>183</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="E38" s="37"/>
       <x:c r="F38" s="37"/>
@@ -5323,11 +5351,11 @@
       <x:c r="CI38" s="29"/>
     </x:row>
     <x:row r="39" spans="1:87" s="1" customFormat="1">
-      <x:c r="A39" s="82"/>
-      <x:c r="B39" s="81"/>
-      <x:c r="C39" s="75"/>
+      <x:c r="A39" s="83"/>
+      <x:c r="B39" s="82"/>
+      <x:c r="C39" s="76"/>
       <x:c r="D39" s="37" t="s">
-        <x:v>182</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="E39" s="37"/>
       <x:c r="F39" s="37"/>
@@ -5414,12 +5442,12 @@
       <x:c r="CI39" s="29"/>
     </x:row>
     <x:row r="40" spans="1:87">
-      <x:c r="A40" s="83"/>
-      <x:c r="B40" s="81" t="s">
-        <x:v>188</x:v>
+      <x:c r="A40" s="84"/>
+      <x:c r="B40" s="82" t="s">
+        <x:v>235</x:v>
       </x:c>
       <x:c r="C40" s="37" t="s">
-        <x:v>218</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="D40" s="37"/>
       <x:c r="E40" s="37"/>
@@ -5507,10 +5535,10 @@
       <x:c r="CI40" s="29"/>
     </x:row>
     <x:row r="41" spans="1:87">
-      <x:c r="A41" s="83"/>
-      <x:c r="B41" s="77"/>
+      <x:c r="A41" s="84"/>
+      <x:c r="B41" s="78"/>
       <x:c r="C41" s="37" t="s">
-        <x:v>132</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="D41" s="37"/>
       <x:c r="E41" s="37"/>
@@ -5598,10 +5626,10 @@
       <x:c r="CI41" s="29"/>
     </x:row>
     <x:row r="42" spans="1:87">
-      <x:c r="A42" s="83"/>
-      <x:c r="B42" s="77"/>
+      <x:c r="A42" s="84"/>
+      <x:c r="B42" s="78"/>
       <x:c r="C42" s="37" t="s">
-        <x:v>125</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="D42" s="37"/>
       <x:c r="E42" s="37"/>
@@ -5689,10 +5717,10 @@
       <x:c r="CI42" s="29"/>
     </x:row>
     <x:row r="43" spans="1:87">
-      <x:c r="A43" s="83"/>
-      <x:c r="B43" s="77"/>
+      <x:c r="A43" s="84"/>
+      <x:c r="B43" s="78"/>
       <x:c r="C43" s="37" t="s">
-        <x:v>146</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="D43" s="37"/>
       <x:c r="E43" s="37"/>
@@ -5780,10 +5808,10 @@
       <x:c r="CI43" s="29"/>
     </x:row>
     <x:row r="44" spans="1:87">
-      <x:c r="A44" s="83"/>
-      <x:c r="B44" s="77"/>
+      <x:c r="A44" s="84"/>
+      <x:c r="B44" s="78"/>
       <x:c r="C44" s="37" t="s">
-        <x:v>212</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="D44" s="37"/>
       <x:c r="E44" s="37"/>
@@ -5871,10 +5899,10 @@
       <x:c r="CI44" s="29"/>
     </x:row>
     <x:row r="45" spans="1:87">
-      <x:c r="A45" s="83"/>
-      <x:c r="B45" s="78"/>
+      <x:c r="A45" s="84"/>
+      <x:c r="B45" s="79"/>
       <x:c r="C45" s="37" t="s">
-        <x:v>155</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D45" s="37"/>
       <x:c r="E45" s="37"/>
@@ -5962,12 +5990,12 @@
       <x:c r="CI45" s="29"/>
     </x:row>
     <x:row r="46" spans="1:87">
-      <x:c r="A46" s="83"/>
-      <x:c r="B46" s="81" t="s">
-        <x:v>219</x:v>
+      <x:c r="A46" s="84"/>
+      <x:c r="B46" s="82" t="s">
+        <x:v>204</x:v>
       </x:c>
       <x:c r="C46" s="37" t="s">
-        <x:v>213</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D46" s="37"/>
       <x:c r="E46" s="37"/>
@@ -6055,10 +6083,10 @@
       <x:c r="CI46" s="29"/>
     </x:row>
     <x:row r="47" spans="1:87">
-      <x:c r="A47" s="83"/>
-      <x:c r="B47" s="77"/>
+      <x:c r="A47" s="84"/>
+      <x:c r="B47" s="78"/>
       <x:c r="C47" s="37" t="s">
-        <x:v>228</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="D47" s="37"/>
       <x:c r="E47" s="37"/>
@@ -6146,10 +6174,10 @@
       <x:c r="CI47" s="29"/>
     </x:row>
     <x:row r="48" spans="1:87">
-      <x:c r="A48" s="83"/>
-      <x:c r="B48" s="77"/>
+      <x:c r="A48" s="84"/>
+      <x:c r="B48" s="78"/>
       <x:c r="C48" s="37" t="s">
-        <x:v>144</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D48" s="37"/>
       <x:c r="E48" s="37"/>
@@ -6237,10 +6265,10 @@
       <x:c r="CI48" s="29"/>
     </x:row>
     <x:row r="49" spans="1:87">
-      <x:c r="A49" s="83"/>
-      <x:c r="B49" s="78"/>
+      <x:c r="A49" s="84"/>
+      <x:c r="B49" s="79"/>
       <x:c r="C49" s="37" t="s">
-        <x:v>166</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="D49" s="37"/>
       <x:c r="E49" s="37"/>
@@ -6328,15 +6356,15 @@
       <x:c r="CI49" s="29"/>
     </x:row>
     <x:row r="50" spans="1:87">
-      <x:c r="A50" s="83"/>
-      <x:c r="B50" s="81" t="s">
-        <x:v>171</x:v>
-      </x:c>
-      <x:c r="C50" s="74" t="s">
-        <x:v>54</x:v>
+      <x:c r="A50" s="84"/>
+      <x:c r="B50" s="82" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="C50" s="75" t="s">
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D50" s="37" t="s">
-        <x:v>133</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="E50" s="37"/>
       <x:c r="F50" s="37"/>
@@ -6423,11 +6451,11 @@
       <x:c r="CI50" s="29"/>
     </x:row>
     <x:row r="51" spans="1:87">
-      <x:c r="A51" s="83"/>
-      <x:c r="B51" s="77"/>
-      <x:c r="C51" s="75"/>
+      <x:c r="A51" s="84"/>
+      <x:c r="B51" s="78"/>
+      <x:c r="C51" s="76"/>
       <x:c r="D51" s="37" t="s">
-        <x:v>165</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="E51" s="37"/>
       <x:c r="F51" s="37"/>
@@ -6514,13 +6542,13 @@
       <x:c r="CI51" s="29"/>
     </x:row>
     <x:row r="52" spans="1:87">
-      <x:c r="A52" s="83"/>
-      <x:c r="B52" s="77"/>
-      <x:c r="C52" s="74" t="s">
-        <x:v>222</x:v>
+      <x:c r="A52" s="84"/>
+      <x:c r="B52" s="78"/>
+      <x:c r="C52" s="75" t="s">
+        <x:v>221</x:v>
       </x:c>
       <x:c r="D52" s="37" t="s">
-        <x:v>83</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E52" s="37"/>
       <x:c r="F52" s="37"/>
@@ -6607,11 +6635,11 @@
       <x:c r="CI52" s="29"/>
     </x:row>
     <x:row r="53" spans="1:87">
-      <x:c r="A53" s="83"/>
-      <x:c r="B53" s="77"/>
-      <x:c r="C53" s="75"/>
+      <x:c r="A53" s="84"/>
+      <x:c r="B53" s="78"/>
+      <x:c r="C53" s="76"/>
       <x:c r="D53" s="37" t="s">
-        <x:v>64</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E53" s="37"/>
       <x:c r="F53" s="37"/>
@@ -6698,13 +6726,13 @@
       <x:c r="CI53" s="29"/>
     </x:row>
     <x:row r="54" spans="1:87">
-      <x:c r="A54" s="83"/>
-      <x:c r="B54" s="77"/>
-      <x:c r="C54" s="74" t="s">
-        <x:v>69</x:v>
+      <x:c r="A54" s="84"/>
+      <x:c r="B54" s="78"/>
+      <x:c r="C54" s="75" t="s">
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D54" s="37" t="s">
-        <x:v>79</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E54" s="37"/>
       <x:c r="F54" s="37"/>
@@ -6791,11 +6819,11 @@
       <x:c r="CI54" s="29"/>
     </x:row>
     <x:row r="55" spans="1:87">
-      <x:c r="A55" s="83"/>
-      <x:c r="B55" s="77"/>
-      <x:c r="C55" s="80"/>
+      <x:c r="A55" s="84"/>
+      <x:c r="B55" s="78"/>
+      <x:c r="C55" s="81"/>
       <x:c r="D55" s="37" t="s">
-        <x:v>62</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E55" s="37"/>
       <x:c r="F55" s="37"/>
@@ -6882,11 +6910,11 @@
       <x:c r="CI55" s="29"/>
     </x:row>
     <x:row r="56" spans="1:87">
-      <x:c r="A56" s="83"/>
-      <x:c r="B56" s="77"/>
-      <x:c r="C56" s="75"/>
+      <x:c r="A56" s="84"/>
+      <x:c r="B56" s="78"/>
+      <x:c r="C56" s="76"/>
       <x:c r="D56" s="37" t="s">
-        <x:v>237</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="E56" s="37"/>
       <x:c r="F56" s="37"/>
@@ -6973,13 +7001,13 @@
       <x:c r="CI56" s="29"/>
     </x:row>
     <x:row r="57" spans="1:87">
-      <x:c r="A57" s="83"/>
-      <x:c r="B57" s="77"/>
-      <x:c r="C57" s="74" t="s">
-        <x:v>143</x:v>
+      <x:c r="A57" s="84"/>
+      <x:c r="B57" s="78"/>
+      <x:c r="C57" s="75" t="s">
+        <x:v>134</x:v>
       </x:c>
       <x:c r="D57" s="37" t="s">
-        <x:v>232</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="E57" s="37"/>
       <x:c r="F57" s="37"/>
@@ -7066,11 +7094,11 @@
       <x:c r="CI57" s="29"/>
     </x:row>
     <x:row r="58" spans="1:87">
-      <x:c r="A58" s="83"/>
-      <x:c r="B58" s="77"/>
-      <x:c r="C58" s="75"/>
+      <x:c r="A58" s="84"/>
+      <x:c r="B58" s="78"/>
+      <x:c r="C58" s="76"/>
       <x:c r="D58" s="37" t="s">
-        <x:v>66</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E58" s="37"/>
       <x:c r="F58" s="37"/>
@@ -7157,13 +7185,13 @@
       <x:c r="CI58" s="29"/>
     </x:row>
     <x:row r="59" spans="1:87">
-      <x:c r="A59" s="83"/>
-      <x:c r="B59" s="77"/>
-      <x:c r="C59" s="74" t="s">
-        <x:v>78</x:v>
+      <x:c r="A59" s="84"/>
+      <x:c r="B59" s="78"/>
+      <x:c r="C59" s="75" t="s">
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D59" s="37" t="s">
-        <x:v>233</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="E59" s="37"/>
       <x:c r="F59" s="37"/>
@@ -7250,11 +7278,11 @@
       <x:c r="CI59" s="29"/>
     </x:row>
     <x:row r="60" spans="1:87">
-      <x:c r="A60" s="83"/>
-      <x:c r="B60" s="77"/>
-      <x:c r="C60" s="75"/>
+      <x:c r="A60" s="84"/>
+      <x:c r="B60" s="78"/>
+      <x:c r="C60" s="76"/>
       <x:c r="D60" s="37" t="s">
-        <x:v>230</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="E60" s="37"/>
       <x:c r="F60" s="37"/>
@@ -7341,13 +7369,13 @@
       <x:c r="CI60" s="29"/>
     </x:row>
     <x:row r="61" spans="1:87">
-      <x:c r="A61" s="83"/>
-      <x:c r="B61" s="77"/>
-      <x:c r="C61" s="74" t="s">
-        <x:v>159</x:v>
+      <x:c r="A61" s="84"/>
+      <x:c r="B61" s="78"/>
+      <x:c r="C61" s="75" t="s">
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D61" s="37" t="s">
-        <x:v>204</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="E61" s="37"/>
       <x:c r="F61" s="37"/>
@@ -7434,11 +7462,11 @@
       <x:c r="CI61" s="29"/>
     </x:row>
     <x:row r="62" spans="1:87">
-      <x:c r="A62" s="84"/>
-      <x:c r="B62" s="78"/>
-      <x:c r="C62" s="75"/>
+      <x:c r="A62" s="85"/>
+      <x:c r="B62" s="79"/>
+      <x:c r="C62" s="76"/>
       <x:c r="D62" s="37" t="s">
-        <x:v>147</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E62" s="37"/>
       <x:c r="F62" s="37"/>
@@ -9480,288 +9508,288 @@
   <x:sheetData>
     <x:row r="1" spans="1:8" ht="17.149999999999999">
       <x:c r="A1" s="32" t="s">
-        <x:v>49</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B1" s="33" t="s">
-        <x:v>153</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C1" s="34" t="s">
-        <x:v>150</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D1" s="34" t="s">
-        <x:v>179</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="E1" s="34" t="s">
-        <x:v>135</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F1" s="34" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="G1" s="34" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="H1" s="35" t="s">
+        <x:v>227</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8" ht="16.75" customHeight="1">
+      <x:c r="A2" s="83" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="B2" s="77" t="s">
         <x:v>124</x:v>
       </x:c>
-      <x:c r="G1" s="34" t="s">
-        <x:v>217</x:v>
-      </x:c>
-      <x:c r="H1" s="35" t="s">
-        <x:v>197</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:8" ht="16.75" customHeight="1">
-      <x:c r="A2" s="82" t="s">
-        <x:v>175</x:v>
-      </x:c>
-      <x:c r="B2" s="76" t="s">
-        <x:v>130</x:v>
-      </x:c>
-      <x:c r="C2" s="89" t="s">
-        <x:v>111</x:v>
-      </x:c>
-      <x:c r="D2" s="87" t="s">
-        <x:v>115</x:v>
+      <x:c r="C2" s="90" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="D2" s="88" t="s">
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E2" s="58" t="s">
-        <x:v>53</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F2" s="58"/>
       <x:c r="G2" s="58"/>
       <x:c r="H2" s="58" t="s">
-        <x:v>231</x:v>
+        <x:v>248</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
-      <x:c r="A3" s="83"/>
-      <x:c r="B3" s="77"/>
-      <x:c r="C3" s="90"/>
-      <x:c r="D3" s="88"/>
+      <x:c r="A3" s="84"/>
+      <x:c r="B3" s="78"/>
+      <x:c r="C3" s="91"/>
+      <x:c r="D3" s="89"/>
       <x:c r="E3" s="59" t="s">
-        <x:v>157</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="F3" s="59"/>
       <x:c r="G3" s="59"/>
       <x:c r="H3" s="59" t="s">
-        <x:v>151</x:v>
+        <x:v>139</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
-      <x:c r="A4" s="83"/>
-      <x:c r="B4" s="77"/>
-      <x:c r="C4" s="90"/>
-      <x:c r="D4" s="86"/>
+      <x:c r="A4" s="84"/>
+      <x:c r="B4" s="78"/>
+      <x:c r="C4" s="91"/>
+      <x:c r="D4" s="87"/>
       <x:c r="E4" s="59" t="s">
-        <x:v>122</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="F4" s="59"/>
       <x:c r="G4" s="59"/>
       <x:c r="H4" s="59" t="s">
-        <x:v>235</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
-      <x:c r="A5" s="83"/>
-      <x:c r="B5" s="77"/>
-      <x:c r="C5" s="90"/>
-      <x:c r="D5" s="85" t="s">
-        <x:v>131</x:v>
+      <x:c r="A5" s="84"/>
+      <x:c r="B5" s="78"/>
+      <x:c r="C5" s="91"/>
+      <x:c r="D5" s="86" t="s">
+        <x:v>118</x:v>
       </x:c>
       <x:c r="E5" s="60" t="s">
-        <x:v>141</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F5" s="59"/>
       <x:c r="G5" s="59"/>
       <x:c r="H5" s="59" t="s">
-        <x:v>257</x:v>
+        <x:v>262</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
-      <x:c r="A6" s="83"/>
-      <x:c r="B6" s="77"/>
-      <x:c r="C6" s="91"/>
-      <x:c r="D6" s="86"/>
+      <x:c r="A6" s="84"/>
+      <x:c r="B6" s="78"/>
+      <x:c r="C6" s="92"/>
+      <x:c r="D6" s="87"/>
       <x:c r="E6" s="60" t="s">
-        <x:v>186</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="F6" s="59"/>
       <x:c r="G6" s="59"/>
       <x:c r="H6" s="59" t="s">
-        <x:v>14</x:v>
+        <x:v>184</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
-      <x:c r="A7" s="83"/>
-      <x:c r="B7" s="77"/>
-      <x:c r="C7" s="93" t="s">
-        <x:v>152</x:v>
-      </x:c>
-      <x:c r="D7" s="85" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E7" s="85" t="s">
-        <x:v>115</x:v>
+      <x:c r="A7" s="84"/>
+      <x:c r="B7" s="78"/>
+      <x:c r="C7" s="94" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="D7" s="86" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="E7" s="86" t="s">
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F7" s="59" t="s">
-        <x:v>206</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="G7" s="59"/>
       <x:c r="H7" s="59"/>
     </x:row>
     <x:row r="8" spans="1:8">
-      <x:c r="A8" s="83"/>
-      <x:c r="B8" s="77"/>
-      <x:c r="C8" s="90"/>
-      <x:c r="D8" s="88"/>
-      <x:c r="E8" s="88"/>
+      <x:c r="A8" s="84"/>
+      <x:c r="B8" s="78"/>
+      <x:c r="C8" s="91"/>
+      <x:c r="D8" s="89"/>
+      <x:c r="E8" s="89"/>
       <x:c r="F8" s="59" t="s">
-        <x:v>76</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G8" s="59"/>
       <x:c r="H8" s="59"/>
     </x:row>
     <x:row r="9" spans="1:8">
-      <x:c r="A9" s="83"/>
-      <x:c r="B9" s="77"/>
-      <x:c r="C9" s="90"/>
-      <x:c r="D9" s="88"/>
-      <x:c r="E9" s="88"/>
+      <x:c r="A9" s="84"/>
+      <x:c r="B9" s="78"/>
+      <x:c r="C9" s="91"/>
+      <x:c r="D9" s="89"/>
+      <x:c r="E9" s="89"/>
       <x:c r="F9" s="59" t="s">
-        <x:v>142</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="G9" s="59"/>
       <x:c r="H9" s="59"/>
     </x:row>
     <x:row r="10" spans="1:8">
-      <x:c r="A10" s="83"/>
-      <x:c r="B10" s="77"/>
-      <x:c r="C10" s="90"/>
-      <x:c r="D10" s="88"/>
-      <x:c r="E10" s="88"/>
+      <x:c r="A10" s="84"/>
+      <x:c r="B10" s="78"/>
+      <x:c r="C10" s="91"/>
+      <x:c r="D10" s="89"/>
+      <x:c r="E10" s="89"/>
       <x:c r="F10" s="59" t="s">
-        <x:v>194</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="G10" s="59"/>
       <x:c r="H10" s="59"/>
     </x:row>
     <x:row r="11" spans="1:8" ht="16.75">
-      <x:c r="A11" s="83"/>
-      <x:c r="B11" s="94"/>
-      <x:c r="C11" s="95"/>
-      <x:c r="D11" s="92"/>
-      <x:c r="E11" s="92"/>
+      <x:c r="A11" s="84"/>
+      <x:c r="B11" s="95"/>
+      <x:c r="C11" s="96"/>
+      <x:c r="D11" s="93"/>
+      <x:c r="E11" s="93"/>
       <x:c r="F11" s="61" t="s">
-        <x:v>137</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="G11" s="61"/>
       <x:c r="H11" s="61"/>
     </x:row>
     <x:row r="12" spans="1:8">
-      <x:c r="A12" s="83"/>
-      <x:c r="B12" s="77" t="s">
-        <x:v>221</x:v>
-      </x:c>
-      <x:c r="C12" s="90" t="s">
-        <x:v>156</x:v>
+      <x:c r="A12" s="84"/>
+      <x:c r="B12" s="78" t="s">
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="C12" s="91" t="s">
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D12" s="58" t="s">
-        <x:v>214</x:v>
-      </x:c>
-      <x:c r="E12" s="88" t="s">
-        <x:v>240</x:v>
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="E12" s="89" t="s">
+        <x:v>250</x:v>
       </x:c>
       <x:c r="F12" s="58"/>
       <x:c r="G12" s="58"/>
       <x:c r="H12" s="58"/>
     </x:row>
     <x:row r="13" spans="1:8">
-      <x:c r="A13" s="83"/>
-      <x:c r="B13" s="77"/>
-      <x:c r="C13" s="90"/>
+      <x:c r="A13" s="84"/>
+      <x:c r="B13" s="78"/>
+      <x:c r="C13" s="91"/>
       <x:c r="D13" s="60" t="s">
-        <x:v>172</x:v>
-      </x:c>
-      <x:c r="E13" s="88"/>
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="E13" s="89"/>
       <x:c r="F13" s="59"/>
       <x:c r="G13" s="59"/>
       <x:c r="H13" s="59"/>
     </x:row>
     <x:row r="14" spans="1:8">
-      <x:c r="A14" s="83"/>
-      <x:c r="B14" s="77"/>
-      <x:c r="C14" s="90"/>
+      <x:c r="A14" s="84"/>
+      <x:c r="B14" s="78"/>
+      <x:c r="C14" s="91"/>
       <x:c r="D14" s="60" t="s">
-        <x:v>136</x:v>
-      </x:c>
-      <x:c r="E14" s="88"/>
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="E14" s="89"/>
       <x:c r="F14" s="59"/>
       <x:c r="G14" s="59"/>
       <x:c r="H14" s="59"/>
     </x:row>
     <x:row r="15" spans="1:8">
-      <x:c r="A15" s="83"/>
-      <x:c r="B15" s="77"/>
-      <x:c r="C15" s="91"/>
+      <x:c r="A15" s="84"/>
+      <x:c r="B15" s="78"/>
+      <x:c r="C15" s="92"/>
       <x:c r="D15" s="60" t="s">
-        <x:v>182</x:v>
-      </x:c>
-      <x:c r="E15" s="86"/>
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="E15" s="87"/>
       <x:c r="F15" s="59"/>
       <x:c r="G15" s="59"/>
       <x:c r="H15" s="59"/>
     </x:row>
     <x:row r="16" spans="1:8">
-      <x:c r="A16" s="83"/>
-      <x:c r="B16" s="77"/>
-      <x:c r="C16" s="93" t="s">
+      <x:c r="A16" s="84"/>
+      <x:c r="B16" s="78"/>
+      <x:c r="C16" s="94" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="D16" s="60" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="E16" s="86" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="F16" s="59" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="G16" s="59"/>
+      <x:c r="H16" s="86" t="s">
+        <x:v>68</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:8">
+      <x:c r="A17" s="84"/>
+      <x:c r="B17" s="78"/>
+      <x:c r="C17" s="92"/>
+      <x:c r="D17" s="59" t="s">
+        <x:v>241</x:v>
+      </x:c>
+      <x:c r="E17" s="87"/>
+      <x:c r="F17" s="59" t="s">
         <x:v>164</x:v>
       </x:c>
-      <x:c r="D16" s="60" t="s">
-        <x:v>177</x:v>
-      </x:c>
-      <x:c r="E16" s="85" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="F16" s="59" t="s">
-        <x:v>133</x:v>
-      </x:c>
-      <x:c r="G16" s="59"/>
-      <x:c r="H16" s="85" t="s">
-        <x:v>241</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:8">
-      <x:c r="A17" s="83"/>
-      <x:c r="B17" s="77"/>
-      <x:c r="C17" s="91"/>
-      <x:c r="D17" s="59" t="s">
-        <x:v>193</x:v>
-      </x:c>
-      <x:c r="E17" s="86"/>
-      <x:c r="F17" s="59" t="s">
-        <x:v>165</x:v>
-      </x:c>
       <x:c r="G17" s="59"/>
-      <x:c r="H17" s="86"/>
+      <x:c r="H17" s="87"/>
     </x:row>
     <x:row r="18" spans="1:8" ht="16.75">
-      <x:c r="A18" s="83"/>
-      <x:c r="B18" s="94"/>
+      <x:c r="A18" s="84"/>
+      <x:c r="B18" s="95"/>
       <x:c r="C18" s="62" t="s">
-        <x:v>121</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="D18" s="61"/>
       <x:c r="E18" s="61"/>
       <x:c r="F18" s="61"/>
       <x:c r="G18" s="61"/>
       <x:c r="H18" s="61" t="s">
-        <x:v>239</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:8">
-      <x:c r="A19" s="83"/>
-      <x:c r="B19" s="77" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C19" s="90" t="s">
-        <x:v>188</x:v>
+      <x:c r="A19" s="84"/>
+      <x:c r="B19" s="78" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C19" s="91" t="s">
+        <x:v>235</x:v>
       </x:c>
       <x:c r="D19" s="58" t="s">
-        <x:v>218</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="E19" s="58"/>
       <x:c r="F19" s="58"/>
@@ -9769,11 +9797,11 @@
       <x:c r="H19" s="58"/>
     </x:row>
     <x:row r="20" spans="1:8">
-      <x:c r="A20" s="83"/>
-      <x:c r="B20" s="77"/>
-      <x:c r="C20" s="90"/>
+      <x:c r="A20" s="84"/>
+      <x:c r="B20" s="78"/>
+      <x:c r="C20" s="91"/>
       <x:c r="D20" s="59" t="s">
-        <x:v>191</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="E20" s="59"/>
       <x:c r="F20" s="59"/>
@@ -9781,11 +9809,11 @@
       <x:c r="H20" s="59"/>
     </x:row>
     <x:row r="21" spans="1:8">
-      <x:c r="A21" s="83"/>
-      <x:c r="B21" s="77"/>
-      <x:c r="C21" s="90"/>
+      <x:c r="A21" s="84"/>
+      <x:c r="B21" s="78"/>
+      <x:c r="C21" s="91"/>
       <x:c r="D21" s="59" t="s">
-        <x:v>125</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="E21" s="59"/>
       <x:c r="F21" s="59"/>
@@ -9793,11 +9821,11 @@
       <x:c r="H21" s="59"/>
     </x:row>
     <x:row r="22" spans="1:8">
-      <x:c r="A22" s="83"/>
-      <x:c r="B22" s="77"/>
-      <x:c r="C22" s="90"/>
+      <x:c r="A22" s="84"/>
+      <x:c r="B22" s="78"/>
+      <x:c r="C22" s="91"/>
       <x:c r="D22" s="59" t="s">
-        <x:v>212</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="E22" s="59"/>
       <x:c r="F22" s="59"/>
@@ -9805,11 +9833,11 @@
       <x:c r="H22" s="59"/>
     </x:row>
     <x:row r="23" spans="1:8">
-      <x:c r="A23" s="83"/>
-      <x:c r="B23" s="77"/>
-      <x:c r="C23" s="91"/>
+      <x:c r="A23" s="84"/>
+      <x:c r="B23" s="78"/>
+      <x:c r="C23" s="92"/>
       <x:c r="D23" s="59" t="s">
-        <x:v>155</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="E23" s="59"/>
       <x:c r="F23" s="59"/>
@@ -9817,90 +9845,90 @@
       <x:c r="H23" s="59"/>
     </x:row>
     <x:row r="24" spans="1:8">
-      <x:c r="A24" s="82"/>
-      <x:c r="B24" s="81"/>
-      <x:c r="C24" s="93" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="D24" s="85" t="s">
-        <x:v>202</x:v>
+      <x:c r="A24" s="83"/>
+      <x:c r="B24" s="82"/>
+      <x:c r="C24" s="94" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="D24" s="86" t="s">
+        <x:v>224</x:v>
       </x:c>
       <x:c r="E24" s="59" t="s">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="F24" s="59"/>
       <x:c r="G24" s="59"/>
       <x:c r="H24" s="59"/>
     </x:row>
     <x:row r="25" spans="1:8">
-      <x:c r="A25" s="83"/>
-      <x:c r="B25" s="77"/>
-      <x:c r="C25" s="90"/>
-      <x:c r="D25" s="86"/>
+      <x:c r="A25" s="84"/>
+      <x:c r="B25" s="78"/>
+      <x:c r="C25" s="91"/>
+      <x:c r="D25" s="87"/>
       <x:c r="E25" s="59" t="s">
-        <x:v>190</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="F25" s="59"/>
       <x:c r="G25" s="59"/>
       <x:c r="H25" s="59"/>
     </x:row>
     <x:row r="26" spans="1:8">
-      <x:c r="A26" s="82"/>
-      <x:c r="B26" s="81"/>
-      <x:c r="C26" s="90"/>
-      <x:c r="D26" s="85" t="s">
-        <x:v>224</x:v>
+      <x:c r="A26" s="83"/>
+      <x:c r="B26" s="82"/>
+      <x:c r="C26" s="91"/>
+      <x:c r="D26" s="86" t="s">
+        <x:v>226</x:v>
       </x:c>
       <x:c r="E26" s="59" t="s">
-        <x:v>210</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F26" s="59"/>
       <x:c r="G26" s="59"/>
       <x:c r="H26" s="59"/>
     </x:row>
     <x:row r="27" spans="1:8">
-      <x:c r="A27" s="83"/>
-      <x:c r="B27" s="77"/>
-      <x:c r="C27" s="90"/>
-      <x:c r="D27" s="88"/>
+      <x:c r="A27" s="84"/>
+      <x:c r="B27" s="78"/>
+      <x:c r="C27" s="91"/>
+      <x:c r="D27" s="89"/>
       <x:c r="E27" s="59" t="s">
-        <x:v>226</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F27" s="59"/>
       <x:c r="G27" s="59"/>
       <x:c r="H27" s="59"/>
     </x:row>
     <x:row r="28" spans="1:8">
-      <x:c r="A28" s="83"/>
-      <x:c r="B28" s="77"/>
-      <x:c r="C28" s="90"/>
-      <x:c r="D28" s="88"/>
+      <x:c r="A28" s="84"/>
+      <x:c r="B28" s="78"/>
+      <x:c r="C28" s="91"/>
+      <x:c r="D28" s="89"/>
       <x:c r="E28" s="59" t="s">
-        <x:v>199</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="F28" s="59"/>
       <x:c r="G28" s="59"/>
       <x:c r="H28" s="59"/>
     </x:row>
     <x:row r="29" spans="1:8" ht="16.75">
-      <x:c r="A29" s="83"/>
-      <x:c r="B29" s="94"/>
-      <x:c r="C29" s="95"/>
-      <x:c r="D29" s="92"/>
+      <x:c r="A29" s="84"/>
+      <x:c r="B29" s="95"/>
+      <x:c r="C29" s="96"/>
+      <x:c r="D29" s="93"/>
       <x:c r="E29" s="61" t="s">
-        <x:v>208</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="F29" s="61"/>
       <x:c r="G29" s="61"/>
       <x:c r="H29" s="61"/>
     </x:row>
     <x:row r="30" spans="1:8">
-      <x:c r="A30" s="83"/>
-      <x:c r="B30" s="77" t="s">
-        <x:v>219</x:v>
+      <x:c r="A30" s="84"/>
+      <x:c r="B30" s="78" t="s">
+        <x:v>204</x:v>
       </x:c>
       <x:c r="C30" s="63" t="s">
-        <x:v>213</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D30" s="58"/>
       <x:c r="E30" s="58"/>
@@ -9909,10 +9937,10 @@
       <x:c r="H30" s="58"/>
     </x:row>
     <x:row r="31" spans="1:8">
-      <x:c r="A31" s="83"/>
-      <x:c r="B31" s="77"/>
+      <x:c r="A31" s="84"/>
+      <x:c r="B31" s="78"/>
       <x:c r="C31" s="57" t="s">
-        <x:v>228</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="D31" s="59"/>
       <x:c r="E31" s="59"/>
@@ -9921,10 +9949,10 @@
       <x:c r="H31" s="59"/>
     </x:row>
     <x:row r="32" spans="1:8">
-      <x:c r="A32" s="83"/>
-      <x:c r="B32" s="77"/>
+      <x:c r="A32" s="84"/>
+      <x:c r="B32" s="78"/>
       <x:c r="C32" s="57" t="s">
-        <x:v>144</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D32" s="59"/>
       <x:c r="E32" s="59"/>
@@ -9933,10 +9961,10 @@
       <x:c r="H32" s="59"/>
     </x:row>
     <x:row r="33" spans="1:8" ht="16.75">
-      <x:c r="A33" s="83"/>
-      <x:c r="B33" s="94"/>
+      <x:c r="A33" s="84"/>
+      <x:c r="B33" s="95"/>
       <x:c r="C33" s="64" t="s">
-        <x:v>166</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="D33" s="61"/>
       <x:c r="E33" s="61"/>
@@ -9945,12 +9973,12 @@
       <x:c r="H33" s="61"/>
     </x:row>
     <x:row r="34" spans="1:8" ht="16.75" customHeight="1">
-      <x:c r="A34" s="83"/>
-      <x:c r="B34" s="76" t="s">
-        <x:v>174</x:v>
+      <x:c r="A34" s="84"/>
+      <x:c r="B34" s="77" t="s">
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C34" s="63" t="s">
-        <x:v>47</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D34" s="58"/>
       <x:c r="E34" s="58"/>
@@ -9959,13 +9987,13 @@
       <x:c r="H34" s="58"/>
     </x:row>
     <x:row r="35" spans="1:8">
-      <x:c r="A35" s="83"/>
-      <x:c r="B35" s="77"/>
-      <x:c r="C35" s="74" t="s">
-        <x:v>159</x:v>
+      <x:c r="A35" s="84"/>
+      <x:c r="B35" s="78"/>
+      <x:c r="C35" s="75" t="s">
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D35" s="59" t="s">
-        <x:v>204</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="E35" s="59"/>
       <x:c r="F35" s="59"/>
@@ -9973,11 +10001,11 @@
       <x:c r="H35" s="59"/>
     </x:row>
     <x:row r="36" spans="1:8">
-      <x:c r="A36" s="83"/>
-      <x:c r="B36" s="77"/>
-      <x:c r="C36" s="80"/>
+      <x:c r="A36" s="84"/>
+      <x:c r="B36" s="78"/>
+      <x:c r="C36" s="81"/>
       <x:c r="D36" s="59" t="s">
-        <x:v>147</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="E36" s="59"/>
       <x:c r="F36" s="59"/>
@@ -9985,11 +10013,11 @@
       <x:c r="H36" s="59"/>
     </x:row>
     <x:row r="37" spans="1:8">
-      <x:c r="A37" s="83"/>
-      <x:c r="B37" s="77"/>
-      <x:c r="C37" s="80"/>
+      <x:c r="A37" s="84"/>
+      <x:c r="B37" s="78"/>
+      <x:c r="C37" s="81"/>
       <x:c r="D37" s="59" t="s">
-        <x:v>50</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E37" s="59"/>
       <x:c r="F37" s="59"/>
@@ -9997,11 +10025,11 @@
       <x:c r="H37" s="59"/>
     </x:row>
     <x:row r="38" spans="1:8">
-      <x:c r="A38" s="83"/>
-      <x:c r="B38" s="77"/>
-      <x:c r="C38" s="80"/>
+      <x:c r="A38" s="84"/>
+      <x:c r="B38" s="78"/>
+      <x:c r="C38" s="81"/>
       <x:c r="D38" s="58" t="s">
-        <x:v>25</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E38" s="58"/>
       <x:c r="F38" s="58"/>
@@ -10009,11 +10037,11 @@
       <x:c r="H38" s="58"/>
     </x:row>
     <x:row r="39" spans="1:8">
-      <x:c r="A39" s="83"/>
-      <x:c r="B39" s="77"/>
-      <x:c r="C39" s="80"/>
+      <x:c r="A39" s="84"/>
+      <x:c r="B39" s="78"/>
+      <x:c r="C39" s="81"/>
       <x:c r="D39" s="59" t="s">
-        <x:v>29</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="E39" s="59"/>
       <x:c r="F39" s="59"/>
@@ -10021,11 +10049,11 @@
       <x:c r="H39" s="59"/>
     </x:row>
     <x:row r="40" spans="1:8" ht="16.75">
-      <x:c r="A40" s="96"/>
-      <x:c r="B40" s="94"/>
-      <x:c r="C40" s="98"/>
+      <x:c r="A40" s="97"/>
+      <x:c r="B40" s="95"/>
+      <x:c r="C40" s="99"/>
       <x:c r="D40" s="47" t="s">
-        <x:v>28</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="E40" s="47"/>
       <x:c r="F40" s="47"/>
@@ -10075,7 +10103,7 @@
     <x:row r="45" spans="1:8">
       <x:c r="A45" s="44"/>
       <x:c r="B45" s="44"/>
-      <x:c r="C45" s="97"/>
+      <x:c r="C45" s="98"/>
       <x:c r="D45" s="56"/>
       <x:c r="E45" s="46"/>
       <x:c r="F45" s="46"/>
@@ -10085,7 +10113,7 @@
     <x:row r="46" spans="1:8">
       <x:c r="A46" s="44"/>
       <x:c r="B46" s="44"/>
-      <x:c r="C46" s="97"/>
+      <x:c r="C46" s="98"/>
       <x:c r="D46" s="56"/>
       <x:c r="E46" s="46"/>
       <x:c r="F46" s="46"/>
@@ -10095,7 +10123,7 @@
     <x:row r="47" spans="1:8">
       <x:c r="A47" s="44"/>
       <x:c r="B47" s="44"/>
-      <x:c r="C47" s="97"/>
+      <x:c r="C47" s="98"/>
       <x:c r="D47" s="56"/>
       <x:c r="E47" s="46"/>
       <x:c r="F47" s="46"/>
@@ -10105,7 +10133,7 @@
     <x:row r="48" spans="1:8">
       <x:c r="A48" s="44"/>
       <x:c r="B48" s="44"/>
-      <x:c r="C48" s="97"/>
+      <x:c r="C48" s="98"/>
       <x:c r="D48" s="56"/>
       <x:c r="E48" s="46"/>
       <x:c r="F48" s="46"/>
@@ -10115,7 +10143,7 @@
     <x:row r="49" spans="1:8">
       <x:c r="A49" s="44"/>
       <x:c r="B49" s="44"/>
-      <x:c r="C49" s="97"/>
+      <x:c r="C49" s="98"/>
       <x:c r="D49" s="56"/>
       <x:c r="E49" s="46"/>
       <x:c r="F49" s="46"/>
@@ -10125,7 +10153,7 @@
     <x:row r="50" spans="1:8">
       <x:c r="A50" s="44"/>
       <x:c r="B50" s="44"/>
-      <x:c r="C50" s="97"/>
+      <x:c r="C50" s="98"/>
       <x:c r="D50" s="56"/>
       <x:c r="E50" s="46"/>
       <x:c r="F50" s="46"/>
@@ -10135,7 +10163,7 @@
     <x:row r="51" spans="1:8">
       <x:c r="A51" s="44"/>
       <x:c r="B51" s="44"/>
-      <x:c r="C51" s="97"/>
+      <x:c r="C51" s="98"/>
       <x:c r="D51" s="56"/>
       <x:c r="E51" s="46"/>
       <x:c r="F51" s="46"/>
@@ -10145,7 +10173,7 @@
     <x:row r="52" spans="1:8">
       <x:c r="A52" s="44"/>
       <x:c r="B52" s="44"/>
-      <x:c r="C52" s="97"/>
+      <x:c r="C52" s="98"/>
       <x:c r="D52" s="56"/>
       <x:c r="E52" s="46"/>
       <x:c r="F52" s="46"/>
@@ -10155,7 +10183,7 @@
     <x:row r="53" spans="1:8">
       <x:c r="A53" s="44"/>
       <x:c r="B53" s="44"/>
-      <x:c r="C53" s="97"/>
+      <x:c r="C53" s="98"/>
       <x:c r="D53" s="56"/>
       <x:c r="E53" s="46"/>
       <x:c r="F53" s="46"/>
@@ -10165,7 +10193,7 @@
     <x:row r="54" spans="1:8">
       <x:c r="A54" s="44"/>
       <x:c r="B54" s="44"/>
-      <x:c r="C54" s="97"/>
+      <x:c r="C54" s="98"/>
       <x:c r="D54" s="56"/>
       <x:c r="E54" s="46"/>
       <x:c r="F54" s="46"/>
@@ -10175,7 +10203,7 @@
     <x:row r="55" spans="1:8">
       <x:c r="A55" s="44"/>
       <x:c r="B55" s="44"/>
-      <x:c r="C55" s="97"/>
+      <x:c r="C55" s="98"/>
       <x:c r="D55" s="56"/>
       <x:c r="E55" s="46"/>
       <x:c r="F55" s="46"/>
@@ -10185,7 +10213,7 @@
     <x:row r="56" spans="1:8">
       <x:c r="A56" s="44"/>
       <x:c r="B56" s="44"/>
-      <x:c r="C56" s="97"/>
+      <x:c r="C56" s="98"/>
       <x:c r="D56" s="56"/>
       <x:c r="E56" s="46"/>
       <x:c r="F56" s="46"/>
@@ -10195,7 +10223,7 @@
     <x:row r="57" spans="1:8">
       <x:c r="A57" s="44"/>
       <x:c r="B57" s="44"/>
-      <x:c r="C57" s="97"/>
+      <x:c r="C57" s="98"/>
       <x:c r="D57" s="56"/>
       <x:c r="E57" s="46"/>
       <x:c r="F57" s="46"/>
@@ -10319,388 +10347,388 @@
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="48"/>
       <x:c r="B2" s="36" t="s">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C2" s="36" t="s">
-        <x:v>43</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D2" s="36" t="s">
-        <x:v>145</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="E2" s="36" t="s">
         <x:v>158</x:v>
       </x:c>
       <x:c r="F2" s="36" t="s">
-        <x:v>197</x:v>
+        <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6" ht="16.75">
       <x:c r="A3" s="48"/>
-      <x:c r="B3" s="76" t="s">
-        <x:v>126</x:v>
-      </x:c>
-      <x:c r="C3" s="79" t="s">
-        <x:v>170</x:v>
-      </x:c>
-      <x:c r="D3" s="79" t="s">
-        <x:v>118</x:v>
+      <x:c r="B3" s="77" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="C3" s="80" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="D3" s="80" t="s">
+        <x:v>114</x:v>
       </x:c>
       <x:c r="E3" s="49" t="s">
-        <x:v>0</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="F3" s="65"/>
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="A4" s="48"/>
-      <x:c r="B4" s="77"/>
-      <x:c r="C4" s="80"/>
-      <x:c r="D4" s="80"/>
+      <x:c r="B4" s="78"/>
+      <x:c r="C4" s="81"/>
+      <x:c r="D4" s="81"/>
       <x:c r="E4" s="50" t="s">
-        <x:v>242</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F4" s="66"/>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="48"/>
-      <x:c r="B5" s="77"/>
-      <x:c r="C5" s="80"/>
-      <x:c r="D5" s="80"/>
+      <x:c r="B5" s="78"/>
+      <x:c r="C5" s="81"/>
+      <x:c r="D5" s="81"/>
       <x:c r="E5" s="50" t="s">
-        <x:v>95</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F5" s="66"/>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="48"/>
-      <x:c r="B6" s="77"/>
-      <x:c r="C6" s="80"/>
-      <x:c r="D6" s="80"/>
+      <x:c r="B6" s="78"/>
+      <x:c r="C6" s="81"/>
+      <x:c r="D6" s="81"/>
       <x:c r="E6" s="50" t="s">
-        <x:v>104</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="F6" s="66"/>
     </x:row>
     <x:row r="7" spans="1:6" ht="32.75">
       <x:c r="A7" s="48"/>
-      <x:c r="B7" s="77"/>
-      <x:c r="C7" s="80"/>
-      <x:c r="D7" s="75"/>
+      <x:c r="B7" s="78"/>
+      <x:c r="C7" s="81"/>
+      <x:c r="D7" s="76"/>
       <x:c r="E7" s="51" t="s">
-        <x:v>19</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F7" s="66"/>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="48"/>
-      <x:c r="B8" s="77"/>
-      <x:c r="C8" s="80"/>
-      <x:c r="D8" s="74" t="s">
-        <x:v>195</x:v>
+      <x:c r="B8" s="78"/>
+      <x:c r="C8" s="81"/>
+      <x:c r="D8" s="75" t="s">
+        <x:v>228</x:v>
       </x:c>
       <x:c r="E8" s="52" t="s">
-        <x:v>1</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F8" s="66"/>
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="A9" s="48"/>
-      <x:c r="B9" s="77"/>
-      <x:c r="C9" s="80"/>
-      <x:c r="D9" s="80"/>
+      <x:c r="B9" s="78"/>
+      <x:c r="C9" s="81"/>
+      <x:c r="D9" s="81"/>
       <x:c r="E9" s="50" t="s">
-        <x:v>248</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="F9" s="66"/>
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="A10" s="48"/>
-      <x:c r="B10" s="77"/>
-      <x:c r="C10" s="80"/>
-      <x:c r="D10" s="75"/>
+      <x:c r="B10" s="78"/>
+      <x:c r="C10" s="81"/>
+      <x:c r="D10" s="76"/>
       <x:c r="E10" s="53" t="s">
-        <x:v>92</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F10" s="66"/>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="48"/>
-      <x:c r="B11" s="77"/>
-      <x:c r="C11" s="80"/>
-      <x:c r="D11" s="74" t="s">
-        <x:v>189</x:v>
+      <x:c r="B11" s="78"/>
+      <x:c r="C11" s="81"/>
+      <x:c r="D11" s="75" t="s">
+        <x:v>237</x:v>
       </x:c>
       <x:c r="E11" s="52" t="s">
-        <x:v>32</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F11" s="66"/>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="48"/>
-      <x:c r="B12" s="77"/>
-      <x:c r="C12" s="75"/>
-      <x:c r="D12" s="75"/>
+      <x:c r="B12" s="78"/>
+      <x:c r="C12" s="76"/>
+      <x:c r="D12" s="76"/>
       <x:c r="E12" s="53" t="s">
-        <x:v>103</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F12" s="66"/>
     </x:row>
     <x:row r="13" spans="1:6">
       <x:c r="A13" s="48"/>
-      <x:c r="B13" s="77"/>
-      <x:c r="C13" s="74" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="D13" s="74" t="s">
-        <x:v>188</x:v>
+      <x:c r="B13" s="78"/>
+      <x:c r="C13" s="75" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D13" s="75" t="s">
+        <x:v>235</x:v>
       </x:c>
       <x:c r="E13" s="52" t="s">
-        <x:v>262</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="F13" s="66"/>
     </x:row>
     <x:row r="14" spans="1:6">
       <x:c r="A14" s="48"/>
-      <x:c r="B14" s="77"/>
-      <x:c r="C14" s="80"/>
-      <x:c r="D14" s="80"/>
+      <x:c r="B14" s="78"/>
+      <x:c r="C14" s="81"/>
+      <x:c r="D14" s="81"/>
       <x:c r="E14" s="50" t="s">
-        <x:v>3</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F14" s="66"/>
     </x:row>
     <x:row r="15" spans="1:6">
       <x:c r="A15" s="48"/>
-      <x:c r="B15" s="77"/>
-      <x:c r="C15" s="80"/>
-      <x:c r="D15" s="80"/>
+      <x:c r="B15" s="78"/>
+      <x:c r="C15" s="81"/>
+      <x:c r="D15" s="81"/>
       <x:c r="E15" s="50" t="s">
-        <x:v>245</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F15" s="66"/>
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="A16" s="48"/>
-      <x:c r="B16" s="77"/>
-      <x:c r="C16" s="80"/>
-      <x:c r="D16" s="75"/>
+      <x:c r="B16" s="78"/>
+      <x:c r="C16" s="81"/>
+      <x:c r="D16" s="76"/>
       <x:c r="E16" s="53" t="s">
-        <x:v>38</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F16" s="66"/>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="A17" s="48"/>
-      <x:c r="B17" s="77"/>
-      <x:c r="C17" s="80"/>
-      <x:c r="D17" s="74" t="s">
-        <x:v>223</x:v>
+      <x:c r="B17" s="78"/>
+      <x:c r="C17" s="81"/>
+      <x:c r="D17" s="75" t="s">
+        <x:v>207</x:v>
       </x:c>
       <x:c r="E17" s="52" t="s">
-        <x:v>251</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="F17" s="66"/>
     </x:row>
     <x:row r="18" spans="1:6" ht="32.75">
       <x:c r="A18" s="48"/>
-      <x:c r="B18" s="77"/>
-      <x:c r="C18" s="75"/>
-      <x:c r="D18" s="75"/>
+      <x:c r="B18" s="78"/>
+      <x:c r="C18" s="76"/>
+      <x:c r="D18" s="76"/>
       <x:c r="E18" s="51" t="s">
-        <x:v>88</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="F18" s="66"/>
     </x:row>
     <x:row r="19" spans="1:6">
       <x:c r="A19" s="48"/>
-      <x:c r="B19" s="77"/>
-      <x:c r="C19" s="74" t="s">
-        <x:v>211</x:v>
-      </x:c>
-      <x:c r="D19" s="74" t="s">
-        <x:v>13</x:v>
+      <x:c r="B19" s="78"/>
+      <x:c r="C19" s="75" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="D19" s="75" t="s">
+        <x:v>183</x:v>
       </x:c>
       <x:c r="E19" s="52" t="s">
-        <x:v>261</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="F19" s="66"/>
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="A20" s="48"/>
-      <x:c r="B20" s="77"/>
-      <x:c r="C20" s="80"/>
-      <x:c r="D20" s="75"/>
+      <x:c r="B20" s="78"/>
+      <x:c r="C20" s="81"/>
+      <x:c r="D20" s="76"/>
       <x:c r="E20" s="53" t="s">
-        <x:v>101</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F20" s="66"/>
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="A21" s="48"/>
-      <x:c r="B21" s="77"/>
-      <x:c r="C21" s="80"/>
-      <x:c r="D21" s="74" t="s">
-        <x:v>82</x:v>
+      <x:c r="B21" s="78"/>
+      <x:c r="C21" s="81"/>
+      <x:c r="D21" s="75" t="s">
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E21" s="52" t="s">
-        <x:v>244</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="F21" s="66"/>
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="A22" s="48"/>
-      <x:c r="B22" s="77"/>
-      <x:c r="C22" s="80"/>
-      <x:c r="D22" s="75"/>
+      <x:c r="B22" s="78"/>
+      <x:c r="C22" s="81"/>
+      <x:c r="D22" s="76"/>
       <x:c r="E22" s="53" t="s">
-        <x:v>35</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F22" s="66"/>
     </x:row>
     <x:row r="23" spans="1:6">
       <x:c r="A23" s="48"/>
-      <x:c r="B23" s="77"/>
-      <x:c r="C23" s="80"/>
+      <x:c r="B23" s="78"/>
+      <x:c r="C23" s="81"/>
       <x:c r="D23" s="37" t="s">
-        <x:v>193</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="E23" s="54" t="s">
-        <x:v>36</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F23" s="66"/>
     </x:row>
     <x:row r="24" spans="1:6">
       <x:c r="A24" s="48"/>
-      <x:c r="B24" s="77"/>
-      <x:c r="C24" s="80"/>
-      <x:c r="D24" s="74" t="s">
-        <x:v>61</x:v>
+      <x:c r="B24" s="78"/>
+      <x:c r="C24" s="81"/>
+      <x:c r="D24" s="75" t="s">
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E24" s="52" t="s">
-        <x:v>12</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="F24" s="66"/>
     </x:row>
     <x:row r="25" spans="1:6">
       <x:c r="A25" s="48"/>
-      <x:c r="B25" s="77"/>
-      <x:c r="C25" s="80"/>
-      <x:c r="D25" s="80"/>
+      <x:c r="B25" s="78"/>
+      <x:c r="C25" s="81"/>
+      <x:c r="D25" s="81"/>
       <x:c r="E25" s="50" t="s">
-        <x:v>34</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F25" s="66"/>
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="A26" s="48"/>
-      <x:c r="B26" s="77"/>
-      <x:c r="C26" s="80"/>
-      <x:c r="D26" s="80"/>
+      <x:c r="B26" s="78"/>
+      <x:c r="C26" s="81"/>
+      <x:c r="D26" s="81"/>
       <x:c r="E26" s="50" t="s">
-        <x:v>31</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F26" s="66"/>
     </x:row>
     <x:row r="27" spans="1:6" ht="16.75">
       <x:c r="A27" s="48"/>
-      <x:c r="B27" s="94"/>
-      <x:c r="C27" s="98"/>
-      <x:c r="D27" s="98"/>
+      <x:c r="B27" s="95"/>
+      <x:c r="C27" s="99"/>
+      <x:c r="D27" s="99"/>
       <x:c r="E27" s="55" t="s">
-        <x:v>253</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="F27" s="67"/>
     </x:row>
     <x:row r="28" spans="1:6" ht="16.75">
       <x:c r="A28" s="48"/>
-      <x:c r="B28" s="76" t="s">
-        <x:v>148</x:v>
+      <x:c r="B28" s="77" t="s">
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C28" s="68" t="s">
-        <x:v>134</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D28" s="68" t="s">
-        <x:v>227</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="E28" s="69" t="s">
-        <x:v>250</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="F28" s="65"/>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="A29" s="48"/>
-      <x:c r="B29" s="77"/>
-      <x:c r="C29" s="74" t="s">
-        <x:v>160</x:v>
+      <x:c r="B29" s="78"/>
+      <x:c r="C29" s="75" t="s">
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D29" s="37" t="s">
-        <x:v>205</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="E29" s="54" t="s">
-        <x:v>37</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F29" s="66"/>
     </x:row>
     <x:row r="30" spans="1:6">
       <x:c r="A30" s="48"/>
-      <x:c r="B30" s="77"/>
-      <x:c r="C30" s="80"/>
-      <x:c r="D30" s="74" t="s">
-        <x:v>187</x:v>
+      <x:c r="B30" s="78"/>
+      <x:c r="C30" s="81"/>
+      <x:c r="D30" s="75" t="s">
+        <x:v>243</x:v>
       </x:c>
       <x:c r="E30" s="52" t="s">
-        <x:v>258</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="F30" s="66"/>
     </x:row>
     <x:row r="31" spans="1:6">
       <x:c r="A31" s="48"/>
-      <x:c r="B31" s="77"/>
-      <x:c r="C31" s="80"/>
-      <x:c r="D31" s="80"/>
+      <x:c r="B31" s="78"/>
+      <x:c r="C31" s="81"/>
+      <x:c r="D31" s="81"/>
       <x:c r="E31" s="50" t="s">
-        <x:v>39</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F31" s="66"/>
     </x:row>
     <x:row r="32" spans="1:6">
       <x:c r="A32" s="48"/>
-      <x:c r="B32" s="77"/>
-      <x:c r="C32" s="80"/>
-      <x:c r="D32" s="80"/>
+      <x:c r="B32" s="78"/>
+      <x:c r="C32" s="81"/>
+      <x:c r="D32" s="81"/>
       <x:c r="E32" s="50" t="s">
-        <x:v>2</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="F32" s="66"/>
     </x:row>
     <x:row r="33" spans="1:6" ht="16.75">
       <x:c r="A33" s="48"/>
-      <x:c r="B33" s="94"/>
-      <x:c r="C33" s="98"/>
-      <x:c r="D33" s="98"/>
+      <x:c r="B33" s="95"/>
+      <x:c r="C33" s="99"/>
+      <x:c r="D33" s="99"/>
       <x:c r="E33" s="55" t="s">
-        <x:v>256</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="F33" s="67"/>
     </x:row>
     <x:row r="34" spans="1:6">
       <x:c r="A34" s="48"/>
-      <x:c r="B34" s="77" t="s">
-        <x:v>181</x:v>
-      </x:c>
-      <x:c r="C34" s="80"/>
-      <x:c r="D34" s="80"/>
+      <x:c r="B34" s="78" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="C34" s="81"/>
+      <x:c r="D34" s="81"/>
       <x:c r="E34" s="50" t="s">
-        <x:v>105</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F34" s="66"/>
     </x:row>
     <x:row r="35" spans="1:6" ht="16.75">
       <x:c r="A35" s="48"/>
-      <x:c r="B35" s="94"/>
-      <x:c r="C35" s="98"/>
-      <x:c r="D35" s="98"/>
+      <x:c r="B35" s="95"/>
+      <x:c r="C35" s="99"/>
+      <x:c r="D35" s="99"/>
       <x:c r="E35" s="55" t="s">
-        <x:v>260</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="F35" s="67"/>
     </x:row>

</xml_diff>